<commit_message>
A bit more tidying up of the code; halfway through getting the HC linear results out cleanly
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F51186A-856A-4C6F-963A-B3E87F700840}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -157,7 +156,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -468,11 +467,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Minor change to include the linear model HC calc; not completely working for some reason it seems
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2264A6C-B97C-47D7-9FB2-8F0E01759199}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -136,12 +137,36 @@
   </si>
   <si>
     <t>kV</t>
+  </si>
+  <si>
+    <t>Manchester LV</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>024</t>
+  </si>
+  <si>
+    <t>074</t>
+  </si>
+  <si>
+    <t>041</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,7 +276,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -279,6 +304,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="3"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -286,7 +318,67 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="3" builtinId="25"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -296,31 +388,31 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor theme="7"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor theme="5"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -599,11 +691,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,7 +1067,9 @@
       <c r="L10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="1"/>
+      <c r="M10" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
@@ -1182,6 +1276,137 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="15">
+        <v>193</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="15">
+        <v>162</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="15">
+        <v>213</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M26" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1189,18 +1414,18 @@
     <mergeCell ref="A2:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="K3:M16">
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="15" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="16" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C16">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1212,7 +1437,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E16">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1224,7 +1449,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:H16">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1236,7 +1461,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G16">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1246,7 +1471,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H16">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1256,7 +1481,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J16">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1266,11 +1491,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E16">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L17:L26">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17:K26 M17:M26">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B17:B22 B26" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Getting a few more HC networks working
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2264A6C-B97C-47D7-9FB2-8F0E01759199}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="48">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -142,18 +141,6 @@
     <t>Manchester LV</t>
   </si>
   <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>004</t>
-  </si>
-  <si>
     <t>024</t>
   </si>
   <si>
@@ -161,12 +148,27 @@
   </si>
   <si>
     <t>041</t>
+  </si>
+  <si>
+    <t>NB: "Buses" &lt;" Nodes"</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>031</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -298,18 +300,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="3"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -691,11 +693,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,23 +746,23 @@
       <c r="J1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
       <c r="K2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1277,32 +1279,71 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="B17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="6">
+        <v>907</v>
+      </c>
+      <c r="D17" s="6">
+        <v>55</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0</v>
+      </c>
       <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
+      <c r="J17" s="6">
+        <f>D17*0.001</f>
+        <v>5.5E-2</v>
+      </c>
       <c r="K17" s="8" t="s">
         <v>30</v>
       </c>
       <c r="L17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="M17" s="8"/>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
-        <v>41</v>
+      <c r="M17" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18">
+        <v>2287</v>
+      </c>
+      <c r="D18">
+        <v>175</v>
+      </c>
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="J18" s="13">
+        <f t="shared" ref="J18:J26" si="0">D18*0.001</f>
+        <v>0.17500000000000002</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>30</v>
@@ -1311,10 +1352,35 @@
         <v>31</v>
       </c>
       <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
-        <v>42</v>
+      <c r="N18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19">
+        <v>1304</v>
+      </c>
+      <c r="D19">
+        <v>94</v>
+      </c>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="J19" s="13">
+        <f t="shared" si="0"/>
+        <v>9.4E-2</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>30</v>
@@ -1323,10 +1389,35 @@
         <v>31</v>
       </c>
       <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="15" t="s">
-        <v>43</v>
+      <c r="N19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20">
+        <v>375</v>
+      </c>
+      <c r="D20">
+        <v>24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="J20" s="13">
+        <f t="shared" si="0"/>
+        <v>2.4E-2</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>30</v>
@@ -1334,11 +1425,35 @@
       <c r="L20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="15" t="s">
-        <v>44</v>
+      <c r="M20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21">
+        <v>1605</v>
+      </c>
+      <c r="D21">
+        <v>115</v>
+      </c>
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="J21" s="13">
+        <f t="shared" si="0"/>
+        <v>0.115</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>30</v>
@@ -1347,10 +1462,35 @@
         <v>31</v>
       </c>
       <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="15" t="s">
-        <v>45</v>
+      <c r="N21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>1545</v>
+      </c>
+      <c r="D22">
+        <v>186</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="J22" s="13">
+        <f t="shared" si="0"/>
+        <v>0.186</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>30</v>
@@ -1359,10 +1499,35 @@
         <v>31</v>
       </c>
       <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="15">
+      <c r="N22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="12">
         <v>193</v>
+      </c>
+      <c r="C23">
+        <v>1391</v>
+      </c>
+      <c r="D23">
+        <v>65</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="J23" s="13">
+        <f t="shared" si="0"/>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>30</v>
@@ -1371,10 +1536,35 @@
         <v>31</v>
       </c>
       <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="15">
+      <c r="N23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="12">
         <v>162</v>
+      </c>
+      <c r="C24">
+        <v>1077</v>
+      </c>
+      <c r="D24">
+        <v>73</v>
+      </c>
+      <c r="E24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="J24" s="13">
+        <f t="shared" si="0"/>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>30</v>
@@ -1382,11 +1572,35 @@
       <c r="L24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="15">
+      <c r="M24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="12">
         <v>213</v>
+      </c>
+      <c r="C25">
+        <v>844</v>
+      </c>
+      <c r="D25">
+        <v>67</v>
+      </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="J25" s="13">
+        <f t="shared" si="0"/>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>30</v>
@@ -1395,10 +1609,35 @@
         <v>31</v>
       </c>
       <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="15" t="s">
-        <v>46</v>
+      <c r="N25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26">
+        <v>375</v>
+      </c>
+      <c r="D26">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="J26" s="13">
+        <f t="shared" si="0"/>
+        <v>2.4E-2</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>30</v>
@@ -1406,7 +1645,14 @@
       <c r="L26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M26" s="1"/>
+      <c r="M26" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1414,18 +1660,18 @@
     <mergeCell ref="A2:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="K3:M16">
-    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="19" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C16">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1436,8 +1682,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:E16">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="D3:E16 E17:E26">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1448,8 +1694,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:H16">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="G3:H16 G18:H27">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1460,8 +1706,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G16">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="G3:G16 G18:G27">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1470,8 +1716,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H16">
-    <cfRule type="colorScale" priority="9">
+  <conditionalFormatting sqref="H3:H16 H18:H27">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1481,7 +1727,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J16">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1490,12 +1736,23 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E16">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+  <conditionalFormatting sqref="E3:E26">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:L26">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17:K26 M17:M26">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -1506,21 +1763,42 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K17:K26 M17:M26">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
-      <formula>0</formula>
+  <conditionalFormatting sqref="G3:H26">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
-      <formula>"O"</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:D26">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"X"</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J26">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B17:B22 B26" numberStoredAsText="1"/>
+    <ignoredError sqref="B21:B22 B26 B17 B18:B20" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor bug fix for LV networks that were not solving
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="54">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -162,7 +162,25 @@
     <t>031</t>
   </si>
   <si>
-    <t>?</t>
+    <t>log(NBNL)</t>
+  </si>
+  <si>
+    <t>TODO ORDER</t>
+  </si>
+  <si>
+    <t>DIFF</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>HARD</t>
+  </si>
+  <si>
+    <t>MED</t>
+  </si>
+  <si>
+    <t>LO</t>
   </si>
 </sst>
 </file>
@@ -694,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,16 +724,17 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="6" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -729,30 +748,33 @@
         <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="14"/>
       <c r="M1" s="14"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="14"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -763,17 +785,24 @@
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="15"/>
+      <c r="L2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -786,26 +815,27 @@
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="6">
+        <f>LOG(D3*C3)</f>
+        <v>0.6020599913279624</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
       <c r="H3" s="6">
         <v>0</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="6">
+      <c r="K3" s="6">
         <v>5.4</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>31</v>
@@ -813,8 +843,11 @@
       <c r="M3" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N3" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -824,35 +857,39 @@
       <c r="D4">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="13">
+        <f t="shared" ref="E4:E26" si="0">LOG(D4*C4)</f>
+        <v>2.3802112417116059</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1.5</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>3.6</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -862,35 +899,39 @@
       <c r="D5">
         <v>68</v>
       </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="E5" s="13">
+        <f t="shared" si="0"/>
+        <v>3.4007106367732312</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="2">
         <v>24.9</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
       </c>
       <c r="H5">
         <v>2</v>
       </c>
       <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
         <v>50</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>2</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -900,35 +941,39 @@
       <c r="D6">
         <v>30</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="13">
+        <f t="shared" si="0"/>
+        <v>3.0681858617461617</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>4.8</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
       <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>1</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>3</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>2.6</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -938,35 +983,39 @@
       <c r="D7">
         <v>92</v>
       </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="E7" s="13">
+        <f t="shared" si="0"/>
+        <v>4.0843617585514052</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="2">
         <v>2.4</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>4</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>3</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>6</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>3.6</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L7" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -976,31 +1025,41 @@
       <c r="D8">
         <v>2355</v>
       </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="E8" s="13">
+        <f t="shared" si="0"/>
+        <v>7.0600546084112592</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="2">
         <v>7.2</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>4</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>3</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>17</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>12.05</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L8" s="1"/>
+      <c r="L8" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="1"/>
+      <c r="P8" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -1010,35 +1069,39 @@
       <c r="D9">
         <v>55</v>
       </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="E9" s="13">
+        <f t="shared" si="0"/>
+        <v>4.6979699765543392</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
         <v>0.3</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>5.5E-2</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>25</v>
       </c>
@@ -1048,32 +1111,36 @@
       <c r="D10">
         <v>694</v>
       </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="E10" s="13">
+        <f t="shared" si="0"/>
+        <v>5.4324240774813539</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="2">
         <v>13.8</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="J10">
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="K10">
         <v>42.8</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -1086,33 +1153,43 @@
       <c r="D11" s="6">
         <v>1379</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="7">
+      <c r="E11" s="6">
+        <f t="shared" si="0"/>
+        <v>6.6163958946881101</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="7">
         <v>12.47</v>
       </c>
-      <c r="G11" s="6">
+      <c r="H11" s="6">
         <v>4</v>
       </c>
-      <c r="H11" s="6">
-        <v>0</v>
-      </c>
       <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6">
         <v>5</v>
       </c>
-      <c r="J11" s="6">
+      <c r="K11" s="6">
         <v>16.3</v>
       </c>
-      <c r="K11" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="L11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="M11" s="8"/>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N11" s="8"/>
+      <c r="P11" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -1122,35 +1199,39 @@
       <c r="D12">
         <v>868</v>
       </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="E12" s="13">
+        <f t="shared" si="0"/>
+        <v>6.0371634509935488</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="2">
         <v>12.47</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>2</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
       <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
         <v>4</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>19.3</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -1160,29 +1241,39 @@
       <c r="D13">
         <v>3891</v>
       </c>
-      <c r="E13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="2">
+      <c r="E13" s="13">
+        <f t="shared" si="0"/>
+        <v>7.3723904998005798</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="2">
         <v>34.5</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>3</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>1</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>10</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>69.400000000000006</v>
       </c>
-      <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N13" s="1"/>
+      <c r="P13" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -1195,27 +1286,37 @@
       <c r="D14" s="6">
         <v>1384</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="7">
+      <c r="E14" s="6">
+        <f t="shared" si="0"/>
+        <v>6.8302672873552366</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="7">
         <v>12.47</v>
       </c>
-      <c r="G14" s="6">
+      <c r="H14" s="6">
         <v>5</v>
       </c>
-      <c r="H14" s="6">
+      <c r="I14" s="6">
         <v>8</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6">
+      <c r="J14" s="6"/>
+      <c r="K14" s="6">
         <v>11.6</v>
       </c>
-      <c r="K14" s="8"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N14" s="8"/>
+      <c r="P14" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -1225,32 +1326,36 @@
       <c r="D15">
         <v>332</v>
       </c>
-      <c r="E15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="E15" s="13">
+        <f t="shared" si="0"/>
+        <v>5.6290261088868352</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="2">
         <v>13.2</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
-      <c r="J15">
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="K15">
         <v>12.74</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L15" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>24</v>
       </c>
@@ -1260,24 +1365,34 @@
       <c r="D16">
         <v>1470</v>
       </c>
-      <c r="E16" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="E16" s="13">
+        <f t="shared" si="0"/>
+        <v>6.5816220228765081</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="2">
         <v>12.47</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>3</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>1</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>15.67</v>
       </c>
-      <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="P16" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q16">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
@@ -1292,30 +1407,34 @@
       <c r="D17" s="6">
         <v>55</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="7">
+      <c r="E17" s="6">
+        <f t="shared" si="0"/>
+        <v>4.6979699765543392</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="7">
         <v>0.41599999999999998</v>
       </c>
-      <c r="G17" s="6">
-        <v>0</v>
-      </c>
       <c r="H17" s="6">
         <v>0</v>
       </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6">
+      <c r="I17" s="6">
+        <v>0</v>
+      </c>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6">
         <f>D17*0.001</f>
         <v>5.5E-2</v>
       </c>
-      <c r="K17" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="L17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="M17" s="8" t="s">
+      <c r="N17" s="8" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1329,31 +1448,34 @@
       <c r="D18">
         <v>175</v>
       </c>
-      <c r="E18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="2">
+      <c r="E18" s="13">
+        <f t="shared" si="0"/>
+        <v>5.602304213293043</v>
+      </c>
+      <c r="F18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
       <c r="H18">
         <v>0</v>
       </c>
-      <c r="J18" s="13">
-        <f t="shared" ref="J18:J26" si="0">D18*0.001</f>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="K18" s="13">
+        <f t="shared" ref="K18:K26" si="1">D18*0.001</f>
         <v>0.17500000000000002</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M18" s="1"/>
-      <c r="N18" t="s">
-        <v>47</v>
+      <c r="N18" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -1366,31 +1488,34 @@
       <c r="D19">
         <v>94</v>
       </c>
-      <c r="E19" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="2">
+      <c r="E19" s="13">
+        <f t="shared" si="0"/>
+        <v>5.0884054449956002</v>
+      </c>
+      <c r="F19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
       <c r="H19">
         <v>0</v>
       </c>
-      <c r="J19" s="13">
-        <f t="shared" si="0"/>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="K19" s="13">
+        <f t="shared" si="1"/>
         <v>9.4E-2</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M19" s="1"/>
-      <c r="N19" t="s">
-        <v>47</v>
+      <c r="N19" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1403,29 +1528,33 @@
       <c r="D20">
         <v>24</v>
       </c>
-      <c r="E20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="E20" s="13">
+        <f t="shared" si="0"/>
+        <v>3.9542425094393248</v>
+      </c>
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
       <c r="H20">
         <v>0</v>
       </c>
-      <c r="J20" s="13">
-        <f t="shared" si="0"/>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="K20" s="13">
+        <f t="shared" si="1"/>
         <v>2.4E-2</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1439,31 +1568,34 @@
       <c r="D21">
         <v>115</v>
       </c>
-      <c r="E21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="2">
+      <c r="E21" s="13">
+        <f t="shared" si="0"/>
+        <v>5.2661728770945029</v>
+      </c>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
       <c r="H21">
         <v>0</v>
       </c>
-      <c r="J21" s="13">
-        <f t="shared" si="0"/>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="K21" s="13">
+        <f t="shared" si="1"/>
         <v>0.115</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M21" s="1"/>
-      <c r="N21" t="s">
-        <v>47</v>
+      <c r="N21" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1476,31 +1608,34 @@
       <c r="D22">
         <v>186</v>
       </c>
-      <c r="E22" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="2">
+      <c r="E22" s="13">
+        <f t="shared" si="0"/>
+        <v>5.4584414279787694</v>
+      </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
       <c r="H22">
         <v>0</v>
       </c>
-      <c r="J22" s="13">
-        <f t="shared" si="0"/>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="K22" s="13">
+        <f t="shared" si="1"/>
         <v>0.186</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M22" s="1"/>
-      <c r="N22" t="s">
-        <v>47</v>
+      <c r="N22" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1513,31 +1648,34 @@
       <c r="D23">
         <v>65</v>
       </c>
-      <c r="E23" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="2">
+      <c r="E23" s="13">
+        <f t="shared" si="0"/>
+        <v>4.9562404866349024</v>
+      </c>
+      <c r="F23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="J23" s="13">
-        <f t="shared" si="0"/>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="K23" s="13">
+        <f t="shared" si="1"/>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M23" s="1"/>
-      <c r="N23" t="s">
-        <v>47</v>
+      <c r="N23" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1550,29 +1688,33 @@
       <c r="D24">
         <v>73</v>
       </c>
-      <c r="E24" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="2">
+      <c r="E24" s="13">
+        <f t="shared" si="0"/>
+        <v>4.8955385634184374</v>
+      </c>
+      <c r="F24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
       <c r="H24">
         <v>0</v>
       </c>
-      <c r="J24" s="13">
-        <f t="shared" si="0"/>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="K24" s="13">
+        <f t="shared" si="1"/>
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="N24" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1586,31 +1728,34 @@
       <c r="D25">
         <v>67</v>
       </c>
-      <c r="E25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="2">
+      <c r="E25" s="13">
+        <f t="shared" si="0"/>
+        <v>4.7524172493264816</v>
+      </c>
+      <c r="F25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
       <c r="H25">
         <v>0</v>
       </c>
-      <c r="J25" s="13">
-        <f t="shared" si="0"/>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="K25" s="13">
+        <f t="shared" si="1"/>
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="K25" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M25" s="1"/>
-      <c r="N25" t="s">
-        <v>47</v>
+      <c r="N25" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -1623,29 +1768,33 @@
       <c r="D26">
         <v>24</v>
       </c>
-      <c r="E26" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" s="2">
+      <c r="E26" s="13">
+        <f t="shared" si="0"/>
+        <v>3.9542425094393248</v>
+      </c>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
       <c r="H26">
         <v>0</v>
       </c>
-      <c r="J26" s="13">
-        <f t="shared" si="0"/>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="K26" s="13">
+        <f t="shared" si="1"/>
         <v>2.4E-2</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="N26" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1656,21 +1805,33 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="A2:K2"/>
   </mergeCells>
-  <conditionalFormatting sqref="K3:M16">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
+  <conditionalFormatting sqref="L3:N16">
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="19" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="20" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C16">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:F16 F17:F26 E4:E26">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -1682,7 +1843,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:E16 E17:E26">
+  <conditionalFormatting sqref="H3:I16 H18:I27">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -1694,8 +1855,75 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:H16 G18:H27">
+  <conditionalFormatting sqref="H3:H16 H18:H27">
     <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I16 I18:I27">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K16">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F26">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M17:M26">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L17:L26 N17:N26">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:I26">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:E26">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1706,28 +1934,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G16 G18:G27">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H16 H18:H27">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J16">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="K3:K26">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1737,44 +1945,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E26">
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L17:L26">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K17:K26 M17:M26">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:H26">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:D26">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1785,16 +1956,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J26">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Getting a few more of the circuits up and running (Ckt 5 done; first part of J1; 8500 halfway through taps). Some small bug fixes.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,25 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B898634F-FAAB-49DB-9E54-F8FB40F2BA86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="53">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -177,16 +183,13 @@
     <t>HARD</t>
   </si>
   <si>
-    <t>MED</t>
-  </si>
-  <si>
-    <t>LO</t>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -711,11 +714,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,7 +737,7 @@
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -774,7 +777,7 @@
       <c r="M1" s="14"/>
       <c r="N1" s="14"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -802,7 +805,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -847,7 +850,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -889,7 +892,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -931,7 +934,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -972,8 +975,11 @@
       <c r="N6" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -1015,7 +1021,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -1039,7 +1045,7 @@
         <v>4</v>
       </c>
       <c r="I8">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="J8">
         <v>17</v>
@@ -1053,13 +1059,13 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="P8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -1101,7 +1107,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>25</v>
       </c>
@@ -1140,7 +1146,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -1181,15 +1187,11 @@
       <c r="M11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="N11" s="8"/>
-      <c r="P11" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N11" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -1231,7 +1233,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -1273,7 +1275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -1306,7 +1308,9 @@
       <c r="K14" s="6">
         <v>11.6</v>
       </c>
-      <c r="L14" s="8"/>
+      <c r="L14" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="P14" t="s">
@@ -1316,7 +1320,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -1355,7 +1359,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
A number of changes. 1. The 8500 node model is now working with tap changers, and HC analysis validated. (LTC controls not added.) 2. The fixed_voltage_testing modified to match ltc_voltage_testing; and, saving the linear model for HC analysis 2. Ckt24 added to circuit lists
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E54D376-F0F6-47B5-82AB-0825A736286B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED9FE98-DFF9-42F5-A1E3-781E84384ABC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="54">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Tap Model</t>
   </si>
 </sst>
 </file>
@@ -328,10 +331,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -341,7 +344,127 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="3" builtinId="25"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -718,7 +841,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,31 +894,35 @@
       <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
       <c r="L2" s="4" t="s">
         <v>27</v>
       </c>
       <c r="M2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>29</v>
       </c>
       <c r="P2" s="4" t="s">
@@ -849,6 +976,9 @@
       <c r="N3" s="8" t="s">
         <v>31</v>
       </c>
+      <c r="O3" s="8" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -891,6 +1021,9 @@
       <c r="N4" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="O4" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -933,6 +1066,9 @@
       <c r="N5" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="O5" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -975,6 +1111,9 @@
       <c r="N6" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="O6" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="R6" t="s">
         <v>52</v>
       </c>
@@ -1020,6 +1159,9 @@
       <c r="N7" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="O7" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -1056,13 +1198,14 @@
       <c r="L8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="P8" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q8">
-        <v>2</v>
+      <c r="M8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1104,6 +1247,9 @@
         <v>31</v>
       </c>
       <c r="N9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1143,6 +1289,9 @@
         <v>31</v>
       </c>
       <c r="N10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1188,6 +1337,9 @@
         <v>31</v>
       </c>
       <c r="N11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="O11" s="8" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1230,6 +1382,9 @@
         <v>31</v>
       </c>
       <c r="N12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1268,11 +1423,12 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
       <c r="P13" t="s">
         <v>51</v>
       </c>
       <c r="Q13">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1313,11 +1469,12 @@
       </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
       <c r="P14" t="s">
         <v>51</v>
       </c>
       <c r="Q14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1358,6 +1515,9 @@
       <c r="N15" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="O15" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1391,14 +1551,15 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
       <c r="P16" t="s">
         <v>50</v>
       </c>
       <c r="Q16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>39</v>
       </c>
@@ -1439,10 +1600,13 @@
         <v>31</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>45</v>
       </c>
@@ -1479,10 +1643,13 @@
         <v>31</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>46</v>
       </c>
@@ -1519,10 +1686,13 @@
         <v>31</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>42</v>
       </c>
@@ -1559,10 +1729,13 @@
         <v>31</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>40</v>
       </c>
@@ -1599,10 +1772,13 @@
         <v>31</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>41</v>
       </c>
@@ -1639,10 +1815,13 @@
         <v>31</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <v>193</v>
       </c>
@@ -1679,10 +1858,13 @@
         <v>31</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>162</v>
       </c>
@@ -1719,10 +1901,13 @@
         <v>31</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25" s="12">
         <v>213</v>
       </c>
@@ -1759,10 +1944,13 @@
         <v>31</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>42</v>
       </c>
@@ -1799,32 +1987,35 @@
         <v>31</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="L1:N1"/>
     <mergeCell ref="A2:K2"/>
+    <mergeCell ref="L1:O1"/>
   </mergeCells>
-  <conditionalFormatting sqref="L3:N16">
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
+  <conditionalFormatting sqref="L3:L16 N3:N16">
+    <cfRule type="cellIs" dxfId="21" priority="30" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="31" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="32" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C16">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1836,7 +2027,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:F16 F17:F26 E4:E26">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1848,6 +2039,85 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:I16 H18:I27">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H16 H18:H27">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I16 I18:I27">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K16">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F26">
+    <cfRule type="cellIs" dxfId="18" priority="23" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N17:N26">
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="21" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="22" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L17:L26">
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="18" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="19" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:I26">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:E26">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -1859,28 +2129,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H16 H18:H27">
+  <conditionalFormatting sqref="K3:K26">
     <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I16 I18:I27">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K16">
-    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1889,45 +2139,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F26">
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M17:M26">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L17:L26 N17:N26">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3:I26">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:E26">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="E3:E26">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1938,26 +2151,48 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K26">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
+  <conditionalFormatting sqref="O3:O16">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E26">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
+  <conditionalFormatting sqref="O17:O26">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M16">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M17:M26">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Got the IEEE Circuit 24 up and running.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED9FE98-DFF9-42F5-A1E3-781E84384ABC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A573FA5-DCFA-4170-A9F7-FEA675CE08F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="54">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -841,26 +841,26 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.453125" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -901,7 +901,7 @@
       <c r="N1" s="15"/>
       <c r="O1" s="15"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -932,7 +932,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -980,7 +980,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>25</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -1420,7 +1420,9 @@
       <c r="K13">
         <v>69.400000000000006</v>
       </c>
-      <c r="L13" s="1"/>
+      <c r="L13" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1431,7 +1433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -1477,7 +1479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -1519,7 +1521,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>24</v>
       </c>
@@ -1559,7 +1561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
         <v>39</v>
       </c>
@@ -1606,7 +1608,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B18" s="12" t="s">
         <v>45</v>
       </c>
@@ -1649,7 +1651,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B19" s="12" t="s">
         <v>46</v>
       </c>
@@ -1692,7 +1694,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B20" s="12" t="s">
         <v>42</v>
       </c>
@@ -1735,7 +1737,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B21" s="12" t="s">
         <v>40</v>
       </c>
@@ -1778,7 +1780,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B22" s="12" t="s">
         <v>41</v>
       </c>
@@ -1821,7 +1823,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B23" s="12">
         <v>193</v>
       </c>
@@ -1864,7 +1866,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B24" s="12">
         <v>162</v>
       </c>
@@ -1907,7 +1909,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B25" s="12">
         <v>213</v>
       </c>
@@ -1950,7 +1952,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B26" s="12" t="s">
         <v>42</v>
       </c>
@@ -1993,7 +1995,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Found the bugger that was causing the linear model to work. It seems that heavy unbalance results in a different result to the single-phase only result. All networks now have working linear models (fixed tap).
Also, some changes for faster checking of linear model validity at the lin/no load points rather than running all cases.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A573FA5-DCFA-4170-A9F7-FEA675CE08F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C4669D-D679-45F0-AE26-B03113AE0CC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="54">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -177,9 +177,6 @@
     <t>DIFF</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>HARD</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>Tap Model</t>
+  </si>
+  <si>
+    <t>MED</t>
   </si>
 </sst>
 </file>
@@ -841,26 +841,26 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -901,7 +901,7 @@
       <c r="N1" s="15"/>
       <c r="O1" s="15"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -917,7 +917,7 @@
         <v>27</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>28</v>
@@ -932,7 +932,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -980,7 +980,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -1115,10 +1115,10 @@
         <v>31</v>
       </c>
       <c r="R6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>25</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -1427,13 +1427,13 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -1473,13 +1473,13 @@
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
       <c r="P14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>24</v>
       </c>
@@ -1550,18 +1550,20 @@
       <c r="K16">
         <v>15.67</v>
       </c>
-      <c r="L16" s="1"/>
+      <c r="L16" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="Q16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>39</v>
       </c>
@@ -1608,7 +1610,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>45</v>
       </c>
@@ -1651,7 +1653,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>46</v>
       </c>
@@ -1694,7 +1696,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>42</v>
       </c>
@@ -1737,7 +1739,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>40</v>
       </c>
@@ -1780,7 +1782,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>41</v>
       </c>
@@ -1823,7 +1825,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <v>193</v>
       </c>
@@ -1866,7 +1868,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>162</v>
       </c>
@@ -1909,7 +1911,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25" s="12">
         <v>213</v>
       </c>
@@ -1952,7 +1954,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>42</v>
       </c>
@@ -1995,7 +1997,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Halfway through getting functionality working for circuit m1 - added a small piece that seems (?) to allow single phase capacitors to be used, although it has been a bit of a quick hack tbh...
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C4669D-D679-45F0-AE26-B03113AE0CC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9290CC36-D24C-48D5-ABAD-50ECBCD62C03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -841,7 +841,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Haflway through a few more bits and pieces getting the networks together.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9290CC36-D24C-48D5-ABAD-50ECBCD62C03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B2FE71-74F0-4293-8A55-3737B16589BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="53">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t>Tap Model</t>
-  </si>
-  <si>
-    <t>MED</t>
   </si>
 </sst>
 </file>
@@ -841,26 +838,26 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.453125" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -901,7 +898,7 @@
       <c r="N1" s="15"/>
       <c r="O1" s="15"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -932,7 +929,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -980,7 +977,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -1025,7 +1022,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -1070,7 +1067,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -1118,7 +1115,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -1163,7 +1160,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -1208,7 +1205,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -1253,7 +1250,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>25</v>
       </c>
@@ -1295,7 +1292,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -1343,7 +1340,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -1388,7 +1385,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -1430,10 +1427,10 @@
         <v>50</v>
       </c>
       <c r="Q13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -1476,10 +1473,10 @@
         <v>50</v>
       </c>
       <c r="Q14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -1521,7 +1518,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>24</v>
       </c>
@@ -1553,17 +1550,17 @@
       <c r="L16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
         <v>39</v>
       </c>
@@ -1610,7 +1607,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B18" s="12" t="s">
         <v>45</v>
       </c>
@@ -1653,7 +1650,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B19" s="12" t="s">
         <v>46</v>
       </c>
@@ -1696,7 +1693,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B20" s="12" t="s">
         <v>42</v>
       </c>
@@ -1739,7 +1736,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B21" s="12" t="s">
         <v>40</v>
       </c>
@@ -1782,7 +1779,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B22" s="12" t="s">
         <v>41</v>
       </c>
@@ -1825,7 +1822,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B23" s="12">
         <v>193</v>
       </c>
@@ -1868,7 +1865,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B24" s="12">
         <v>162</v>
       </c>
@@ -1911,7 +1908,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B25" s="12">
         <v>213</v>
       </c>
@@ -1954,7 +1951,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B26" s="12" t="s">
         <v>42</v>
       </c>
@@ -1997,7 +1994,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Updating the distribution circuits table with some solution times
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B2FE71-74F0-4293-8A55-3737B16589BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="plotTts" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="59">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -184,12 +184,30 @@
   </si>
   <si>
     <t>Tap Model</t>
+  </si>
+  <si>
+    <t>Log(Time to solve) (us)</t>
+  </si>
+  <si>
+    <t>Load points</t>
+  </si>
+  <si>
+    <t>Gen Points</t>
+  </si>
+  <si>
+    <t>Scenarios</t>
+  </si>
+  <si>
+    <t>Sln time (mins)</t>
+  </si>
+  <si>
+    <t>slns per s-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -235,7 +253,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -292,6 +310,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -299,7 +326,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -328,6 +355,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -570,6 +601,1037 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>plotTts!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4876</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>907</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1255</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6058</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4888</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1282</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2596</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>plotTts!$D$2:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>7.0300000000000007E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.000000000000007E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9070000000000012E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9650000000000015E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27576300000000048</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1440000000000088E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2061000000000023E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2321000000000009E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7450000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.7955000000000019E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.6279000000000014E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0153000000000025E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.7688000000000022E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-066E-490A-8007-7A7F6D9C8EBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="128672392"/>
+        <c:axId val="128676656"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="128672392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400"/>
+                  <a:t>Number of Nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="128676656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="128676656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+                  <a:t>Solution Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="128672392"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>271460</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -834,30 +1896,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -891,45 +1954,49 @@
       <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="4" t="s">
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -964,9 +2031,7 @@
       <c r="K3" s="6">
         <v>5.4</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="L3" s="6"/>
       <c r="M3" s="8" t="s">
         <v>31</v>
       </c>
@@ -976,8 +2041,11 @@
       <c r="O3" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="P3" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -1009,8 +2077,9 @@
       <c r="K4">
         <v>3.6</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>30</v>
+      <c r="L4">
+        <f>LOG10(703)</f>
+        <v>2.8469553250198238</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>30</v>
@@ -1021,8 +2090,11 @@
       <c r="O4" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="P4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -1054,8 +2126,9 @@
       <c r="K5">
         <v>2</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>30</v>
+      <c r="L5">
+        <f>LOG10(4000)</f>
+        <v>3.6020599913279625</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>30</v>
@@ -1066,8 +2139,11 @@
       <c r="O5" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="P5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -1099,11 +2175,12 @@
       <c r="K6">
         <v>2.6</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>30</v>
+      <c r="L6">
+        <f>LOG10(2907)</f>
+        <v>3.4634450317704277</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>31</v>
@@ -1111,11 +2188,14 @@
       <c r="O6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="R6" t="s">
+      <c r="P6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -1147,8 +2227,9 @@
       <c r="K7">
         <v>3.6</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>30</v>
+      <c r="L7">
+        <f>LOG10(4965)</f>
+        <v>3.6959192528313998</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>30</v>
@@ -1159,8 +2240,11 @@
       <c r="O7" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="P7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -1192,20 +2276,24 @@
       <c r="K8">
         <v>12.05</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>30</v>
+      <c r="L8">
+        <f>LOG10(275763)</f>
+        <v>5.4405359950748213</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="P8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -1237,20 +2325,24 @@
       <c r="K9">
         <v>5.5E-2</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>30</v>
+      <c r="L9">
+        <f>LOG10(5144)</f>
+        <v>3.7113009599161657</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>25</v>
       </c>
@@ -1279,20 +2371,24 @@
       <c r="K10">
         <v>42.8</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>30</v>
+      <c r="L10" s="15">
+        <f>LOG10(12061)</f>
+        <v>4.0813833174622856</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>31</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -1327,20 +2423,24 @@
       <c r="K11" s="6">
         <v>16.3</v>
       </c>
-      <c r="L11" s="8" t="s">
-        <v>30</v>
+      <c r="L11">
+        <f>LOG10(32321)</f>
+        <v>4.50948478922394</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N11" s="8" t="s">
         <v>31</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -1372,20 +2472,24 @@
       <c r="K12">
         <v>19.3</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>30</v>
+      <c r="L12">
+        <f>LOG10(17450)</f>
+        <v>4.2417954312951984</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -1417,20 +2521,24 @@
       <c r="K13">
         <v>69.400000000000006</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M13" s="1"/>
+      <c r="L13" s="15">
+        <f>LOG10(87955)</f>
+        <v>4.9442605329428515</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" t="s">
+      <c r="P13" s="1"/>
+      <c r="Q13" t="s">
         <v>50</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -1463,20 +2571,24 @@
       <c r="K14" s="6">
         <v>11.6</v>
       </c>
-      <c r="L14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="M14" s="8"/>
+      <c r="L14">
+        <f>LOG10(26279)</f>
+        <v>4.4196088349081029</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
-      <c r="P14" t="s">
+      <c r="P14" s="8"/>
+      <c r="Q14" t="s">
         <v>50</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -1505,8 +2617,9 @@
       <c r="K15">
         <v>12.74</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>30</v>
+      <c r="L15">
+        <f>LOG10(20153)</f>
+        <v>4.3043397048923389</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>30</v>
@@ -1517,8 +2630,11 @@
       <c r="O15" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="P15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>24</v>
       </c>
@@ -1547,20 +2663,24 @@
       <c r="K16">
         <v>15.67</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>30</v>
+      <c r="L16" s="15">
+        <f>LOG10(27688)</f>
+        <v>4.4422915862860712</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>39</v>
       </c>
@@ -1594,20 +2714,24 @@
         <f>D17*0.001</f>
         <v>5.5E-2</v>
       </c>
-      <c r="L17" s="8" t="s">
-        <v>30</v>
+      <c r="L17">
+        <f t="shared" ref="L17:L26" si="1">LOG10(1)</f>
+        <v>0</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N17" s="8" t="s">
         <v>31</v>
       </c>
       <c r="O17" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>45</v>
       </c>
@@ -1634,23 +2758,27 @@
         <v>0</v>
       </c>
       <c r="K18" s="13">
-        <f t="shared" ref="K18:K26" si="1">D18*0.001</f>
+        <f t="shared" ref="K18:K26" si="2">D18*0.001</f>
         <v>0.17500000000000002</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>30</v>
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>46</v>
       </c>
@@ -1677,23 +2805,27 @@
         <v>0</v>
       </c>
       <c r="K19" s="13">
+        <f t="shared" si="2"/>
+        <v>9.4E-2</v>
+      </c>
+      <c r="L19">
         <f t="shared" si="1"/>
-        <v>9.4E-2</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>42</v>
       </c>
@@ -1720,23 +2852,27 @@
         <v>0</v>
       </c>
       <c r="K20" s="13">
+        <f t="shared" si="2"/>
+        <v>2.4E-2</v>
+      </c>
+      <c r="L20">
         <f t="shared" si="1"/>
-        <v>2.4E-2</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>40</v>
       </c>
@@ -1763,23 +2899,27 @@
         <v>0</v>
       </c>
       <c r="K21" s="13">
+        <f t="shared" si="2"/>
+        <v>0.115</v>
+      </c>
+      <c r="L21">
         <f t="shared" si="1"/>
-        <v>0.115</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>41</v>
       </c>
@@ -1806,23 +2946,27 @@
         <v>0</v>
       </c>
       <c r="K22" s="13">
+        <f t="shared" si="2"/>
+        <v>0.186</v>
+      </c>
+      <c r="L22">
         <f t="shared" si="1"/>
-        <v>0.186</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <v>193</v>
       </c>
@@ -1849,23 +2993,27 @@
         <v>0</v>
       </c>
       <c r="K23" s="13">
+        <f t="shared" si="2"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="L23">
         <f t="shared" si="1"/>
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>162</v>
       </c>
@@ -1892,23 +3040,27 @@
         <v>0</v>
       </c>
       <c r="K24" s="13">
+        <f t="shared" si="2"/>
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="L24">
         <f t="shared" si="1"/>
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B25" s="12">
         <v>213</v>
       </c>
@@ -1935,23 +3087,27 @@
         <v>0</v>
       </c>
       <c r="K25" s="13">
+        <f t="shared" si="2"/>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="L25">
         <f t="shared" si="1"/>
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>42</v>
       </c>
@@ -1978,23 +3134,27 @@
         <v>0</v>
       </c>
       <c r="K26" s="13">
+        <f t="shared" si="2"/>
+        <v>2.4E-2</v>
+      </c>
+      <c r="L26">
         <f t="shared" si="1"/>
-        <v>2.4E-2</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -2002,20 +3162,32 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:K2"/>
-    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="M1:P1"/>
   </mergeCells>
-  <conditionalFormatting sqref="L3:L16 N3:N16">
-    <cfRule type="cellIs" dxfId="21" priority="30" operator="equal">
+  <conditionalFormatting sqref="M3:M16 O3:O16">
+    <cfRule type="cellIs" dxfId="21" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="32" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="33" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C16">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:F16 F17:F26 E4:E26">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -2027,7 +3199,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:F16 F17:F26 E4:E26">
+  <conditionalFormatting sqref="H3:I16 H18:I27">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -2039,8 +3211,75 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:I16 H18:I27">
+  <conditionalFormatting sqref="H3:H16 H18:H27">
     <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I16 I18:I27">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:L16 L10:L26">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F26">
+    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17:O26">
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="22" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="23" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M17:M26">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="20" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:I26">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:E26">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2051,28 +3290,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H16 H18:H27">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I16 I18:I27">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K16">
-    <cfRule type="colorScale" priority="24">
+  <conditionalFormatting sqref="K3:L26">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2081,45 +3300,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F26">
-    <cfRule type="cellIs" dxfId="18" priority="23" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N17:N26">
-    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="21" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="22" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L17:L26">
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="18" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="19" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3:I26">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:E26">
-    <cfRule type="colorScale" priority="15">
+  <conditionalFormatting sqref="E3:E26">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2130,8 +3312,52 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K26">
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="P3:P16">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P17:P26">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N16">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N17:N26">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L26">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2140,8 +3366,494 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E26">
-    <cfRule type="colorScale" priority="13">
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B21:B22 B26 B17 B18:B20" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>2.8469553250198238</v>
+      </c>
+      <c r="D2">
+        <f>(10^C2)/1000000</f>
+        <v>7.0300000000000007E-4</v>
+      </c>
+      <c r="E2">
+        <f>1/D2</f>
+        <v>1422.4751066856329</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>20</v>
+      </c>
+      <c r="H2">
+        <v>1000</v>
+      </c>
+      <c r="I2">
+        <f>(H2*G2*F2*D2)/60</f>
+        <v>0.93733333333333335</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>37</v>
+      </c>
+      <c r="C3">
+        <v>3.6020599913279625</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D14" si="0">(10^C3)/1000000</f>
+        <v>4.000000000000007E-3</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E14" si="1">1/D3</f>
+        <v>249.99999999999957</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>1000</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I14" si="2">(H3*G3*F3*D3)/60</f>
+        <v>5.3333333333333428</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>39</v>
+      </c>
+      <c r="C4">
+        <v>3.4634450317704277</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>2.9070000000000012E-3</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>343.9972480220157</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>1000</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>3.8760000000000017</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>132</v>
+      </c>
+      <c r="C5">
+        <v>3.6959192528313998</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>4.9650000000000015E-3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>201.40986908358502</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>1000</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>6.6200000000000019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>4876</v>
+      </c>
+      <c r="C6">
+        <v>5.4405359950748213</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.27576300000000048</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>3.6263022958119771</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>1000</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>367.68400000000059</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>907</v>
+      </c>
+      <c r="C7">
+        <v>3.7113009599161657</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>5.1440000000000088E-3</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>194.40124416796235</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>1000</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>6.8586666666666787</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>390</v>
+      </c>
+      <c r="C8" s="15">
+        <v>4.0813833174622856</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1.2061000000000023E-2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>82.911864687836669</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>1000</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>16.081333333333365</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2998</v>
+      </c>
+      <c r="C9">
+        <v>4.50948478922394</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>3.2321000000000009E-2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>30.939636768664325</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>20</v>
+      </c>
+      <c r="H9">
+        <v>1000</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>43.094666666666676</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>1255</v>
+      </c>
+      <c r="C10">
+        <v>4.2417954312951984</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1.7450000000000004E-2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>57.306590257879641</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>20</v>
+      </c>
+      <c r="H10">
+        <v>1000</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>23.266666666666669</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>6058</v>
+      </c>
+      <c r="C11" s="15">
+        <v>4.9442605329428515</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>8.7955000000000019E-2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>11.369450287078617</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>20</v>
+      </c>
+      <c r="H11">
+        <v>1000</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>117.27333333333335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="6">
+        <v>4888</v>
+      </c>
+      <c r="C12">
+        <v>4.4196088349081029</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>2.6279000000000014E-2</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>38.053198371323091</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>20</v>
+      </c>
+      <c r="H12">
+        <v>1000</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>35.038666666666686</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>1282</v>
+      </c>
+      <c r="C13">
+        <v>4.3043397048923389</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>2.0153000000000025E-2</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>49.620403910087767</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>20</v>
+      </c>
+      <c r="H13">
+        <v>1000</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>26.8706666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <v>2596</v>
+      </c>
+      <c r="C14" s="15">
+        <v>4.4422915862860712</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>2.7688000000000022E-2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>36.116729268997375</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <v>20</v>
+      </c>
+      <c r="H14">
+        <v>1000</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>36.91733333333336</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:C14">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C14">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C14">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B14">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2152,54 +3864,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O16">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O17:O26">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M16">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M17:M26">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>"X"</formula>
+  <conditionalFormatting sqref="B2:B14">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="B21:B22 B26 B17 B18:B20" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
This morning's work: - validated ckt24; just J1 to go now - script written to automate finding a linearization point and sensible voltage bounds -  tidied up some other bits and pieces
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA136C9-DF7E-4252-AE47-AAC65AC6B751}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="plotTts" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="59">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -207,7 +208,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -809,7 +810,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -927,7 +927,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1616,7 +1615,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1896,11 +1901,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2528,14 +2533,14 @@
       <c r="M13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" t="s">
-        <v>50</v>
-      </c>
-      <c r="R13">
-        <v>1</v>
+      <c r="N13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2585,7 +2590,7 @@
         <v>50</v>
       </c>
       <c r="R14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3375,10 +3380,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
All networks now have a linear model working that seems to give some sort of reasonable results. A few minor tweaks to chooseLinPoint too.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA136C9-DF7E-4252-AE47-AAC65AC6B751}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CABF8C2-A3D0-4BBA-9C95-735A348EFB68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="56">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -170,15 +170,6 @@
   </si>
   <si>
     <t>log(NBNL)</t>
-  </si>
-  <si>
-    <t>TODO ORDER</t>
-  </si>
-  <si>
-    <t>DIFF</t>
-  </si>
-  <si>
-    <t>HARD</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
@@ -1905,7 +1896,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1960,7 +1951,7 @@
         <v>18</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M1" s="17" t="s">
         <v>26</v>
@@ -1986,7 +1977,7 @@
         <v>27</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>28</v>
@@ -1994,12 +1985,8 @@
       <c r="P2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -2197,7 +2184,7 @@
         <v>31</v>
       </c>
       <c r="S6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -2570,7 +2557,7 @@
         <v>5</v>
       </c>
       <c r="I14" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6">
@@ -2583,14 +2570,14 @@
       <c r="M14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" t="s">
-        <v>50</v>
-      </c>
-      <c r="R14">
-        <v>1</v>
+      <c r="N14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3395,19 +3382,19 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" t="s">
         <v>54</v>
-      </c>
-      <c r="G1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
A whole bunch of changes based on todays work. 1. the original script charFuncMcVal_v2 has had a lot tidied up. 2. charFuncMcVal_v2 has also been brahcned to a new script just for making hosting capacity calculations (linHcCalcs) 3. a folder for results has been created and a script written for starting to plot the results of these as they come out. Calculating results from OpenDSS is very slow at this stage and feels quite error prone.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CABF8C2-A3D0-4BBA-9C95-735A348EFB68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F5FEED-06BC-4C60-9D3C-B25071B2A655}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="57">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>slns per s-1</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -318,7 +321,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -351,12 +354,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -1893,30 +1895,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1"/>
-    <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1924,109 +1927,111 @@
         <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="N1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="4" t="s">
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S2" s="4"/>
+    </row>
+    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6">
         <v>4</v>
       </c>
-      <c r="D3" s="6">
+      <c r="E3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="6">
-        <f>LOG(D3*C3)</f>
+      <c r="F3" s="6">
+        <f>LOG(E3*D3)</f>
         <v>0.6020599913279624</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
       <c r="I3" s="6">
         <v>0</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="6">
+      <c r="L3" s="6">
         <v>5.4</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="M3" s="6"/>
       <c r="N3" s="8" t="s">
         <v>31</v>
       </c>
@@ -2036,46 +2041,49 @@
       <c r="P3" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="Q3" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
         <v>16</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>15</v>
       </c>
-      <c r="E4" s="13">
-        <f t="shared" ref="E4:E26" si="0">LOG(D4*C4)</f>
+      <c r="F4" s="13">
+        <f t="shared" ref="F4:F26" si="0">LOG(E4*D4)</f>
         <v>2.3802112417116059</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1.5</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>3.6</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <f>LOG10(703)</f>
         <v>2.8469553250198238</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N4" s="1" t="s">
         <v>30</v>
       </c>
@@ -2085,46 +2093,49 @@
       <c r="P4" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
         <v>37</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>68</v>
       </c>
-      <c r="E5" s="13">
+      <c r="F5" s="13">
         <f t="shared" si="0"/>
         <v>3.4007106367732312</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>24.9</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
       </c>
       <c r="I5">
         <v>2</v>
       </c>
       <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
         <v>50</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>2</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <f>LOG10(4000)</f>
         <v>3.6020599913279625</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N5" s="1" t="s">
         <v>30</v>
       </c>
@@ -2134,48 +2145,51 @@
       <c r="P5" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
         <v>39</v>
       </c>
-      <c r="D6">
-        <v>30</v>
-      </c>
-      <c r="E6" s="13">
+      <c r="E6">
+        <v>30</v>
+      </c>
+      <c r="F6" s="13">
         <f t="shared" si="0"/>
         <v>3.0681858617461617</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>4.8</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
       <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
         <v>1</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>3</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>2.6</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f>LOG10(2907)</f>
         <v>3.4634450317704277</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>31</v>
@@ -2183,49 +2197,52 @@
       <c r="P6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S6" t="s">
+      <c r="Q6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
         <v>132</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>92</v>
       </c>
-      <c r="E7" s="13">
+      <c r="F7" s="13">
         <f t="shared" si="0"/>
         <v>4.0843617585514052</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>2.4</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>4</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>3</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>6</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>3.6</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f>LOG10(4965)</f>
         <v>3.6959192528313998</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N7" s="1" t="s">
         <v>30</v>
       </c>
@@ -2235,152 +2252,164 @@
       <c r="P7" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
         <v>4876</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>2355</v>
       </c>
-      <c r="E8" s="13">
+      <c r="F8" s="13">
         <f t="shared" si="0"/>
         <v>7.0600546084112592</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>7.2</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>4</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>12</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>17</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>12.05</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f>LOG10(275763)</f>
         <v>5.4405359950748213</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
         <v>907</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>55</v>
       </c>
-      <c r="E9" s="13">
+      <c r="F9" s="13">
         <f t="shared" si="0"/>
         <v>4.6979699765543392</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
         <v>0.3</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>5.5E-2</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f>LOG10(5144)</f>
         <v>3.7113009599161657</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>31</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>25</v>
       </c>
       <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="D10">
         <v>390</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>694</v>
       </c>
-      <c r="E10" s="13">
+      <c r="F10" s="13">
         <f t="shared" si="0"/>
         <v>5.4324240774813539</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>13.8</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
       <c r="I10">
         <v>0</v>
       </c>
-      <c r="K10">
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="L10">
         <v>42.8</v>
       </c>
-      <c r="L10" s="15">
+      <c r="M10" s="15">
         <f>LOG10(12061)</f>
         <v>4.0813833174622856</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -2388,149 +2417,158 @@
         <v>14</v>
       </c>
       <c r="C11" s="6">
+        <v>17</v>
+      </c>
+      <c r="D11" s="6">
         <v>2998</v>
       </c>
-      <c r="D11" s="6">
+      <c r="E11" s="6">
         <v>1379</v>
       </c>
-      <c r="E11" s="6">
+      <c r="F11" s="6">
         <f t="shared" si="0"/>
         <v>6.6163958946881101</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="7">
+      <c r="H11" s="7">
         <v>12.47</v>
       </c>
-      <c r="H11" s="6">
+      <c r="I11" s="6">
         <v>4</v>
       </c>
-      <c r="I11" s="6">
-        <v>0</v>
-      </c>
       <c r="J11" s="6">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6">
         <v>5</v>
       </c>
-      <c r="K11" s="6">
+      <c r="L11" s="6">
         <v>16.3</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <f>LOG10(32321)</f>
         <v>4.50948478922394</v>
       </c>
-      <c r="M11" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="N11" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O11" s="8" t="s">
         <v>31</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="18">
+        <v>18</v>
+      </c>
+      <c r="D12">
         <v>1255</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>868</v>
       </c>
-      <c r="E12" s="13">
+      <c r="F12" s="13">
         <f t="shared" si="0"/>
         <v>6.0371634509935488</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>12.47</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>2</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
       <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
         <v>4</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>19.3</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <f>LOG10(17450)</f>
         <v>4.2417954312951984</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>31</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13">
+        <v>22</v>
+      </c>
+      <c r="D13">
         <v>6058</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>3891</v>
       </c>
-      <c r="E13" s="13">
+      <c r="F13" s="13">
         <f t="shared" si="0"/>
         <v>7.3723904998005798</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>34.5</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>3</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>1</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>10</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>69.400000000000006</v>
       </c>
-      <c r="L13" s="15">
+      <c r="M13" s="15">
         <f>LOG10(87955)</f>
         <v>4.9442605329428515</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N13" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -2538,84 +2576,87 @@
         <v>22</v>
       </c>
       <c r="C14" s="6">
+        <v>19</v>
+      </c>
+      <c r="D14" s="6">
         <v>4888</v>
       </c>
-      <c r="D14" s="6">
+      <c r="E14" s="6">
         <v>1384</v>
       </c>
-      <c r="E14" s="6">
+      <c r="F14" s="6">
         <f t="shared" si="0"/>
         <v>6.8302672873552366</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="7">
+      <c r="H14" s="7">
         <v>12.47</v>
       </c>
-      <c r="H14" s="6">
+      <c r="I14" s="6">
         <v>5</v>
       </c>
-      <c r="I14" s="6">
+      <c r="J14" s="6">
         <v>9</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6">
+      <c r="K14" s="6"/>
+      <c r="L14" s="6">
         <v>11.6</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <f>LOG10(26279)</f>
         <v>4.4196088349081029</v>
       </c>
-      <c r="M14" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="N14" s="8" t="s">
         <v>30</v>
       </c>
       <c r="O14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="P14" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="Q14" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>23</v>
       </c>
       <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15">
         <v>1282</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>332</v>
       </c>
-      <c r="E15" s="13">
+      <c r="F15" s="13">
         <f t="shared" si="0"/>
         <v>5.6290261088868352</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>13.2</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
-      <c r="K15">
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="L15">
         <v>12.74</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <f>LOG10(20153)</f>
         <v>4.3043397048923389</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N15" s="1" t="s">
         <v>30</v>
       </c>
@@ -2625,538 +2666,553 @@
       <c r="P15" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>24</v>
       </c>
       <c r="C16">
+        <v>21</v>
+      </c>
+      <c r="D16">
         <v>2596</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>1470</v>
       </c>
-      <c r="E16" s="13">
+      <c r="F16" s="13">
         <f t="shared" si="0"/>
         <v>6.5816220228765081</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>12.47</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>3</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>1</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>15.67</v>
       </c>
-      <c r="L16" s="15">
+      <c r="M16" s="15">
         <f>LOG10(27688)</f>
         <v>4.4422915862860712</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="11"/>
+      <c r="D17" s="6">
         <v>907</v>
       </c>
-      <c r="D17" s="6">
+      <c r="E17" s="6">
         <v>55</v>
       </c>
-      <c r="E17" s="6">
+      <c r="F17" s="6">
         <f t="shared" si="0"/>
         <v>4.6979699765543392</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="7">
+      <c r="H17" s="7">
         <v>0.41599999999999998</v>
       </c>
-      <c r="H17" s="6">
-        <v>0</v>
-      </c>
       <c r="I17" s="6">
         <v>0</v>
       </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6">
-        <f>D17*0.001</f>
+      <c r="J17" s="6">
+        <v>0</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6">
+        <f>E17*0.001</f>
         <v>5.5E-2</v>
       </c>
-      <c r="L17">
-        <f t="shared" ref="L17:L26" si="1">LOG10(1)</f>
-        <v>0</v>
-      </c>
-      <c r="M17" s="8" t="s">
-        <v>30</v>
+      <c r="M17">
+        <f t="shared" ref="M17:M26" si="1">LOG10(1)</f>
+        <v>0</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O17" s="8" t="s">
         <v>31</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="Q17" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="12"/>
+      <c r="D18">
         <v>2287</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>175</v>
       </c>
-      <c r="E18" s="13">
+      <c r="F18" s="13">
         <f t="shared" si="0"/>
         <v>5.602304213293043</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
       <c r="I18">
         <v>0</v>
       </c>
-      <c r="K18" s="13">
-        <f t="shared" ref="K18:K26" si="2">D18*0.001</f>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="L18" s="13">
+        <f t="shared" ref="L18:L26" si="2">E18*0.001</f>
         <v>0.17500000000000002</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>31</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="12"/>
+      <c r="D19">
         <v>1304</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>94</v>
       </c>
-      <c r="E19" s="13">
+      <c r="F19" s="13">
         <f t="shared" si="0"/>
         <v>5.0884054449956002</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
       <c r="I19">
         <v>0</v>
       </c>
-      <c r="K19" s="13">
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="L19" s="13">
         <f t="shared" si="2"/>
         <v>9.4E-2</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>31</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="12"/>
+      <c r="D20">
         <v>375</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>24</v>
       </c>
-      <c r="E20" s="13">
+      <c r="F20" s="13">
         <f t="shared" si="0"/>
         <v>3.9542425094393248</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
       <c r="I20">
         <v>0</v>
       </c>
-      <c r="K20" s="13">
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="L20" s="13">
         <f t="shared" si="2"/>
         <v>2.4E-2</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M20" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>31</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="12"/>
+      <c r="D21">
         <v>1605</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>115</v>
       </c>
-      <c r="E21" s="13">
+      <c r="F21" s="13">
         <f t="shared" si="0"/>
         <v>5.2661728770945029</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H21" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
       <c r="I21">
         <v>0</v>
       </c>
-      <c r="K21" s="13">
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="L21" s="13">
         <f t="shared" si="2"/>
         <v>0.115</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>31</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="12"/>
+      <c r="D22">
         <v>1545</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>186</v>
       </c>
-      <c r="E22" s="13">
+      <c r="F22" s="13">
         <f t="shared" si="0"/>
         <v>5.4584414279787694</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
       <c r="I22">
         <v>0</v>
       </c>
-      <c r="K22" s="13">
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="L22" s="13">
         <f t="shared" si="2"/>
         <v>0.186</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>31</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <v>193</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="12"/>
+      <c r="D23">
         <v>1391</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>65</v>
       </c>
-      <c r="E23" s="13">
+      <c r="F23" s="13">
         <f t="shared" si="0"/>
         <v>4.9562404866349024</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
       <c r="I23">
         <v>0</v>
       </c>
-      <c r="K23" s="13">
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="L23" s="13">
         <f t="shared" si="2"/>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M23" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>31</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>162</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="12"/>
+      <c r="D24">
         <v>1077</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>73</v>
       </c>
-      <c r="E24" s="13">
+      <c r="F24" s="13">
         <f t="shared" si="0"/>
         <v>4.8955385634184374</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
       <c r="I24">
         <v>0</v>
       </c>
-      <c r="K24" s="13">
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="L24" s="13">
         <f t="shared" si="2"/>
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>31</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25" s="12">
         <v>213</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="12"/>
+      <c r="D25">
         <v>844</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>67</v>
       </c>
-      <c r="E25" s="13">
+      <c r="F25" s="13">
         <f t="shared" si="0"/>
         <v>4.7524172493264816</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="2">
+      <c r="H25" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
       <c r="I25">
         <v>0</v>
       </c>
-      <c r="K25" s="13">
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="L25" s="13">
         <f t="shared" si="2"/>
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>31</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="12"/>
+      <c r="D26">
         <v>375</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>24</v>
       </c>
-      <c r="E26" s="13">
+      <c r="F26" s="13">
         <f t="shared" si="0"/>
         <v>3.9542425094393248</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>34</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
       <c r="I26">
         <v>0</v>
       </c>
-      <c r="K26" s="13">
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="L26" s="13">
         <f t="shared" si="2"/>
         <v>2.4E-2</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M26" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>31</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="M1:P1"/>
+  <mergeCells count="1">
+    <mergeCell ref="N1:Q1"/>
   </mergeCells>
-  <conditionalFormatting sqref="M3:M16 O3:O16">
+  <conditionalFormatting sqref="N3:N16 P3:P16">
     <cfRule type="cellIs" dxfId="21" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3167,7 +3223,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C16">
+  <conditionalFormatting sqref="D3:D16">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -3179,7 +3235,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:F16 F17:F26 E4:E26">
+  <conditionalFormatting sqref="E3:G16 G17:G26 F4:F26">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -3191,7 +3247,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:I16 H18:I27">
+  <conditionalFormatting sqref="I3:J16 I18:J27">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -3203,7 +3259,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H16 H18:H27">
+  <conditionalFormatting sqref="I3:I16 I18:I27">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -3213,7 +3269,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I16 I18:I27">
+  <conditionalFormatting sqref="J3:J16 J18:J27">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -3223,7 +3279,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:L16 L10:L26">
+  <conditionalFormatting sqref="L3:M16 M10:M26">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -3233,12 +3289,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F26">
+  <conditionalFormatting sqref="G3:G26">
     <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O17:O26">
+  <conditionalFormatting sqref="P17:P26">
     <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3249,7 +3305,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M17:M26">
+  <conditionalFormatting sqref="N17:N26">
     <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3260,7 +3316,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:I26">
+  <conditionalFormatting sqref="I3:J26">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -3270,7 +3326,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:E26">
+  <conditionalFormatting sqref="D3:F26">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -3282,7 +3338,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:L26">
+  <conditionalFormatting sqref="L3:M26">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -3292,7 +3348,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E26">
+  <conditionalFormatting sqref="F3:F26">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -3304,7 +3360,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P16">
+  <conditionalFormatting sqref="Q3:Q16">
     <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3315,7 +3371,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P17:P26">
+  <conditionalFormatting sqref="Q17:Q26">
     <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3326,7 +3382,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N16">
+  <conditionalFormatting sqref="O3:O16">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3337,7 +3393,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N17:N26">
+  <conditionalFormatting sqref="O17:O26">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3348,7 +3404,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L26">
+  <conditionalFormatting sqref="M3:M26">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Main thing: adding source impedances to all of the networks for more accurate calculations (particularly those networks without regulators), and also for checking voltage devation.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F5FEED-06BC-4C60-9D3C-B25071B2A655}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E673E71D-D2F1-42C0-AF5B-09CFFD9A94F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="plotTts" sheetId="2" r:id="rId2"/>
+    <sheet name="master" sheetId="1" r:id="rId1"/>
+    <sheet name="sourceParams" sheetId="3" r:id="rId2"/>
+    <sheet name="plotTts" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="73">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -197,13 +198,61 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>MVAsc3</t>
+  </si>
+  <si>
+    <t>MVAsc1</t>
+  </si>
+  <si>
+    <t>X0</t>
+  </si>
+  <si>
+    <t>ISC3</t>
+  </si>
+  <si>
+    <t>ISC1</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
+  </si>
+  <si>
+    <t>Base:</t>
+  </si>
+  <si>
+    <t>basekv</t>
+  </si>
+  <si>
+    <t>X1R1</t>
+  </si>
+  <si>
+    <t>X0R0</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>SRC Z</t>
+  </si>
+  <si>
+    <t>NB problems converging</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,8 +276,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,8 +303,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -314,14 +375,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -354,19 +431,90 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="4"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Heading 4" xfId="2" builtinId="19"/>
+    <cellStyle name="Input" xfId="4" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="3" builtinId="25"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1895,10 +2043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,11 +2063,12 @@
     <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.28515625" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1959,50 +2108,56 @@
       <c r="M1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
       <c r="M2" s="14"/>
       <c r="N2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="4"/>
       <c r="S2" s="4"/>
-    </row>
-    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T2" s="4"/>
+    </row>
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="D3" s="6">
         <v>4</v>
       </c>
@@ -2031,7 +2186,9 @@
       <c r="L3" s="6">
         <v>5.4</v>
       </c>
-      <c r="M3" s="6"/>
+      <c r="M3" s="21" t="s">
+        <v>30</v>
+      </c>
       <c r="N3" s="8" t="s">
         <v>31</v>
       </c>
@@ -2044,8 +2201,11 @@
       <c r="Q3" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="R3" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -2096,8 +2256,11 @@
       <c r="Q4" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -2148,8 +2311,11 @@
       <c r="Q5" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -2189,10 +2355,10 @@
         <v>3.4634450317704277</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>31</v>
@@ -2200,11 +2366,14 @@
       <c r="Q6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T6" t="s">
+      <c r="R6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -2244,7 +2413,7 @@
         <v>3.6959192528313998</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>30</v>
@@ -2255,8 +2424,11 @@
       <c r="Q7" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -2296,19 +2468,22 @@
         <v>5.4405359950748213</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="P8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Q8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -2351,16 +2526,19 @@
         <v>30</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>25</v>
       </c>
@@ -2400,16 +2578,19 @@
         <v>30</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -2452,23 +2633,26 @@
         <v>4.50948478922394</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P11" s="8" t="s">
         <v>31</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="R11" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="17">
         <v>18</v>
       </c>
       <c r="D12">
@@ -2507,16 +2691,19 @@
         <v>30</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -2562,13 +2749,16 @@
         <v>30</v>
       </c>
       <c r="P13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Q13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -2615,13 +2805,19 @@
         <v>30</v>
       </c>
       <c r="P14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="Q14" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="R14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="S14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -2669,8 +2865,11 @@
       <c r="Q15" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>24</v>
       </c>
@@ -2713,20 +2912,25 @@
         <v>30</v>
       </c>
       <c r="P16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Q16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="19" t="s">
+        <v>70</v>
+      </c>
       <c r="D17" s="6">
         <v>907</v>
       </c>
@@ -2755,27 +2959,32 @@
         <v>5.5E-2</v>
       </c>
       <c r="M17">
-        <f t="shared" ref="M17:M26" si="1">LOG10(1)</f>
-        <v>0</v>
+        <f>LOG10(10388)</f>
+        <v>4.0165319409572655</v>
       </c>
       <c r="N17" s="8" t="s">
         <v>30</v>
       </c>
       <c r="O17" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P17" s="8" t="s">
         <v>31</v>
       </c>
       <c r="Q17" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="R17" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="D18">
         <v>2287</v>
       </c>
@@ -2799,31 +3008,36 @@
         <v>0</v>
       </c>
       <c r="L18" s="13">
-        <f t="shared" ref="L18:L26" si="2">E18*0.001</f>
+        <f t="shared" ref="L18:L26" si="1">E18*0.001</f>
         <v>0.17500000000000002</v>
       </c>
       <c r="M18">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>LOG10(24732)</f>
+        <v>4.3932592378268378</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="D19">
         <v>1304</v>
       </c>
@@ -2847,31 +3061,36 @@
         <v>0</v>
       </c>
       <c r="L19" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9.4E-2</v>
       </c>
       <c r="M19">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>LOG10(24431)</f>
+        <v>4.3879412437066989</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="12"/>
+      <c r="C20" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="D20">
         <v>375</v>
       </c>
@@ -2895,31 +3114,36 @@
         <v>0</v>
       </c>
       <c r="L20" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.4E-2</v>
       </c>
       <c r="M20">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>LOG10(6773)</f>
+        <v>3.8307810756063612</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="12"/>
+      <c r="C21" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="D21">
         <v>1605</v>
       </c>
@@ -2943,31 +3167,36 @@
         <v>0</v>
       </c>
       <c r="L21" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.115</v>
       </c>
       <c r="M21">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>LOG10(26276)</f>
+        <v>4.4195592531957208</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="12"/>
+      <c r="C22" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="D22">
         <v>1545</v>
       </c>
@@ -2991,31 +3220,36 @@
         <v>0</v>
       </c>
       <c r="L22" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.186</v>
       </c>
       <c r="M22">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>LOG10(20720)</f>
+        <v>4.3163897510731957</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <v>193</v>
       </c>
-      <c r="C23" s="12"/>
+      <c r="C23" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="D23">
         <v>1391</v>
       </c>
@@ -3039,31 +3273,36 @@
         <v>0</v>
       </c>
       <c r="L23" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="M23">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>LOG10(16241)</f>
+        <v>4.2106127663528978</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P23" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>162</v>
       </c>
-      <c r="C24" s="12"/>
+      <c r="C24" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="D24">
         <v>1077</v>
       </c>
@@ -3087,31 +3326,36 @@
         <v>0</v>
       </c>
       <c r="L24" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="M24">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>LOG10(10072)</f>
+        <v>4.0031157170998064</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B25" s="12">
         <v>213</v>
       </c>
-      <c r="C25" s="12"/>
+      <c r="C25" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="D25">
         <v>844</v>
       </c>
@@ -3135,31 +3379,36 @@
         <v>0</v>
       </c>
       <c r="L25" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="M25">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>LOG10(7623)</f>
+        <v>3.882125919770032</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="12"/>
+      <c r="C26" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="D26">
         <v>375</v>
       </c>
@@ -3183,48 +3432,51 @@
         <v>0</v>
       </c>
       <c r="L26" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.4E-2</v>
       </c>
       <c r="M26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>LOG10(5757)</f>
+        <v>3.7601962294551341</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N1:R1"/>
   </mergeCells>
-  <conditionalFormatting sqref="N3:N16 P3:P16">
-    <cfRule type="cellIs" dxfId="21" priority="31" operator="equal">
+  <conditionalFormatting sqref="N3:N16 Q3:Q16">
+    <cfRule type="cellIs" dxfId="27" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="38" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="39" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D16">
-    <cfRule type="colorScale" priority="30">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3236,7 +3488,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:G16 G17:G26 F4:F26">
-    <cfRule type="colorScale" priority="29">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3248,7 +3500,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:J16 I18:J27">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3260,7 +3512,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I16 I18:I27">
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3270,7 +3522,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J16 J18:J27">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3280,7 +3532,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:M16 M10:M26">
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3290,34 +3542,34 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G26">
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P17:P26">
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+  <conditionalFormatting sqref="Q17:Q26">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="28" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17:N26">
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="25" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="26" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:J26">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3327,7 +3579,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:F26">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3339,7 +3591,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:M26">
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3349,7 +3601,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F26">
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3360,7 +3612,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q16">
+  <conditionalFormatting sqref="R3:R16">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R17:R26">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P16">
     <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3371,7 +3645,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q17:Q26">
+  <conditionalFormatting sqref="P17:P26">
     <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3382,36 +3656,36 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O16">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O17:O26">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="M3:M26">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:O16">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17:O26">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3423,11 +3697,668 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5A0278A-93BE-4383-9DF3-975F5622E3E8}">
+  <dimension ref="A1:M26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1.6037999999999999</v>
+      </c>
+      <c r="D2" s="18">
+        <v>6.4150999999999998</v>
+      </c>
+      <c r="E2" s="18">
+        <v>1.796</v>
+      </c>
+      <c r="F2" s="18">
+        <v>5.3880999999999997</v>
+      </c>
+      <c r="G2" s="18">
+        <v>2000</v>
+      </c>
+      <c r="H2" s="18">
+        <v>2100</v>
+      </c>
+      <c r="I2" s="18">
+        <v>10041</v>
+      </c>
+      <c r="J2" s="18">
+        <v>10543</v>
+      </c>
+      <c r="K2" s="18">
+        <v>4</v>
+      </c>
+      <c r="L2" s="18">
+        <v>3</v>
+      </c>
+      <c r="M2" s="18">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <f>C$2*($G$2/$G4)</f>
+        <v>0.16037999999999999</v>
+      </c>
+      <c r="D4">
+        <f>D$2*($G$2/$G4)</f>
+        <v>0.64151000000000002</v>
+      </c>
+      <c r="E4">
+        <f>E2/10</f>
+        <v>0.17960000000000001</v>
+      </c>
+      <c r="F4">
+        <f>F2/10</f>
+        <v>0.53881000000000001</v>
+      </c>
+      <c r="G4" s="18">
+        <v>20000</v>
+      </c>
+      <c r="H4" s="18">
+        <v>21000</v>
+      </c>
+      <c r="M4" s="18">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>5.7736000000000003E-3</v>
+      </c>
+      <c r="D5">
+        <v>2.3094E-2</v>
+      </c>
+      <c r="E5">
+        <v>2.1358000000000001</v>
+      </c>
+      <c r="F5">
+        <v>6.4074</v>
+      </c>
+      <c r="G5" s="18">
+        <v>200000</v>
+      </c>
+      <c r="M5" s="18">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>6.4151E-2</v>
+      </c>
+      <c r="D6">
+        <v>0.25659999999999999</v>
+      </c>
+      <c r="E6">
+        <v>7.1841000000000002E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.21551999999999999</v>
+      </c>
+      <c r="G6" s="18">
+        <v>200000</v>
+      </c>
+      <c r="H6" s="18">
+        <v>210000</v>
+      </c>
+      <c r="M6" s="18">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="18">
+        <v>0</v>
+      </c>
+      <c r="D7" s="18">
+        <v>1E-4</v>
+      </c>
+      <c r="E7" s="18">
+        <v>0</v>
+      </c>
+      <c r="F7" s="18">
+        <v>1E-4</v>
+      </c>
+      <c r="M7" s="18">
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="18">
+        <v>0</v>
+      </c>
+      <c r="D8" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="E8" s="18">
+        <v>0</v>
+      </c>
+      <c r="F8" s="18">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>0.51344000000000001</v>
+      </c>
+      <c r="D9">
+        <v>2.0537000000000001</v>
+      </c>
+      <c r="E9">
+        <v>1203.7</v>
+      </c>
+      <c r="F9">
+        <v>3611</v>
+      </c>
+      <c r="I9" s="18">
+        <v>3000</v>
+      </c>
+      <c r="J9" s="18">
+        <v>5</v>
+      </c>
+      <c r="M9" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>6.4151E-2</v>
+      </c>
+      <c r="D10">
+        <v>0.25659999999999999</v>
+      </c>
+      <c r="E10">
+        <v>-0.14523</v>
+      </c>
+      <c r="F10">
+        <v>-0.43568000000000001</v>
+      </c>
+      <c r="G10" s="18">
+        <v>200000</v>
+      </c>
+      <c r="H10" s="18">
+        <v>2000000</v>
+      </c>
+      <c r="M10" s="18">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="18">
+        <v>0</v>
+      </c>
+      <c r="D11" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="E11" s="18">
+        <v>0</v>
+      </c>
+      <c r="F11" s="18">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="18">
+        <v>2.3140000000000001</v>
+      </c>
+      <c r="D12" s="18">
+        <v>28.52</v>
+      </c>
+      <c r="E12" s="18">
+        <v>1E-4</v>
+      </c>
+      <c r="F12" s="18">
+        <v>1E-4</v>
+      </c>
+      <c r="M12" s="18">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="18">
+        <v>0.63</v>
+      </c>
+      <c r="D13" s="18">
+        <v>6.72</v>
+      </c>
+      <c r="E13" s="18">
+        <v>4.07</v>
+      </c>
+      <c r="F13" s="18">
+        <v>15.55</v>
+      </c>
+      <c r="M13" s="18">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="18">
+        <v>1.3759999999999999</v>
+      </c>
+      <c r="D14" s="18">
+        <v>14.257</v>
+      </c>
+      <c r="E14" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="F14" s="18">
+        <v>8.2029999999999994</v>
+      </c>
+      <c r="M14" s="18">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="18">
+        <v>0.80626299999999995</v>
+      </c>
+      <c r="D15" s="18">
+        <v>7.8137910000000002</v>
+      </c>
+      <c r="E15" s="18">
+        <v>0.91630699999999998</v>
+      </c>
+      <c r="F15" s="18">
+        <v>14.556789999999999</v>
+      </c>
+      <c r="M15" s="18">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="18">
+        <v>5.1799999999999999E-2</v>
+      </c>
+      <c r="D16" s="18">
+        <v>0.15554999999999999</v>
+      </c>
+      <c r="E16" s="18">
+        <v>5.1799999999999999E-2</v>
+      </c>
+      <c r="F16" s="18">
+        <v>0.155</v>
+      </c>
+      <c r="M16" s="18">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17">
+        <v>0.51344000000000001</v>
+      </c>
+      <c r="D17">
+        <v>2.0537000000000001</v>
+      </c>
+      <c r="E17">
+        <v>1.0729</v>
+      </c>
+      <c r="F17">
+        <v>3.2185999999999999</v>
+      </c>
+      <c r="I17" s="18">
+        <v>3000</v>
+      </c>
+      <c r="J17" s="18">
+        <v>2500</v>
+      </c>
+      <c r="M17" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18">
+        <v>0.51344000000000001</v>
+      </c>
+      <c r="D18">
+        <v>2.0537000000000001</v>
+      </c>
+      <c r="E18">
+        <v>1.0729</v>
+      </c>
+      <c r="F18">
+        <v>3.2185999999999999</v>
+      </c>
+      <c r="I18" s="18">
+        <v>3000</v>
+      </c>
+      <c r="J18" s="18">
+        <v>2500</v>
+      </c>
+      <c r="M18" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19">
+        <v>0.51344000000000001</v>
+      </c>
+      <c r="D19">
+        <v>2.0537000000000001</v>
+      </c>
+      <c r="E19">
+        <v>1.0729</v>
+      </c>
+      <c r="F19">
+        <v>3.2185999999999999</v>
+      </c>
+      <c r="I19" s="18">
+        <v>3000</v>
+      </c>
+      <c r="J19" s="18">
+        <v>2500</v>
+      </c>
+      <c r="M19" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20">
+        <v>0.51344000000000001</v>
+      </c>
+      <c r="D20">
+        <v>2.0537000000000001</v>
+      </c>
+      <c r="E20">
+        <v>1.0729</v>
+      </c>
+      <c r="F20">
+        <v>3.2185999999999999</v>
+      </c>
+      <c r="I20" s="18">
+        <v>3000</v>
+      </c>
+      <c r="J20" s="18">
+        <v>2500</v>
+      </c>
+      <c r="M20" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21">
+        <v>0.51344000000000001</v>
+      </c>
+      <c r="D21">
+        <v>2.0537000000000001</v>
+      </c>
+      <c r="E21">
+        <v>1.0729</v>
+      </c>
+      <c r="F21">
+        <v>3.2185999999999999</v>
+      </c>
+      <c r="I21" s="18">
+        <v>3000</v>
+      </c>
+      <c r="J21" s="18">
+        <v>2500</v>
+      </c>
+      <c r="M21" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>0.51344000000000001</v>
+      </c>
+      <c r="D22">
+        <v>2.0537000000000001</v>
+      </c>
+      <c r="E22">
+        <v>1.0729</v>
+      </c>
+      <c r="F22">
+        <v>3.2185999999999999</v>
+      </c>
+      <c r="I22" s="18">
+        <v>3000</v>
+      </c>
+      <c r="J22" s="18">
+        <v>2500</v>
+      </c>
+      <c r="M22" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="12">
+        <v>193</v>
+      </c>
+      <c r="C23">
+        <v>0.51344000000000001</v>
+      </c>
+      <c r="D23">
+        <v>2.0537000000000001</v>
+      </c>
+      <c r="E23">
+        <v>1.0729</v>
+      </c>
+      <c r="F23">
+        <v>3.2185999999999999</v>
+      </c>
+      <c r="I23" s="18">
+        <v>3000</v>
+      </c>
+      <c r="J23" s="18">
+        <v>2500</v>
+      </c>
+      <c r="M23" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="12">
+        <v>162</v>
+      </c>
+      <c r="C24">
+        <v>0.51344000000000001</v>
+      </c>
+      <c r="D24">
+        <v>2.0537000000000001</v>
+      </c>
+      <c r="E24">
+        <v>1.0729</v>
+      </c>
+      <c r="F24">
+        <v>3.2185999999999999</v>
+      </c>
+      <c r="I24" s="18">
+        <v>3000</v>
+      </c>
+      <c r="J24" s="18">
+        <v>2500</v>
+      </c>
+      <c r="M24" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="12">
+        <v>213</v>
+      </c>
+      <c r="C25">
+        <v>0.51344000000000001</v>
+      </c>
+      <c r="D25">
+        <v>2.0537000000000001</v>
+      </c>
+      <c r="E25">
+        <v>1.0729</v>
+      </c>
+      <c r="F25">
+        <v>3.2185999999999999</v>
+      </c>
+      <c r="I25" s="18">
+        <v>3000</v>
+      </c>
+      <c r="J25" s="18">
+        <v>2500</v>
+      </c>
+      <c r="M25" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26">
+        <v>0.51344000000000001</v>
+      </c>
+      <c r="D26">
+        <v>2.0537000000000001</v>
+      </c>
+      <c r="E26">
+        <v>1.0729</v>
+      </c>
+      <c r="F26">
+        <v>3.2185999999999999</v>
+      </c>
+      <c r="I26" s="18">
+        <v>3000</v>
+      </c>
+      <c r="J26" s="18">
+        <v>2500</v>
+      </c>
+      <c r="M26" s="18">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mostly running analyses to get some results for the meeting today.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E673E71D-D2F1-42C0-AF5B-09CFFD9A94F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
     <sheet name="sourceParams" sheetId="3" r:id="rId2"/>
     <sheet name="plotTts" sheetId="2" r:id="rId3"/>
+    <sheet name="notes" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="90">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -246,13 +246,64 @@
   </si>
   <si>
     <t>NB problems converging</t>
+  </si>
+  <si>
+    <t>http://smartgrid.epri.com/SimulationTool.aspx</t>
+  </si>
+  <si>
+    <t>https://dpv.epri.com/feeder_j.html</t>
+  </si>
+  <si>
+    <t>https://dpv.epri.com/feeder_k.html</t>
+  </si>
+  <si>
+    <t>https://dpv.epri.com/feeder_m.html</t>
+  </si>
+  <si>
+    <t>96% Res</t>
+  </si>
+  <si>
+    <t>39% Res</t>
+  </si>
+  <si>
+    <t>87% Res</t>
+  </si>
+  <si>
+    <t>"Primarily residential"</t>
+  </si>
+  <si>
+    <t>Mixture of res + commercial</t>
+  </si>
+  <si>
+    <t>Mixture of res + comm + ind</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/stamp/stamp.jsp?tp=&amp;arnumber=5484381</t>
+  </si>
+  <si>
+    <t>Problem?</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Problem with outlier removal?</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>Timings (3000 LFs)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +330,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -391,14 +450,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -446,10 +506,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Heading 4" xfId="2" builtinId="19"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Input" xfId="4" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="3" builtinId="25"/>
@@ -2042,11 +2104,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2066,6 +2128,8 @@
     <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
     <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2146,7 +2210,9 @@
         <v>29</v>
       </c>
       <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
+      <c r="T2" s="4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -2647,6 +2713,10 @@
       <c r="R11" s="8" t="s">
         <v>30</v>
       </c>
+      <c r="T11">
+        <f>726/60</f>
+        <v>12.1</v>
+      </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -2702,6 +2772,9 @@
       <c r="R12" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="S12" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -2757,6 +2830,10 @@
       <c r="R13" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="T13">
+        <f>3145/60</f>
+        <v>52.416666666666664</v>
+      </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
@@ -2816,6 +2893,10 @@
       <c r="S14" t="s">
         <v>72</v>
       </c>
+      <c r="T14">
+        <f>886/60</f>
+        <v>14.766666666666667</v>
+      </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -2868,6 +2949,10 @@
       <c r="R15" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="T15">
+        <f>188/60</f>
+        <v>3.1333333333333333</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -2919,6 +3004,10 @@
       </c>
       <c r="R16" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="T16">
+        <f>806/60</f>
+        <v>13.433333333333334</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3697,7 +3786,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5A0278A-93BE-4383-9DF3-975F5622E3E8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4354,7 +4443,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4858,4 +4947,346 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="5.28515625" customWidth="1"/>
+    <col min="4" max="4" width="65.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6">
+        <v>17</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="17">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="6">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="12">
+        <v>193</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="12">
+        <v>162</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="12">
+        <v>213</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D11" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
A bunch of changes - Code updated to 'early bindings' as per Davis' notice, which seems to have speeded up calculations by about a factor of 3. This requires syntax to be more correct (e.g. .command -> .Command) - All nominal cases have now been run and timed to check that speeds are in the right ballpark and if the linear model is giving sensible results (it seems to be)
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3CF792-A567-4DA0-AD80-FEBE0CEFDE56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -12,7 +13,7 @@
     <sheet name="plotTts" sheetId="2" r:id="rId3"/>
     <sheet name="notes" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="89">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -110,15 +111,6 @@
     <t>Implemented</t>
   </si>
   <si>
-    <t>Fixed model</t>
-  </si>
-  <si>
-    <t>LTC Model</t>
-  </si>
-  <si>
-    <t>HC Calcs</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -137,12 +129,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>12.47/4.16</t>
-  </si>
-  <si>
-    <t>4.16/2/.277</t>
-  </si>
-  <si>
     <t>kV</t>
   </si>
   <si>
@@ -173,15 +159,6 @@
     <t>log(NBNL)</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t>Tap Model</t>
-  </si>
-  <si>
-    <t>Log(Time to solve) (us)</t>
-  </si>
-  <si>
     <t>Load points</t>
   </si>
   <si>
@@ -242,9 +219,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>SRC Z</t>
-  </si>
-  <si>
     <t>NB problems converging</t>
   </si>
   <si>
@@ -296,13 +270,37 @@
     <t>XX</t>
   </si>
   <si>
-    <t>Timings (3000 LFs)</t>
+    <t>Feeder (MW)</t>
+  </si>
+  <si>
+    <t>Predicted</t>
+  </si>
+  <si>
+    <t>V2 (6000 LFs)</t>
+  </si>
+  <si>
+    <t>Log(t2s) (us)</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Tap</t>
+  </si>
+  <si>
+    <t>LTC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>Zsrc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -503,10 +501,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -2104,35 +2102,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" customWidth="1"/>
     <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.28515625" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -2140,7 +2141,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -2149,13 +2150,13 @@
         <v>13</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>2</v>
@@ -2170,17 +2171,20 @@
         <v>18</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2193,28 +2197,32 @@
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" s="16"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="M2" s="16"/>
+      <c r="N2" s="14"/>
       <c r="O2" s="4" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -2222,7 +2230,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D3" s="6">
         <v>4</v>
@@ -2235,11 +2243,9 @@
         <v>0.6020599913279624</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>36</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="H3" s="7"/>
       <c r="I3" s="6">
         <v>0</v>
       </c>
@@ -2252,26 +2258,29 @@
       <c r="L3" s="6">
         <v>5.4</v>
       </c>
-      <c r="M3" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>31</v>
+      <c r="M3" s="6">
+        <v>5.4</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>27</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -2289,10 +2298,10 @@
         <v>2.3802112417116059</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="H4" s="2">
+        <v>4.16</v>
       </c>
       <c r="I4">
         <v>2</v>
@@ -2307,26 +2316,37 @@
         <v>3.6</v>
       </c>
       <c r="M4">
+        <v>3.6</v>
+      </c>
+      <c r="N4">
         <f>LOG10(703)</f>
         <v>2.8469553250198238</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U4">
+        <f>9/60</f>
+        <v>0.15</v>
+      </c>
+      <c r="V4">
+        <f>(10^N4)*6000*0.000001/60</f>
+        <v>7.0300000000000015E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -2344,7 +2364,7 @@
         <v>3.4007106367732312</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H5" s="2">
         <v>24.9</v>
@@ -2362,26 +2382,37 @@
         <v>2</v>
       </c>
       <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
         <f>LOG10(4000)</f>
         <v>3.6020599913279625</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U5">
+        <f>19/60</f>
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="V5">
+        <f t="shared" ref="V5:V26" si="1">(10^N5)*6000*0.000001/60</f>
+        <v>0.40000000000000063</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -2399,7 +2430,7 @@
         <v>3.0681858617461617</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H6" s="2">
         <v>4.8</v>
@@ -2417,29 +2448,33 @@
         <v>2.6</v>
       </c>
       <c r="M6">
+        <v>2.6</v>
+      </c>
+      <c r="N6">
         <f>LOG10(2907)</f>
         <v>3.4634450317704277</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="O6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="U6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="1"/>
+        <v>0.29070000000000012</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -2457,7 +2492,7 @@
         <v>4.0843617585514052</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H7" s="2">
         <v>2.4</v>
@@ -2475,26 +2510,37 @@
         <v>3.6</v>
       </c>
       <c r="M7">
+        <v>3.6</v>
+      </c>
+      <c r="N7">
         <f>LOG10(4965)</f>
         <v>3.6959192528313998</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="O7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U7">
+        <f>33/60</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="1"/>
+        <v>0.49650000000000016</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -2512,7 +2558,7 @@
         <v>7.0600546084112592</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H8" s="2">
         <v>7.2</v>
@@ -2530,26 +2576,37 @@
         <v>12.05</v>
       </c>
       <c r="M8">
+        <v>12.05</v>
+      </c>
+      <c r="N8">
         <f>LOG10(275763)</f>
         <v>5.4405359950748213</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="O8" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U8">
+        <f>958/60</f>
+        <v>15.966666666666667</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="1"/>
+        <v>27.576300000000046</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -2567,7 +2624,7 @@
         <v>4.6979699765543392</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H9" s="2">
         <v>0.41599999999999998</v>
@@ -2585,26 +2642,37 @@
         <v>5.5E-2</v>
       </c>
       <c r="M9">
+        <v>5.5E-2</v>
+      </c>
+      <c r="N9">
         <f>LOG10(5144)</f>
         <v>3.7113009599161657</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O9" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U9">
+        <f>59/60</f>
+        <v>0.98333333333333328</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="1"/>
+        <v>0.51440000000000086</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>25</v>
       </c>
@@ -2622,7 +2690,7 @@
         <v>5.4324240774813539</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H10" s="2">
         <v>13.8</v>
@@ -2636,27 +2704,38 @@
       <c r="L10">
         <v>42.8</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10">
+        <v>42.8</v>
+      </c>
+      <c r="N10" s="15">
         <f>LOG10(12061)</f>
         <v>4.0813833174622856</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O10" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U10">
+        <f>145/60</f>
+        <v>2.4166666666666665</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="1"/>
+        <v>1.2061000000000024</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -2677,7 +2756,7 @@
         <v>6.6163958946881101</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H11" s="7">
         <v>12.47</v>
@@ -2694,31 +2773,38 @@
       <c r="L11" s="6">
         <v>16.3</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="6">
+        <v>16.3</v>
+      </c>
+      <c r="N11">
         <f>LOG10(32321)</f>
         <v>4.50948478922394</v>
       </c>
-      <c r="N11" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="O11" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="T11">
-        <f>726/60</f>
-        <v>12.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="U11">
+        <f>371/60</f>
+        <v>6.1833333333333336</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="1"/>
+        <v>3.2321000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -2736,7 +2822,7 @@
         <v>6.0371634509935488</v>
       </c>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H12" s="2">
         <v>12.47</v>
@@ -2751,32 +2837,43 @@
         <v>4</v>
       </c>
       <c r="L12">
+        <v>78</v>
+      </c>
+      <c r="M12">
         <v>19.3</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <f>LOG10(17450)</f>
         <v>4.2417954312951984</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O12" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T12" t="s">
+        <v>79</v>
+      </c>
+      <c r="U12">
+        <f>367/60</f>
+        <v>6.1166666666666663</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="1"/>
+        <v>1.7450000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -2794,7 +2891,7 @@
         <v>7.3723904998005798</v>
       </c>
       <c r="G13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H13" s="2">
         <v>34.5</v>
@@ -2809,33 +2906,40 @@
         <v>10</v>
       </c>
       <c r="L13">
+        <v>52.2</v>
+      </c>
+      <c r="M13">
         <v>69.400000000000006</v>
       </c>
-      <c r="M13" s="15">
+      <c r="N13" s="15">
         <f>LOG10(87955)</f>
         <v>4.9442605329428515</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O13" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T13">
-        <f>3145/60</f>
-        <v>52.416666666666664</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U13">
+        <f>1996/60</f>
+        <v>33.266666666666666</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="1"/>
+        <v>8.7955000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -2856,7 +2960,7 @@
         <v>6.8302672873552366</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H14" s="7">
         <v>12.47</v>
@@ -2871,34 +2975,41 @@
       <c r="L14" s="6">
         <v>11.6</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="6">
+        <v>11.6</v>
+      </c>
+      <c r="N14">
         <f>LOG10(26279)</f>
         <v>4.4196088349081029</v>
       </c>
-      <c r="N14" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="O14" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P14" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Q14" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="R14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="S14" t="s">
-        <v>72</v>
-      </c>
-      <c r="T14">
-        <f>886/60</f>
-        <v>14.766666666666667</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T14" t="s">
+        <v>63</v>
+      </c>
+      <c r="U14">
+        <f>551/60</f>
+        <v>9.1833333333333336</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="1"/>
+        <v>2.6279000000000017</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -2916,7 +3027,7 @@
         <v>5.6290261088868352</v>
       </c>
       <c r="G15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H15" s="2">
         <v>13.2</v>
@@ -2931,30 +3042,37 @@
         <v>12.74</v>
       </c>
       <c r="M15">
+        <v>12.74</v>
+      </c>
+      <c r="N15">
         <f>LOG10(20153)</f>
         <v>4.3043397048923389</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O15" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T15">
-        <f>188/60</f>
-        <v>3.1333333333333333</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U15">
+        <f>107/60</f>
+        <v>1.7833333333333334</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="1"/>
+        <v>2.0153000000000025</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>24</v>
       </c>
@@ -2972,7 +3090,7 @@
         <v>6.5816220228765081</v>
       </c>
       <c r="G16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H16" s="2">
         <v>12.47</v>
@@ -2986,39 +3104,46 @@
       <c r="L16">
         <v>15.67</v>
       </c>
-      <c r="M16" s="15">
+      <c r="M16">
+        <v>15.67</v>
+      </c>
+      <c r="N16" s="15">
         <f>LOG10(27688)</f>
         <v>4.4422915862860712</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O16" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T16">
-        <f>806/60</f>
-        <v>13.433333333333334</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U16">
+        <f>445/60</f>
+        <v>7.416666666666667</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="1"/>
+        <v>2.7688000000000015</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>44</v>
-      </c>
       <c r="C17" s="19" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D17" s="6">
         <v>907</v>
@@ -3031,7 +3156,7 @@
         <v>4.6979699765543392</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H17" s="7">
         <v>0.41599999999999998</v>
@@ -3047,32 +3172,39 @@
         <f>E17*0.001</f>
         <v>5.5E-2</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="6">
+        <v>5.5E-2</v>
+      </c>
+      <c r="N17">
         <f>LOG10(10388)</f>
         <v>4.0165319409572655</v>
       </c>
-      <c r="N17" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="O17" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q17" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R17" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="1"/>
+        <v>1.0388000000000011</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D18">
         <v>2287</v>
@@ -3085,7 +3217,7 @@
         <v>5.602304213293043</v>
       </c>
       <c r="G18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H18" s="2">
         <v>0.41599999999999998</v>
@@ -3097,35 +3229,42 @@
         <v>0</v>
       </c>
       <c r="L18" s="13">
-        <f t="shared" ref="L18:L26" si="1">E18*0.001</f>
+        <f t="shared" ref="L18:L26" si="2">E18*0.001</f>
         <v>0.17500000000000002</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="13">
+        <v>0.17500000000000002</v>
+      </c>
+      <c r="N18">
         <f>LOG10(24732)</f>
         <v>4.3932592378268378</v>
       </c>
-      <c r="N18" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O18" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="1"/>
+        <v>2.4732000000000034</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D19">
         <v>1304</v>
@@ -3138,7 +3277,7 @@
         <v>5.0884054449956002</v>
       </c>
       <c r="G19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H19" s="2">
         <v>0.41599999999999998</v>
@@ -3150,35 +3289,42 @@
         <v>0</v>
       </c>
       <c r="L19" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.4E-2</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="13">
+        <v>9.4E-2</v>
+      </c>
+      <c r="N19">
         <f>LOG10(24431)</f>
         <v>4.3879412437066989</v>
       </c>
-      <c r="N19" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O19" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="1"/>
+        <v>2.4431000000000025</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D20">
         <v>375</v>
@@ -3191,7 +3337,7 @@
         <v>3.9542425094393248</v>
       </c>
       <c r="G20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H20" s="2">
         <v>0.41599999999999998</v>
@@ -3203,35 +3349,42 @@
         <v>0</v>
       </c>
       <c r="L20" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4E-2</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="13">
+        <v>2.4E-2</v>
+      </c>
+      <c r="N20">
         <f>LOG10(6773)</f>
         <v>3.8307810756063612</v>
       </c>
-      <c r="N20" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O20" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="1"/>
+        <v>0.67730000000000024</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D21">
         <v>1605</v>
@@ -3244,7 +3397,7 @@
         <v>5.2661728770945029</v>
       </c>
       <c r="G21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H21" s="2">
         <v>0.41599999999999998</v>
@@ -3256,35 +3409,42 @@
         <v>0</v>
       </c>
       <c r="L21" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.115</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="13">
+        <v>0.115</v>
+      </c>
+      <c r="N21">
         <f>LOG10(26276)</f>
         <v>4.4195592531957208</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O21" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="1"/>
+        <v>2.6276000000000033</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D22">
         <v>1545</v>
@@ -3297,7 +3457,7 @@
         <v>5.4584414279787694</v>
       </c>
       <c r="G22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H22" s="2">
         <v>0.41599999999999998</v>
@@ -3309,35 +3469,42 @@
         <v>0</v>
       </c>
       <c r="L22" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.186</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="13">
+        <v>0.186</v>
+      </c>
+      <c r="N22">
         <f>LOG10(20720)</f>
         <v>4.3163897510731957</v>
       </c>
-      <c r="N22" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O22" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="1"/>
+        <v>2.0720000000000023</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <v>193</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D23">
         <v>1391</v>
@@ -3350,7 +3517,7 @@
         <v>4.9562404866349024</v>
       </c>
       <c r="G23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H23" s="2">
         <v>0.41599999999999998</v>
@@ -3362,35 +3529,42 @@
         <v>0</v>
       </c>
       <c r="L23" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="13">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="N23">
         <f>LOG10(16241)</f>
         <v>4.2106127663528978</v>
       </c>
-      <c r="N23" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O23" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="1"/>
+        <v>1.624100000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>162</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D24">
         <v>1077</v>
@@ -3403,7 +3577,7 @@
         <v>4.8955385634184374</v>
       </c>
       <c r="G24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H24" s="2">
         <v>0.41599999999999998</v>
@@ -3415,35 +3589,42 @@
         <v>0</v>
       </c>
       <c r="L24" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="13">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="N24">
         <f>LOG10(10072)</f>
         <v>4.0031157170998064</v>
       </c>
-      <c r="N24" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O24" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="1"/>
+        <v>1.0072000000000012</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B25" s="12">
         <v>213</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D25">
         <v>844</v>
@@ -3456,7 +3637,7 @@
         <v>4.7524172493264816</v>
       </c>
       <c r="G25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H25" s="2">
         <v>0.41599999999999998</v>
@@ -3468,35 +3649,42 @@
         <v>0</v>
       </c>
       <c r="L25" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="13">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="N25">
         <f>LOG10(7623)</f>
         <v>3.882125919770032</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O25" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="1"/>
+        <v>0.76230000000000087</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D26">
         <v>375</v>
@@ -3509,7 +3697,7 @@
         <v>3.9542425094393248</v>
       </c>
       <c r="G26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H26" s="2">
         <v>0.41599999999999998</v>
@@ -3521,50 +3709,81 @@
         <v>0</v>
       </c>
       <c r="L26" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4E-2</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="13">
+        <v>2.4E-2</v>
+      </c>
+      <c r="N26">
         <f>LOG10(5757)</f>
         <v>3.7601962294551341</v>
       </c>
-      <c r="N26" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O26" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="1"/>
+        <v>0.5757000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="O1:S1"/>
   </mergeCells>
-  <conditionalFormatting sqref="N3:N16 Q3:Q16">
-    <cfRule type="cellIs" dxfId="27" priority="37" operator="equal">
+  <conditionalFormatting sqref="O3:O16 R3:R16">
+    <cfRule type="cellIs" dxfId="27" priority="39" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="40" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="41" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D16">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:G16 G17:G26 F4:F26">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:J16 I18:J27">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -3576,8 +3795,75 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:G16 G17:G26 F4:F26">
+  <conditionalFormatting sqref="I3:I16 I18:I27">
     <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J16 J18:J27">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L16 N3:N26">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G26">
+    <cfRule type="cellIs" dxfId="24" priority="32" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R17:R26">
+    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="30" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="31" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17:O26">
+    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="28" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:J26">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:F26">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3588,40 +3874,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:J16 I18:J27">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I16 I18:I27">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J16 J18:J27">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L3:M16 M10:M26">
-    <cfRule type="colorScale" priority="31">
+  <conditionalFormatting sqref="L3:L26 N3:N26">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3630,44 +3884,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G26">
-    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q17:Q26">
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="28" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="29" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N17:N26">
-    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="25" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="26" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:J26">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:F26">
+  <conditionalFormatting sqref="F3:F26">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -3679,8 +3896,52 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:M26">
-    <cfRule type="colorScale" priority="21">
+  <conditionalFormatting sqref="S3:S16">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S17:S26">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3:Q16">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q17:Q26">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N26">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3689,64 +3950,30 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F26">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R3:R16">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+  <conditionalFormatting sqref="P3:P16">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R17:R26">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P16">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17:P26">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M26">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="M3:M16">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3755,26 +3982,14 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O16">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O17:O26">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>"X"</formula>
+  <conditionalFormatting sqref="M3:M26">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3786,11 +4001,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:F17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3801,45 +4016,45 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" t="s">
         <v>59</v>
-      </c>
-      <c r="F1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C2" s="18">
         <v>1.6037999999999999</v>
@@ -4176,10 +4391,10 @@
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>44</v>
       </c>
       <c r="C17">
         <v>0.51344000000000001</v>
@@ -4205,7 +4420,7 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C18">
         <v>0.51344000000000001</v>
@@ -4231,7 +4446,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C19">
         <v>0.51344000000000001</v>
@@ -4257,7 +4472,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C20">
         <v>0.51344000000000001</v>
@@ -4283,7 +4498,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C21">
         <v>0.51344000000000001</v>
@@ -4309,7 +4524,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C22">
         <v>0.51344000000000001</v>
@@ -4413,7 +4628,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C26">
         <v>0.51344000000000001</v>
@@ -4443,7 +4658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4458,19 +4673,19 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -4950,11 +5165,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4972,13 +5187,13 @@
         <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4994,7 +5209,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -5005,7 +5220,7 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -5016,7 +5231,7 @@
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -5035,10 +5250,10 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G7" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -5049,13 +5264,13 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F8" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G8" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -5084,17 +5299,17 @@
       <c r="C11" s="6">
         <v>17</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>73</v>
+      <c r="D11" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="E11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" t="s">
         <v>77</v>
       </c>
-      <c r="F11" t="s">
-        <v>86</v>
-      </c>
       <c r="G11" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -5105,16 +5320,16 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G12" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -5125,16 +5340,16 @@
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G13" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5148,16 +5363,16 @@
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G14" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -5168,16 +5383,16 @@
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -5188,67 +5403,67 @@
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G16" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>44</v>
-      </c>
       <c r="C17" s="19" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -5256,7 +5471,7 @@
         <v>193</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -5264,7 +5479,7 @@
         <v>162</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -5272,20 +5487,20 @@
         <v>213</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="D11" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
A bunch of changes: - Updated scripts in the critical path to be 'early bindings' - Updated chooseLinPoint to include minimum voltage bounds in calculations and also including tap change hysteresis - Included an additional loading point in hosting capacity calculations (although at this stage it doesn't actually seem to make any difference to calculations...)
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3CF792-A567-4DA0-AD80-FEBE0CEFDE56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C6F155-DEDE-448C-B338-D4685113E678}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="90">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -276,9 +276,6 @@
     <t>Predicted</t>
   </si>
   <si>
-    <t>V2 (6000 LFs)</t>
-  </si>
-  <si>
     <t>Log(t2s) (us)</t>
   </si>
   <si>
@@ -295,6 +292,12 @@
   </si>
   <si>
     <t>Zsrc</t>
+  </si>
+  <si>
+    <t>V2 (9000 LFs)</t>
+  </si>
+  <si>
+    <t>6000 LFs</t>
   </si>
 </sst>
 </file>
@@ -2103,10 +2106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V29"/>
+  <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,7 +2136,7 @@
     <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -2174,7 +2177,7 @@
         <v>80</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O1" s="23" t="s">
         <v>26</v>
@@ -2184,7 +2187,7 @@
       <c r="R1" s="23"/>
       <c r="S1" s="23"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2200,29 +2203,32 @@
       <c r="M2" s="16"/>
       <c r="N2" s="14"/>
       <c r="O2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="T2" s="4"/>
       <c r="U2" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W2" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -2280,7 +2286,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -2338,15 +2344,19 @@
         <v>27</v>
       </c>
       <c r="U4">
-        <f>9/60</f>
-        <v>0.15</v>
+        <f>18/60</f>
+        <v>0.3</v>
       </c>
       <c r="V4">
-        <f>(10^N4)*6000*0.000001/60</f>
-        <v>7.0300000000000015E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+        <f>(10^N4)*9000*0.000001/60</f>
+        <v>0.10545000000000002</v>
+      </c>
+      <c r="W4">
+        <f>18/60</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -2403,16 +2413,16 @@
       <c r="S5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U5">
+      <c r="V5">
+        <f t="shared" ref="V5:V26" si="1">(10^N5)*9000*0.000001/60</f>
+        <v>0.60000000000000098</v>
+      </c>
+      <c r="W5">
         <f>19/60</f>
         <v>0.31666666666666665</v>
       </c>
-      <c r="V5">
-        <f t="shared" ref="V5:V26" si="1">(10^N5)*6000*0.000001/60</f>
-        <v>0.40000000000000063</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -2471,10 +2481,10 @@
       </c>
       <c r="V6">
         <f t="shared" si="1"/>
-        <v>0.29070000000000012</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.43605000000000016</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -2531,16 +2541,16 @@
       <c r="S7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U7">
+      <c r="V7">
+        <f t="shared" si="1"/>
+        <v>0.74475000000000013</v>
+      </c>
+      <c r="W7">
         <f>33/60</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="V7">
-        <f t="shared" si="1"/>
-        <v>0.49650000000000016</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -2597,16 +2607,16 @@
       <c r="S8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U8">
+      <c r="V8">
+        <f t="shared" si="1"/>
+        <v>41.364450000000069</v>
+      </c>
+      <c r="W8">
         <f>958/60</f>
         <v>15.966666666666667</v>
       </c>
-      <c r="V8">
-        <f t="shared" si="1"/>
-        <v>27.576300000000046</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -2663,16 +2673,16 @@
       <c r="S9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U9">
+      <c r="V9">
+        <f t="shared" si="1"/>
+        <v>0.77160000000000128</v>
+      </c>
+      <c r="W9">
         <f>59/60</f>
         <v>0.98333333333333328</v>
       </c>
-      <c r="V9">
-        <f t="shared" si="1"/>
-        <v>0.51440000000000086</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>25</v>
       </c>
@@ -2726,16 +2736,16 @@
       <c r="S10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U10">
+      <c r="V10">
+        <f t="shared" si="1"/>
+        <v>1.8091500000000034</v>
+      </c>
+      <c r="W10">
         <f>145/60</f>
         <v>2.4166666666666665</v>
       </c>
-      <c r="V10">
-        <f t="shared" si="1"/>
-        <v>1.2061000000000024</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -2795,16 +2805,16 @@
       <c r="S11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="U11">
+      <c r="V11">
+        <f t="shared" si="1"/>
+        <v>4.8481500000000013</v>
+      </c>
+      <c r="W11">
         <f>371/60</f>
         <v>6.1833333333333336</v>
       </c>
-      <c r="V11">
-        <f t="shared" si="1"/>
-        <v>3.2321000000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -2864,16 +2874,16 @@
       <c r="T12" t="s">
         <v>79</v>
       </c>
-      <c r="U12">
+      <c r="V12">
+        <f t="shared" si="1"/>
+        <v>2.6175000000000002</v>
+      </c>
+      <c r="W12">
         <f>367/60</f>
         <v>6.1166666666666663</v>
       </c>
-      <c r="V12">
-        <f t="shared" si="1"/>
-        <v>1.7450000000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -2930,16 +2940,16 @@
       <c r="S13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U13">
+      <c r="V13">
+        <f t="shared" si="1"/>
+        <v>13.193250000000001</v>
+      </c>
+      <c r="W13">
         <f>1996/60</f>
         <v>33.266666666666666</v>
       </c>
-      <c r="V13">
-        <f t="shared" si="1"/>
-        <v>8.7955000000000005</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -3000,16 +3010,16 @@
       <c r="T14" t="s">
         <v>63</v>
       </c>
-      <c r="U14">
+      <c r="V14">
+        <f t="shared" si="1"/>
+        <v>3.9418500000000019</v>
+      </c>
+      <c r="W14">
         <f>551/60</f>
         <v>9.1833333333333336</v>
       </c>
-      <c r="V14">
-        <f t="shared" si="1"/>
-        <v>2.6279000000000017</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -3063,16 +3073,16 @@
       <c r="S15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U15">
+      <c r="V15">
+        <f t="shared" si="1"/>
+        <v>3.0229500000000038</v>
+      </c>
+      <c r="W15">
         <f>107/60</f>
         <v>1.7833333333333334</v>
       </c>
-      <c r="V15">
-        <f t="shared" si="1"/>
-        <v>2.0153000000000025</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>24</v>
       </c>
@@ -3126,13 +3136,13 @@
       <c r="S16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U16">
+      <c r="V16">
+        <f t="shared" si="1"/>
+        <v>4.1532000000000036</v>
+      </c>
+      <c r="W16">
         <f>445/60</f>
         <v>7.416666666666667</v>
-      </c>
-      <c r="V16">
-        <f t="shared" si="1"/>
-        <v>2.7688000000000015</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3196,7 +3206,7 @@
       </c>
       <c r="V17">
         <f t="shared" si="1"/>
-        <v>1.0388000000000011</v>
+        <v>1.5582000000000018</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3256,7 +3266,7 @@
       </c>
       <c r="V18">
         <f t="shared" si="1"/>
-        <v>2.4732000000000034</v>
+        <v>3.7098000000000053</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
@@ -3316,7 +3326,7 @@
       </c>
       <c r="V19">
         <f t="shared" si="1"/>
-        <v>2.4431000000000025</v>
+        <v>3.6646500000000035</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
@@ -3376,7 +3386,7 @@
       </c>
       <c r="V20">
         <f t="shared" si="1"/>
-        <v>0.67730000000000024</v>
+        <v>1.0159500000000004</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
@@ -3436,7 +3446,7 @@
       </c>
       <c r="V21">
         <f t="shared" si="1"/>
-        <v>2.6276000000000033</v>
+        <v>3.9414000000000047</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
@@ -3496,7 +3506,7 @@
       </c>
       <c r="V22">
         <f t="shared" si="1"/>
-        <v>2.0720000000000023</v>
+        <v>3.1080000000000032</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
@@ -3556,7 +3566,7 @@
       </c>
       <c r="V23">
         <f t="shared" si="1"/>
-        <v>1.624100000000001</v>
+        <v>2.4361500000000018</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
@@ -3616,7 +3626,7 @@
       </c>
       <c r="V24">
         <f t="shared" si="1"/>
-        <v>1.0072000000000012</v>
+        <v>1.5108000000000019</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -3676,7 +3686,7 @@
       </c>
       <c r="V25">
         <f t="shared" si="1"/>
-        <v>0.76230000000000087</v>
+        <v>1.1434500000000012</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -3736,7 +3746,7 @@
       </c>
       <c r="V26">
         <f t="shared" si="1"/>
-        <v>0.5757000000000001</v>
+        <v>0.86355000000000015</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added some small stuff to save load names and buses for the losses phase work
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C6F155-DEDE-448C-B338-D4685113E678}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C39C443-82B2-411E-BDAC-330DEF0990C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2108,8 +2108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Halfway through new set of HC calculations.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C39C443-82B2-411E-BDAC-330DEF0990C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B563F3CB-40F1-47DA-AAF9-C4AB299E4B83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="92">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -298,6 +298,12 @@
   </si>
   <si>
     <t>6000 LFs</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Done - nominal undervoltage?</t>
   </si>
 </sst>
 </file>
@@ -2108,8 +2114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2413,6 +2419,10 @@
       <c r="S5" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="U5">
+        <f>53.7/60</f>
+        <v>0.89500000000000002</v>
+      </c>
       <c r="V5">
         <f t="shared" ref="V5:V26" si="1">(10^N5)*9000*0.000001/60</f>
         <v>0.60000000000000098</v>
@@ -2541,6 +2551,10 @@
       <c r="S7" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="U7">
+        <f>72/60</f>
+        <v>1.2</v>
+      </c>
       <c r="V7">
         <f t="shared" si="1"/>
         <v>0.74475000000000013</v>
@@ -2805,6 +2819,10 @@
       <c r="S11" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="U11">
+        <f>637/60</f>
+        <v>10.616666666666667</v>
+      </c>
       <c r="V11">
         <f t="shared" si="1"/>
         <v>4.8481500000000013</v>
@@ -2874,6 +2892,9 @@
       <c r="T12" t="s">
         <v>79</v>
       </c>
+      <c r="U12" t="s">
+        <v>91</v>
+      </c>
       <c r="V12">
         <f t="shared" si="1"/>
         <v>2.6175000000000002</v>
@@ -2939,6 +2960,9 @@
       </c>
       <c r="S13" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="U13" t="s">
+        <v>90</v>
       </c>
       <c r="V13">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
A bunch of changes: 1. full set of HC analyses run for all networks, showing good performance 2. linSvdCalcs scripts, with a start of circuit plotting 3. Most circuits can not be plotted (at least on the primary circuit).
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B563F3CB-40F1-47DA-AAF9-C4AB299E4B83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -13,7 +12,7 @@
     <sheet name="plotTts" sheetId="2" r:id="rId3"/>
     <sheet name="notes" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="93">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -304,12 +303,15 @@
   </si>
   <si>
     <t>Done - nominal undervoltage?</t>
+  </si>
+  <si>
+    <t>PLT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -465,7 +467,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -514,6 +516,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -523,7 +528,67 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="3" builtinId="25"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -2111,11 +2176,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2138,11 +2203,12 @@
     <col min="17" max="17" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.42578125" customWidth="1"/>
+    <col min="21" max="21" width="23" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -2185,15 +2251,16 @@
       <c r="N1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="23"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2223,18 +2290,21 @@
       <c r="S2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4" t="s">
+      <c r="T2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -2291,8 +2361,11 @@
       <c r="S3" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="T3" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -2349,20 +2422,23 @@
       <c r="S4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U4">
+      <c r="T4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V4">
         <f>18/60</f>
         <v>0.3</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <f>(10^N4)*9000*0.000001/60</f>
         <v>0.10545000000000002</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <f>18/60</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -2419,20 +2495,23 @@
       <c r="S5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U5">
+      <c r="T5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V5">
         <f>53.7/60</f>
         <v>0.89500000000000002</v>
       </c>
-      <c r="V5">
-        <f t="shared" ref="V5:V26" si="1">(10^N5)*9000*0.000001/60</f>
+      <c r="W5">
+        <f t="shared" ref="W5:W26" si="1">(10^N5)*9000*0.000001/60</f>
         <v>0.60000000000000098</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <f>19/60</f>
         <v>0.31666666666666665</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -2489,12 +2568,15 @@
       <c r="S6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="V6">
+      <c r="T6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W6">
         <f t="shared" si="1"/>
         <v>0.43605000000000016</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -2551,20 +2633,23 @@
       <c r="S7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U7">
+      <c r="T7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V7">
         <f>72/60</f>
         <v>1.2</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <f t="shared" si="1"/>
         <v>0.74475000000000013</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <f>33/60</f>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -2621,16 +2706,19 @@
       <c r="S8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V8">
+      <c r="T8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W8">
         <f t="shared" si="1"/>
         <v>41.364450000000069</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <f>958/60</f>
         <v>15.966666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -2687,16 +2775,19 @@
       <c r="S9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V9">
+      <c r="T9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W9">
         <f t="shared" si="1"/>
         <v>0.77160000000000128</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <f>59/60</f>
         <v>0.98333333333333328</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>25</v>
       </c>
@@ -2750,16 +2841,19 @@
       <c r="S10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V10">
+      <c r="T10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W10">
         <f t="shared" si="1"/>
         <v>1.8091500000000034</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <f>145/60</f>
         <v>2.4166666666666665</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -2819,20 +2913,23 @@
       <c r="S11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="U11">
+      <c r="T11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="V11">
         <f>637/60</f>
         <v>10.616666666666667</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <f t="shared" si="1"/>
         <v>4.8481500000000013</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <f>371/60</f>
         <v>6.1833333333333336</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -2889,22 +2986,25 @@
       <c r="S12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U12" t="s">
         <v>79</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>91</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <f t="shared" si="1"/>
         <v>2.6175000000000002</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <f>367/60</f>
         <v>6.1166666666666663</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -2961,19 +3061,22 @@
       <c r="S13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U13" t="s">
+      <c r="T13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V13" t="s">
         <v>90</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <f t="shared" si="1"/>
         <v>13.193250000000001</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <f>1996/60</f>
         <v>33.266666666666666</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -3031,19 +3134,22 @@
       <c r="S14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="T14" t="s">
+      <c r="T14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="U14" t="s">
         <v>63</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <f t="shared" si="1"/>
         <v>3.9418500000000019</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <f>551/60</f>
         <v>9.1833333333333336</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -3097,16 +3203,19 @@
       <c r="S15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V15">
+      <c r="T15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W15">
         <f t="shared" si="1"/>
         <v>3.0229500000000038</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <f>107/60</f>
         <v>1.7833333333333334</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>24</v>
       </c>
@@ -3160,16 +3269,19 @@
       <c r="S16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V16">
+      <c r="T16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W16">
         <f t="shared" si="1"/>
         <v>4.1532000000000036</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <f>445/60</f>
         <v>7.416666666666667</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>34</v>
       </c>
@@ -3228,12 +3340,13 @@
       <c r="S17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="V17">
+      <c r="T17" s="8"/>
+      <c r="W17">
         <f t="shared" si="1"/>
         <v>1.5582000000000018</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>40</v>
       </c>
@@ -3288,12 +3401,13 @@
       <c r="S18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V18">
+      <c r="T18" s="1"/>
+      <c r="W18">
         <f t="shared" si="1"/>
         <v>3.7098000000000053</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>41</v>
       </c>
@@ -3348,12 +3462,13 @@
       <c r="S19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V19">
+      <c r="T19" s="1"/>
+      <c r="W19">
         <f t="shared" si="1"/>
         <v>3.6646500000000035</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>37</v>
       </c>
@@ -3408,12 +3523,13 @@
       <c r="S20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V20">
+      <c r="T20" s="1"/>
+      <c r="W20">
         <f t="shared" si="1"/>
         <v>1.0159500000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>35</v>
       </c>
@@ -3468,12 +3584,13 @@
       <c r="S21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V21">
+      <c r="T21" s="1"/>
+      <c r="W21">
         <f t="shared" si="1"/>
         <v>3.9414000000000047</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>36</v>
       </c>
@@ -3528,12 +3645,13 @@
       <c r="S22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V22">
+      <c r="T22" s="1"/>
+      <c r="W22">
         <f t="shared" si="1"/>
         <v>3.1080000000000032</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <v>193</v>
       </c>
@@ -3588,12 +3706,13 @@
       <c r="S23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V23">
+      <c r="T23" s="1"/>
+      <c r="W23">
         <f t="shared" si="1"/>
         <v>2.4361500000000018</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>162</v>
       </c>
@@ -3648,12 +3767,13 @@
       <c r="S24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V24">
+      <c r="T24" s="1"/>
+      <c r="W24">
         <f t="shared" si="1"/>
         <v>1.5108000000000019</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B25" s="12">
         <v>213</v>
       </c>
@@ -3708,12 +3828,13 @@
       <c r="S25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V25">
+      <c r="T25" s="1"/>
+      <c r="W25">
         <f t="shared" si="1"/>
         <v>1.1434500000000012</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>37</v>
       </c>
@@ -3768,12 +3889,13 @@
       <c r="S26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V26">
+      <c r="T26" s="1"/>
+      <c r="W26">
         <f t="shared" si="1"/>
         <v>0.86355000000000015</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -3783,18 +3905,18 @@
     <mergeCell ref="O1:S1"/>
   </mergeCells>
   <conditionalFormatting sqref="O3:O16 R3:R16">
-    <cfRule type="cellIs" dxfId="27" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="45" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="46" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="47" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D16">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3806,7 +3928,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:G16 G17:G26 F4:F26">
-    <cfRule type="colorScale" priority="37">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3818,7 +3940,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:J16 I18:J27">
-    <cfRule type="colorScale" priority="36">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3830,7 +3952,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I16 I18:I27">
-    <cfRule type="colorScale" priority="35">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3840,7 +3962,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J16 J18:J27">
-    <cfRule type="colorScale" priority="34">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3850,7 +3972,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L16 N3:N26">
-    <cfRule type="colorScale" priority="33">
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3860,34 +3982,34 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G26">
-    <cfRule type="cellIs" dxfId="24" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="38" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17:R26">
-    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="36" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="37" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17:O26">
-    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="32" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="33" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="34" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:J26">
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3897,7 +4019,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:F26">
-    <cfRule type="colorScale" priority="24">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3909,7 +4031,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L26 N3:N26">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3919,7 +4041,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F26">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3931,6 +4053,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:S16">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="27" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S17:S26">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3:Q16">
     <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3941,7 +4085,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S17:S26">
+  <conditionalFormatting sqref="Q17:Q26">
     <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3952,30 +4096,8 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q16">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q17:Q26">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="N3:N26">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3985,29 +4107,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P16">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17:P26">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M16">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4017,13 +4139,35 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M26">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T3:T16">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T17:T26">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4035,7 +4179,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4692,7 +4836,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5199,7 +5343,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5534,7 +5678,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Main change: - fixed and validated really annoying bug that was giving us the wrong voltage buses, and validated that this is now working.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="94">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -89,9 +89,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Length (km)</t>
-  </si>
-  <si>
     <t>EPRI HC</t>
   </si>
   <si>
@@ -306,6 +303,12 @@
   </si>
   <si>
     <t>PLT</t>
+  </si>
+  <si>
+    <t>Len (km)</t>
+  </si>
+  <si>
+    <t>Manc LV</t>
   </si>
 </sst>
 </file>
@@ -2180,21 +2183,21 @@
   <dimension ref="A1:X29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" customWidth="1"/>
     <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
@@ -2216,7 +2219,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -2225,13 +2228,13 @@
         <v>13</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>2</v>
@@ -2240,19 +2243,19 @@
         <v>3</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>18</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O1" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" s="24"/>
       <c r="Q1" s="24"/>
@@ -2276,32 +2279,32 @@
       <c r="M2" s="16"/>
       <c r="N2" s="14"/>
       <c r="O2" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="S2" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="T2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="U2" s="4"/>
       <c r="V2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X2" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2312,7 +2315,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="6">
         <v>4</v>
@@ -2325,7 +2328,7 @@
         <v>0.6020599913279624</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="6">
@@ -2344,25 +2347,25 @@
         <v>5.4</v>
       </c>
       <c r="N3" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="P3" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2383,7 +2386,7 @@
         <v>2.3802112417116059</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" s="2">
         <v>4.16</v>
@@ -2408,22 +2411,22 @@
         <v>2.8469553250198238</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V4">
         <f>18/60</f>
@@ -2456,7 +2459,7 @@
         <v>3.4007106367732312</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="2">
         <v>24.9</v>
@@ -2481,22 +2484,22 @@
         <v>3.6020599913279625</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V5">
         <f>53.7/60</f>
@@ -2529,7 +2532,7 @@
         <v>3.0681858617461617</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="2">
         <v>4.8</v>
@@ -2554,22 +2557,22 @@
         <v>3.4634450317704277</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q6" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="R6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W6">
         <f t="shared" si="1"/>
@@ -2594,7 +2597,7 @@
         <v>4.0843617585514052</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H7" s="2">
         <v>2.4</v>
@@ -2619,22 +2622,22 @@
         <v>3.6959192528313998</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V7">
         <f>72/60</f>
@@ -2667,7 +2670,7 @@
         <v>7.0600546084112592</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="2">
         <v>7.2</v>
@@ -2692,22 +2695,22 @@
         <v>5.4405359950748213</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="S8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W8">
         <f t="shared" si="1"/>
@@ -2736,7 +2739,7 @@
         <v>4.6979699765543392</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H9" s="2">
         <v>0.41599999999999998</v>
@@ -2761,22 +2764,22 @@
         <v>3.7113009599161657</v>
       </c>
       <c r="O9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="S9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W9">
         <f t="shared" si="1"/>
@@ -2789,7 +2792,7 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>14</v>
@@ -2805,7 +2808,7 @@
         <v>5.4324240774813539</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H10" s="2">
         <v>13.8</v>
@@ -2827,22 +2830,22 @@
         <v>4.0813833174622856</v>
       </c>
       <c r="O10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="S10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="W10">
         <f t="shared" si="1"/>
@@ -2874,7 +2877,7 @@
         <v>6.6163958946881101</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H11" s="7">
         <v>12.47</v>
@@ -2899,22 +2902,22 @@
         <v>4.50948478922394</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Q11" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="R11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S11" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T11" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V11">
         <f>637/60</f>
@@ -2947,7 +2950,7 @@
         <v>6.0371634509935488</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12" s="2">
         <v>12.47</v>
@@ -2972,28 +2975,28 @@
         <v>4.2417954312951984</v>
       </c>
       <c r="O12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="S12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="V12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="W12">
         <f t="shared" si="1"/>
@@ -3022,7 +3025,7 @@
         <v>7.3723904998005798</v>
       </c>
       <c r="G13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H13" s="2">
         <v>34.5</v>
@@ -3047,25 +3050,25 @@
         <v>4.9442605329428515</v>
       </c>
       <c r="O13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="S13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="W13">
         <f t="shared" si="1"/>
@@ -3078,10 +3081,10 @@
     </row>
     <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="C14" s="6">
         <v>19</v>
@@ -3097,7 +3100,7 @@
         <v>6.8302672873552366</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H14" s="7">
         <v>12.47</v>
@@ -3120,25 +3123,25 @@
         <v>4.4196088349081029</v>
       </c>
       <c r="O14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="R14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R14" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="S14" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T14" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W14">
         <f t="shared" si="1"/>
@@ -3151,7 +3154,7 @@
     </row>
     <row r="15" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -3167,7 +3170,7 @@
         <v>5.6290261088868352</v>
       </c>
       <c r="G15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H15" s="2">
         <v>13.2</v>
@@ -3189,22 +3192,22 @@
         <v>4.3043397048923389</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W15">
         <f t="shared" si="1"/>
@@ -3217,7 +3220,7 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16">
         <v>21</v>
@@ -3233,7 +3236,7 @@
         <v>6.5816220228765081</v>
       </c>
       <c r="G16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H16" s="2">
         <v>12.47</v>
@@ -3255,22 +3258,22 @@
         <v>4.4422915862860712</v>
       </c>
       <c r="O16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="S16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W16">
         <f t="shared" si="1"/>
@@ -3283,13 +3286,13 @@
     </row>
     <row r="17" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="6">
         <v>907</v>
@@ -3302,7 +3305,7 @@
         <v>4.6979699765543392</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H17" s="7">
         <v>0.41599999999999998</v>
@@ -3326,19 +3329,19 @@
         <v>4.0165319409572655</v>
       </c>
       <c r="O17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P17" s="8" t="s">
+      <c r="R17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Q17" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="R17" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="S17" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T17" s="8"/>
       <c r="W17">
@@ -3348,10 +3351,10 @@
     </row>
     <row r="18" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D18">
         <v>2287</v>
@@ -3364,7 +3367,7 @@
         <v>5.602304213293043</v>
       </c>
       <c r="G18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H18" s="2">
         <v>0.41599999999999998</v>
@@ -3387,19 +3390,19 @@
         <v>4.3932592378268378</v>
       </c>
       <c r="O18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="R18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="S18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T18" s="1"/>
       <c r="W18">
@@ -3409,10 +3412,10 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19">
         <v>1304</v>
@@ -3425,7 +3428,7 @@
         <v>5.0884054449956002</v>
       </c>
       <c r="G19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H19" s="2">
         <v>0.41599999999999998</v>
@@ -3448,19 +3451,19 @@
         <v>4.3879412437066989</v>
       </c>
       <c r="O19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="R19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="S19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T19" s="1"/>
       <c r="W19">
@@ -3470,10 +3473,10 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20">
         <v>375</v>
@@ -3486,7 +3489,7 @@
         <v>3.9542425094393248</v>
       </c>
       <c r="G20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H20" s="2">
         <v>0.41599999999999998</v>
@@ -3509,19 +3512,19 @@
         <v>3.8307810756063612</v>
       </c>
       <c r="O20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="R20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="S20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T20" s="1"/>
       <c r="W20">
@@ -3531,10 +3534,10 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D21">
         <v>1605</v>
@@ -3547,7 +3550,7 @@
         <v>5.2661728770945029</v>
       </c>
       <c r="G21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H21" s="2">
         <v>0.41599999999999998</v>
@@ -3570,19 +3573,19 @@
         <v>4.4195592531957208</v>
       </c>
       <c r="O21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="R21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="S21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T21" s="1"/>
       <c r="W21">
@@ -3592,10 +3595,10 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22">
         <v>1545</v>
@@ -3608,7 +3611,7 @@
         <v>5.4584414279787694</v>
       </c>
       <c r="G22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H22" s="2">
         <v>0.41599999999999998</v>
@@ -3631,19 +3634,19 @@
         <v>4.3163897510731957</v>
       </c>
       <c r="O22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="R22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="S22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T22" s="1"/>
       <c r="W22">
@@ -3656,7 +3659,7 @@
         <v>193</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D23">
         <v>1391</v>
@@ -3669,7 +3672,7 @@
         <v>4.9562404866349024</v>
       </c>
       <c r="G23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H23" s="2">
         <v>0.41599999999999998</v>
@@ -3692,19 +3695,19 @@
         <v>4.2106127663528978</v>
       </c>
       <c r="O23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P23" s="1" t="s">
+      <c r="R23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="S23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T23" s="1"/>
       <c r="W23">
@@ -3717,7 +3720,7 @@
         <v>162</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D24">
         <v>1077</v>
@@ -3730,7 +3733,7 @@
         <v>4.8955385634184374</v>
       </c>
       <c r="G24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H24" s="2">
         <v>0.41599999999999998</v>
@@ -3753,19 +3756,19 @@
         <v>4.0031157170998064</v>
       </c>
       <c r="O24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P24" s="1" t="s">
+      <c r="R24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="S24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T24" s="1"/>
       <c r="W24">
@@ -3778,7 +3781,7 @@
         <v>213</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25">
         <v>844</v>
@@ -3791,7 +3794,7 @@
         <v>4.7524172493264816</v>
       </c>
       <c r="G25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H25" s="2">
         <v>0.41599999999999998</v>
@@ -3814,19 +3817,19 @@
         <v>3.882125919770032</v>
       </c>
       <c r="O25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="R25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="S25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T25" s="1"/>
       <c r="W25">
@@ -3836,10 +3839,10 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D26">
         <v>375</v>
@@ -3852,7 +3855,7 @@
         <v>3.9542425094393248</v>
       </c>
       <c r="G26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H26" s="2">
         <v>0.41599999999999998</v>
@@ -3875,19 +3878,19 @@
         <v>3.7601962294551341</v>
       </c>
       <c r="O26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P26" s="1" t="s">
+      <c r="R26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="S26" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T26" s="1"/>
       <c r="W26">
@@ -3897,7 +3900,7 @@
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -4194,45 +4197,45 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>55</v>
       </c>
-      <c r="J1" t="s">
-        <v>56</v>
-      </c>
       <c r="K1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" t="s">
         <v>60</v>
       </c>
-      <c r="L1" t="s">
-        <v>61</v>
-      </c>
       <c r="M1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="18">
         <v>1.6037999999999999</v>
@@ -4420,7 +4423,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>6.4151E-2</v>
@@ -4506,10 +4509,10 @@
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="C14" s="18">
         <v>1.3759999999999999</v>
@@ -4529,7 +4532,7 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="18">
         <v>0.80626299999999995</v>
@@ -4549,7 +4552,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="18">
         <v>5.1799999999999999E-2</v>
@@ -4569,10 +4572,10 @@
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17">
         <v>0.51344000000000001</v>
@@ -4598,7 +4601,7 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18">
         <v>0.51344000000000001</v>
@@ -4624,7 +4627,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19">
         <v>0.51344000000000001</v>
@@ -4650,7 +4653,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20">
         <v>0.51344000000000001</v>
@@ -4676,7 +4679,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21">
         <v>0.51344000000000001</v>
@@ -4702,7 +4705,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22">
         <v>0.51344000000000001</v>
@@ -4806,7 +4809,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26">
         <v>0.51344000000000001</v>
@@ -4851,19 +4854,19 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>45</v>
-      </c>
-      <c r="I1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -5060,7 +5063,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>390</v>
@@ -5188,7 +5191,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="6">
         <v>4888</v>
@@ -5220,7 +5223,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>1282</v>
@@ -5252,7 +5255,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>2596</v>
@@ -5365,13 +5368,13 @@
         <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -5387,7 +5390,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -5398,7 +5401,7 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -5409,7 +5412,7 @@
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -5428,10 +5431,10 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -5442,13 +5445,13 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -5461,7 +5464,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>14</v>
@@ -5478,16 +5481,16 @@
         <v>17</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -5498,16 +5501,16 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -5518,130 +5521,130 @@
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="C14" s="6">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16">
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -5649,7 +5652,7 @@
         <v>193</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -5657,7 +5660,7 @@
         <v>162</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -5665,15 +5668,15 @@
         <v>213</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continuing to work to try and reduce the computational complexity of the model. As part of this, have been looking at 'the pearson's correlation coefficient'. A robust method to test the model reduction methods is needed next really.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C346D2-61C5-4F0B-9435-A13BF505DEE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
     <sheet name="sourceParams" sheetId="3" r:id="rId2"/>
     <sheet name="plotTts" sheetId="2" r:id="rId3"/>
     <sheet name="notes" sheetId="4" r:id="rId4"/>
+    <sheet name="svdStuff" sheetId="5" r:id="rId5"/>
+    <sheet name="varStuff" sheetId="6" r:id="rId6"/>
+    <sheet name="varV2stuff" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="102">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -309,12 +313,36 @@
   </si>
   <si>
     <t>Manc LV</t>
+  </si>
+  <si>
+    <t>3500-&gt;0.9986</t>
+  </si>
+  <si>
+    <t>midNodes</t>
+  </si>
+  <si>
+    <t>500 sec</t>
+  </si>
+  <si>
+    <t>2500 sec</t>
+  </si>
+  <si>
+    <t>Fraction of time</t>
+  </si>
+  <si>
+    <t>99%, 99%</t>
+  </si>
+  <si>
+    <t>99%, 98%</t>
+  </si>
+  <si>
+    <t>99%, 95%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -470,7 +498,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -519,6 +547,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2179,11 +2210,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,7 +2223,6 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" customWidth="1"/>
     <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
@@ -2224,9 +2254,6 @@
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="F1" s="3" t="s">
         <v>41</v>
       </c>
@@ -2254,13 +2281,13 @@
       <c r="N1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
       <c r="T1" s="23"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -2268,7 +2295,6 @@
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
@@ -2320,11 +2346,8 @@
       <c r="D3" s="6">
         <v>4</v>
       </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
       <c r="F3" s="6">
-        <f>LOG(E3*D3)</f>
+        <f>LOG(svdStuff!E3*D3)</f>
         <v>0.6020599913279624</v>
       </c>
       <c r="G3" s="10" t="s">
@@ -2378,11 +2401,8 @@
       <c r="D4">
         <v>16</v>
       </c>
-      <c r="E4">
-        <v>15</v>
-      </c>
       <c r="F4" s="13">
-        <f t="shared" ref="F4:F26" si="0">LOG(E4*D4)</f>
+        <f>LOG(svdStuff!E4*D4)</f>
         <v>2.3802112417116059</v>
       </c>
       <c r="G4" t="s">
@@ -2451,11 +2471,8 @@
       <c r="D5">
         <v>37</v>
       </c>
-      <c r="E5">
-        <v>68</v>
-      </c>
       <c r="F5" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E5*D5)</f>
         <v>3.4007106367732312</v>
       </c>
       <c r="G5" t="s">
@@ -2506,7 +2523,7 @@
         <v>0.89500000000000002</v>
       </c>
       <c r="W5">
-        <f t="shared" ref="W5:W26" si="1">(10^N5)*9000*0.000001/60</f>
+        <f t="shared" ref="W5:W26" si="0">(10^N5)*9000*0.000001/60</f>
         <v>0.60000000000000098</v>
       </c>
       <c r="X5">
@@ -2524,11 +2541,8 @@
       <c r="D6">
         <v>39</v>
       </c>
-      <c r="E6">
-        <v>30</v>
-      </c>
       <c r="F6" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E6*D6)</f>
         <v>3.0681858617461617</v>
       </c>
       <c r="G6" s="9" t="s">
@@ -2575,7 +2589,7 @@
         <v>27</v>
       </c>
       <c r="W6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.43605000000000016</v>
       </c>
     </row>
@@ -2589,11 +2603,8 @@
       <c r="D7">
         <v>132</v>
       </c>
-      <c r="E7">
-        <v>92</v>
-      </c>
       <c r="F7" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E7*D7)</f>
         <v>4.0843617585514052</v>
       </c>
       <c r="G7" t="s">
@@ -2644,7 +2655,7 @@
         <v>1.2</v>
       </c>
       <c r="W7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.74475000000000013</v>
       </c>
       <c r="X7">
@@ -2662,11 +2673,8 @@
       <c r="D8">
         <v>4876</v>
       </c>
-      <c r="E8">
-        <v>2355</v>
-      </c>
       <c r="F8" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E8*D8)</f>
         <v>7.0600546084112592</v>
       </c>
       <c r="G8" t="s">
@@ -2713,7 +2721,7 @@
         <v>26</v>
       </c>
       <c r="W8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>41.364450000000069</v>
       </c>
       <c r="X8">
@@ -2731,11 +2739,8 @@
       <c r="D9">
         <v>907</v>
       </c>
-      <c r="E9">
-        <v>55</v>
-      </c>
       <c r="F9" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E9*D9)</f>
         <v>4.6979699765543392</v>
       </c>
       <c r="G9" t="s">
@@ -2782,7 +2787,7 @@
         <v>26</v>
       </c>
       <c r="W9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.77160000000000128</v>
       </c>
       <c r="X9">
@@ -2800,11 +2805,8 @@
       <c r="D10">
         <v>390</v>
       </c>
-      <c r="E10">
-        <v>694</v>
-      </c>
       <c r="F10" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E10*D10)</f>
         <v>5.4324240774813539</v>
       </c>
       <c r="G10" t="s">
@@ -2848,7 +2850,7 @@
         <v>27</v>
       </c>
       <c r="W10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.8091500000000034</v>
       </c>
       <c r="X10">
@@ -2869,11 +2871,8 @@
       <c r="D11" s="6">
         <v>2998</v>
       </c>
-      <c r="E11" s="6">
-        <v>1379</v>
-      </c>
       <c r="F11" s="6">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E11*D11)</f>
         <v>6.6163958946881101</v>
       </c>
       <c r="G11" s="6" t="s">
@@ -2924,7 +2923,7 @@
         <v>10.616666666666667</v>
       </c>
       <c r="W11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.8481500000000013</v>
       </c>
       <c r="X11">
@@ -2942,11 +2941,8 @@
       <c r="D12">
         <v>1255</v>
       </c>
-      <c r="E12">
-        <v>868</v>
-      </c>
       <c r="F12" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E12*D12)</f>
         <v>6.0371634509935488</v>
       </c>
       <c r="G12" t="s">
@@ -2999,7 +2995,7 @@
         <v>90</v>
       </c>
       <c r="W12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.6175000000000002</v>
       </c>
       <c r="X12">
@@ -3017,11 +3013,8 @@
       <c r="D13">
         <v>6058</v>
       </c>
-      <c r="E13">
-        <v>3891</v>
-      </c>
       <c r="F13" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E13*D13)</f>
         <v>7.3723904998005798</v>
       </c>
       <c r="G13" t="s">
@@ -3071,7 +3064,7 @@
         <v>89</v>
       </c>
       <c r="W13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13.193250000000001</v>
       </c>
       <c r="X13">
@@ -3092,11 +3085,8 @@
       <c r="D14" s="6">
         <v>4888</v>
       </c>
-      <c r="E14" s="6">
-        <v>1384</v>
-      </c>
       <c r="F14" s="6">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E14*D14)</f>
         <v>6.8302672873552366</v>
       </c>
       <c r="G14" s="6" t="s">
@@ -3144,7 +3134,7 @@
         <v>62</v>
       </c>
       <c r="W14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.9418500000000019</v>
       </c>
       <c r="X14">
@@ -3162,11 +3152,8 @@
       <c r="D15">
         <v>1282</v>
       </c>
-      <c r="E15">
-        <v>332</v>
-      </c>
       <c r="F15" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E15*D15)</f>
         <v>5.6290261088868352</v>
       </c>
       <c r="G15" t="s">
@@ -3210,7 +3197,7 @@
         <v>26</v>
       </c>
       <c r="W15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.0229500000000038</v>
       </c>
       <c r="X15">
@@ -3228,11 +3215,8 @@
       <c r="D16">
         <v>2596</v>
       </c>
-      <c r="E16">
-        <v>1470</v>
-      </c>
       <c r="F16" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E16*D16)</f>
         <v>6.5816220228765081</v>
       </c>
       <c r="G16" t="s">
@@ -3276,7 +3260,7 @@
         <v>26</v>
       </c>
       <c r="W16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.1532000000000036</v>
       </c>
       <c r="X16">
@@ -3297,11 +3281,8 @@
       <c r="D17" s="6">
         <v>907</v>
       </c>
-      <c r="E17" s="6">
-        <v>55</v>
-      </c>
       <c r="F17" s="6">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E17*D17)</f>
         <v>4.6979699765543392</v>
       </c>
       <c r="G17" s="6" t="s">
@@ -3318,7 +3299,7 @@
       </c>
       <c r="K17" s="6"/>
       <c r="L17" s="6">
-        <f>E17*0.001</f>
+        <f>svdStuff!E17*0.001</f>
         <v>5.5E-2</v>
       </c>
       <c r="M17" s="6">
@@ -3345,7 +3326,7 @@
       </c>
       <c r="T17" s="8"/>
       <c r="W17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.5582000000000018</v>
       </c>
     </row>
@@ -3359,11 +3340,8 @@
       <c r="D18">
         <v>2287</v>
       </c>
-      <c r="E18">
-        <v>175</v>
-      </c>
       <c r="F18" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E18*D18)</f>
         <v>5.602304213293043</v>
       </c>
       <c r="G18" t="s">
@@ -3379,7 +3357,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="13">
-        <f t="shared" ref="L18:L26" si="2">E18*0.001</f>
+        <f>svdStuff!E18*0.001</f>
         <v>0.17500000000000002</v>
       </c>
       <c r="M18" s="13">
@@ -3406,7 +3384,7 @@
       </c>
       <c r="T18" s="1"/>
       <c r="W18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.7098000000000053</v>
       </c>
     </row>
@@ -3420,11 +3398,8 @@
       <c r="D19">
         <v>1304</v>
       </c>
-      <c r="E19">
-        <v>94</v>
-      </c>
       <c r="F19" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E19*D19)</f>
         <v>5.0884054449956002</v>
       </c>
       <c r="G19" t="s">
@@ -3440,7 +3415,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="13">
-        <f t="shared" si="2"/>
+        <f>svdStuff!E19*0.001</f>
         <v>9.4E-2</v>
       </c>
       <c r="M19" s="13">
@@ -3467,7 +3442,7 @@
       </c>
       <c r="T19" s="1"/>
       <c r="W19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.6646500000000035</v>
       </c>
     </row>
@@ -3481,11 +3456,8 @@
       <c r="D20">
         <v>375</v>
       </c>
-      <c r="E20">
-        <v>24</v>
-      </c>
       <c r="F20" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E20*D20)</f>
         <v>3.9542425094393248</v>
       </c>
       <c r="G20" t="s">
@@ -3501,7 +3473,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="13">
-        <f t="shared" si="2"/>
+        <f>svdStuff!E20*0.001</f>
         <v>2.4E-2</v>
       </c>
       <c r="M20" s="13">
@@ -3528,7 +3500,7 @@
       </c>
       <c r="T20" s="1"/>
       <c r="W20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.0159500000000004</v>
       </c>
     </row>
@@ -3542,11 +3514,8 @@
       <c r="D21">
         <v>1605</v>
       </c>
-      <c r="E21">
-        <v>115</v>
-      </c>
       <c r="F21" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E21*D21)</f>
         <v>5.2661728770945029</v>
       </c>
       <c r="G21" t="s">
@@ -3562,7 +3531,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="13">
-        <f t="shared" si="2"/>
+        <f>svdStuff!E21*0.001</f>
         <v>0.115</v>
       </c>
       <c r="M21" s="13">
@@ -3589,7 +3558,7 @@
       </c>
       <c r="T21" s="1"/>
       <c r="W21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.9414000000000047</v>
       </c>
     </row>
@@ -3603,11 +3572,8 @@
       <c r="D22">
         <v>1545</v>
       </c>
-      <c r="E22">
-        <v>186</v>
-      </c>
       <c r="F22" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E22*D22)</f>
         <v>5.4584414279787694</v>
       </c>
       <c r="G22" t="s">
@@ -3623,7 +3589,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="13">
-        <f t="shared" si="2"/>
+        <f>svdStuff!E22*0.001</f>
         <v>0.186</v>
       </c>
       <c r="M22" s="13">
@@ -3650,7 +3616,7 @@
       </c>
       <c r="T22" s="1"/>
       <c r="W22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.1080000000000032</v>
       </c>
     </row>
@@ -3664,11 +3630,8 @@
       <c r="D23">
         <v>1391</v>
       </c>
-      <c r="E23">
-        <v>65</v>
-      </c>
       <c r="F23" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E23*D23)</f>
         <v>4.9562404866349024</v>
       </c>
       <c r="G23" t="s">
@@ -3684,7 +3647,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="13">
-        <f t="shared" si="2"/>
+        <f>svdStuff!E23*0.001</f>
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="M23" s="13">
@@ -3711,7 +3674,7 @@
       </c>
       <c r="T23" s="1"/>
       <c r="W23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.4361500000000018</v>
       </c>
     </row>
@@ -3725,11 +3688,8 @@
       <c r="D24">
         <v>1077</v>
       </c>
-      <c r="E24">
-        <v>73</v>
-      </c>
       <c r="F24" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E24*D24)</f>
         <v>4.8955385634184374</v>
       </c>
       <c r="G24" t="s">
@@ -3745,7 +3705,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="13">
-        <f t="shared" si="2"/>
+        <f>svdStuff!E24*0.001</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="M24" s="13">
@@ -3772,7 +3732,7 @@
       </c>
       <c r="T24" s="1"/>
       <c r="W24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.5108000000000019</v>
       </c>
     </row>
@@ -3786,11 +3746,8 @@
       <c r="D25">
         <v>844</v>
       </c>
-      <c r="E25">
-        <v>67</v>
-      </c>
       <c r="F25" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E25*D25)</f>
         <v>4.7524172493264816</v>
       </c>
       <c r="G25" t="s">
@@ -3806,7 +3763,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="13">
-        <f t="shared" si="2"/>
+        <f>svdStuff!E25*0.001</f>
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="M25" s="13">
@@ -3833,7 +3790,7 @@
       </c>
       <c r="T25" s="1"/>
       <c r="W25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.1434500000000012</v>
       </c>
     </row>
@@ -3847,11 +3804,8 @@
       <c r="D26">
         <v>375</v>
       </c>
-      <c r="E26">
-        <v>24</v>
-      </c>
       <c r="F26" s="13">
-        <f t="shared" si="0"/>
+        <f>LOG(svdStuff!E26*D26)</f>
         <v>3.9542425094393248</v>
       </c>
       <c r="G26" t="s">
@@ -3867,7 +3821,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="13">
-        <f t="shared" si="2"/>
+        <f>svdStuff!E26*0.001</f>
         <v>2.4E-2</v>
       </c>
       <c r="M26" s="13">
@@ -3894,7 +3848,7 @@
       </c>
       <c r="T26" s="1"/>
       <c r="W26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.86355000000000015</v>
       </c>
     </row>
@@ -3930,7 +3884,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:G16 G17:G26 F4:F26">
+  <conditionalFormatting sqref="F3:G16 G17:G26 F4:F26">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -4021,7 +3975,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:F26">
+  <conditionalFormatting sqref="D3:D26 F3:F26">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -4182,7 +4136,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4839,7 +4793,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5346,11 +5300,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5681,8 +5635,3137 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="D11" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11FE248-93EC-498A-B149-79239CF2A22B}">
+  <dimension ref="A1:V26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="3.85546875" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="R1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="26"/>
+      <c r="H2" s="24">
+        <v>0.95</v>
+      </c>
+      <c r="I2" s="24">
+        <v>0.98</v>
+      </c>
+      <c r="J2" s="24">
+        <v>0.99</v>
+      </c>
+      <c r="K2" s="25">
+        <v>0.995</v>
+      </c>
+      <c r="L2" s="24">
+        <v>0.99900000000000011</v>
+      </c>
+      <c r="M2" s="24">
+        <v>0.95</v>
+      </c>
+      <c r="N2" s="24">
+        <v>0.98</v>
+      </c>
+      <c r="O2" s="24">
+        <v>0.99</v>
+      </c>
+      <c r="P2" s="25">
+        <v>0.995</v>
+      </c>
+      <c r="Q2" s="24">
+        <v>0.99900000000000011</v>
+      </c>
+      <c r="R2" s="24">
+        <v>0.95</v>
+      </c>
+      <c r="S2" s="24">
+        <v>0.98</v>
+      </c>
+      <c r="T2" s="24">
+        <v>0.99</v>
+      </c>
+      <c r="U2" s="25">
+        <v>0.995</v>
+      </c>
+      <c r="V2" s="24">
+        <v>0.99900000000000011</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>31</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <f>H4/$E4</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:Q16" si="0">I4/$E4</f>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="R4">
+        <f>MIN((H4*($F4+$E4))/($E4*$F4),1)</f>
+        <v>0.19784946236559139</v>
+      </c>
+      <c r="S4">
+        <f t="shared" ref="S4:V4" si="1">MIN((I4*($F4+$E4))/($E4*$F4),1)</f>
+        <v>0.39569892473118279</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="1"/>
+        <v>0.59354838709677415</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="1"/>
+        <v>0.79139784946236558</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="1"/>
+        <v>0.989247311827957</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>37</v>
+      </c>
+      <c r="E5">
+        <v>68</v>
+      </c>
+      <c r="F5">
+        <v>74</v>
+      </c>
+      <c r="H5">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>13</v>
+      </c>
+      <c r="J5">
+        <v>13</v>
+      </c>
+      <c r="K5">
+        <v>13</v>
+      </c>
+      <c r="L5">
+        <v>15</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M16" si="2">H5/$E5</f>
+        <v>0.17647058823529413</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>0.19117647058823528</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>0.19117647058823528</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>0.19117647058823528</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>0.22058823529411764</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5:R16" si="3">MIN((H5*($F5+$E5))/($E5*$F5),1)</f>
+        <v>0.33863275039745627</v>
+      </c>
+      <c r="S5">
+        <f t="shared" ref="S5:S16" si="4">MIN((I5*($F5+$E5))/($E5*$F5),1)</f>
+        <v>0.36685214626391099</v>
+      </c>
+      <c r="T5">
+        <f t="shared" ref="T5:T16" si="5">MIN((J5*($F5+$E5))/($E5*$F5),1)</f>
+        <v>0.36685214626391099</v>
+      </c>
+      <c r="U5">
+        <f t="shared" ref="U5:U16" si="6">MIN((K5*($F5+$E5))/($E5*$F5),1)</f>
+        <v>0.36685214626391099</v>
+      </c>
+      <c r="V5">
+        <f t="shared" ref="V5:V16" si="7">MIN((L5*($F5+$E5))/($E5*$F5),1)</f>
+        <v>0.42329093799682033</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>39</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R6" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S6" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T6" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U6" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V6" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>132</v>
+      </c>
+      <c r="E7">
+        <v>92</v>
+      </c>
+      <c r="F7">
+        <v>119</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>15</v>
+      </c>
+      <c r="K7">
+        <v>21</v>
+      </c>
+      <c r="L7">
+        <v>35</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>5.434782608695652E-2</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>0.10869565217391304</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>0.16304347826086957</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>0.22826086956521738</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>0.38043478260869568</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="3"/>
+        <v>9.6364632809645592E-2</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="4"/>
+        <v>0.19272926561929118</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="5"/>
+        <v>0.28909389842893679</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="6"/>
+        <v>0.40473145780051151</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="7"/>
+        <v>0.67455242966751916</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>4876</v>
+      </c>
+      <c r="E8">
+        <v>2355</v>
+      </c>
+      <c r="F8">
+        <v>5900</v>
+      </c>
+      <c r="G8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8">
+        <v>1214</v>
+      </c>
+      <c r="I8">
+        <v>1504</v>
+      </c>
+      <c r="J8">
+        <v>1676</v>
+      </c>
+      <c r="K8">
+        <v>1811</v>
+      </c>
+      <c r="L8">
+        <v>2034</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>0.51549893842887473</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0.63864118895966027</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>0.71167728237791927</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>0.76900212314225058</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>0.8636942675159236</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="3"/>
+        <v>0.72126165029328149</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="4"/>
+        <v>0.89355644319694838</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="5"/>
+        <v>0.99574507898808884</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>907</v>
+      </c>
+      <c r="E9">
+        <v>55</v>
+      </c>
+      <c r="F9">
+        <v>61</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>6</v>
+      </c>
+      <c r="K9">
+        <v>9</v>
+      </c>
+      <c r="L9">
+        <v>21</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>5.4545454545454543E-2</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>7.2727272727272724E-2</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>0.10909090909090909</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>0.16363636363636364</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>0.38181818181818183</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="3"/>
+        <v>0.10372578241430701</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="4"/>
+        <v>0.13830104321907602</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="5"/>
+        <v>0.20745156482861402</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="6"/>
+        <v>0.31117734724292101</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="7"/>
+        <v>0.72608047690014899</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>390</v>
+      </c>
+      <c r="E10">
+        <v>694</v>
+      </c>
+      <c r="F10">
+        <v>729</v>
+      </c>
+      <c r="H10">
+        <v>102</v>
+      </c>
+      <c r="I10">
+        <v>146</v>
+      </c>
+      <c r="J10">
+        <v>176</v>
+      </c>
+      <c r="K10">
+        <v>204</v>
+      </c>
+      <c r="L10">
+        <v>272</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>0.14697406340057637</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>0.21037463976945245</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>0.25360230547550433</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>0.29394812680115273</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>0.39193083573487031</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="3"/>
+        <v>0.2868917588738274</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="4"/>
+        <v>0.410648988191949</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="5"/>
+        <v>0.49502891727248649</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="6"/>
+        <v>0.57378351774765479</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="7"/>
+        <v>0.76504469033020639</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6">
+        <v>17</v>
+      </c>
+      <c r="D11" s="6">
+        <v>2998</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1379</v>
+      </c>
+      <c r="F11" s="17">
+        <v>2567</v>
+      </c>
+      <c r="H11">
+        <v>588</v>
+      </c>
+      <c r="I11">
+        <v>872</v>
+      </c>
+      <c r="J11">
+        <v>1031</v>
+      </c>
+      <c r="K11">
+        <v>1147</v>
+      </c>
+      <c r="L11">
+        <v>1299</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>0.42639593908629442</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>0.63234227701232781</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>0.74764321972443804</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>0.83176214648295865</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>0.94198694706308916</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="3"/>
+        <v>0.65545709997449075</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="4"/>
+        <v>0.97203842037033328</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="17">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>1255</v>
+      </c>
+      <c r="E12">
+        <v>868</v>
+      </c>
+      <c r="F12" s="17">
+        <v>1975</v>
+      </c>
+      <c r="H12">
+        <v>103</v>
+      </c>
+      <c r="I12">
+        <v>172</v>
+      </c>
+      <c r="J12">
+        <v>259</v>
+      </c>
+      <c r="K12">
+        <v>385</v>
+      </c>
+      <c r="L12">
+        <v>779</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>0.11866359447004608</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>0.19815668202764977</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>0.29838709677419356</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>0.44354838709677419</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>0.89746543778801846</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="3"/>
+        <v>0.17081549320422329</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="4"/>
+        <v>0.2852452896225865</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="5"/>
+        <v>0.42952633728052264</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="6"/>
+        <v>0.63848509595753367</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>22</v>
+      </c>
+      <c r="D13">
+        <v>6058</v>
+      </c>
+      <c r="E13">
+        <v>3891</v>
+      </c>
+      <c r="F13" s="17">
+        <v>6328</v>
+      </c>
+      <c r="G13" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13">
+        <v>1028</v>
+      </c>
+      <c r="I13">
+        <v>1681</v>
+      </c>
+      <c r="J13">
+        <v>2231</v>
+      </c>
+      <c r="K13">
+        <v>2743</v>
+      </c>
+      <c r="L13" t="s">
+        <v>94</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="2"/>
+        <v>0.26419943459264972</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>0.43202261629401184</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>0.57337445386790031</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>0.70496016448213827</v>
+      </c>
+      <c r="Q13" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="3"/>
+        <v>0.42665202624878118</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="4"/>
+        <v>0.69766736977062371</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="5"/>
+        <v>0.92593450443680037</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V13" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="6">
+        <v>19</v>
+      </c>
+      <c r="D14" s="6">
+        <v>4888</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1384</v>
+      </c>
+      <c r="F14" s="17">
+        <v>3056</v>
+      </c>
+      <c r="H14">
+        <v>667</v>
+      </c>
+      <c r="I14">
+        <v>774</v>
+      </c>
+      <c r="J14">
+        <v>841</v>
+      </c>
+      <c r="K14">
+        <v>929</v>
+      </c>
+      <c r="L14">
+        <v>1144</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>0.48193641618497107</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0.55924855491329484</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>0.60765895953757221</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>0.67124277456647397</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>0.82658959537572252</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="3"/>
+        <v>0.70019557848863601</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="4"/>
+        <v>0.81252080622219536</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="5"/>
+        <v>0.88285529461610623</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="6"/>
+        <v>0.97523492116333266</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>1282</v>
+      </c>
+      <c r="E15">
+        <v>332</v>
+      </c>
+      <c r="F15" s="17">
+        <v>1041</v>
+      </c>
+      <c r="H15">
+        <v>226</v>
+      </c>
+      <c r="I15">
+        <v>261</v>
+      </c>
+      <c r="J15">
+        <v>277</v>
+      </c>
+      <c r="K15">
+        <v>290</v>
+      </c>
+      <c r="L15">
+        <v>308</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>0.68072289156626509</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>0.78614457831325302</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>0.83433734939759041</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>0.87349397590361444</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>0.92771084337349397</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="3"/>
+        <v>0.89782183488999223</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>21</v>
+      </c>
+      <c r="D16">
+        <v>2596</v>
+      </c>
+      <c r="E16">
+        <v>1470</v>
+      </c>
+      <c r="F16" s="17">
+        <v>1820</v>
+      </c>
+      <c r="H16">
+        <v>314</v>
+      </c>
+      <c r="I16">
+        <v>512</v>
+      </c>
+      <c r="J16">
+        <v>781</v>
+      </c>
+      <c r="K16">
+        <v>1037</v>
+      </c>
+      <c r="L16">
+        <v>1328</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>0.21360544217687075</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>0.34829931972789113</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>0.53129251700680269</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="0"/>
+        <v>0.70544217687074828</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>0.90340136054421771</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="3"/>
+        <v>0.3861329147043433</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="4"/>
+        <v>0.62961800104657251</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="5"/>
+        <v>0.96041339612768184</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="6">
+        <v>907</v>
+      </c>
+      <c r="E17" s="6">
+        <v>55</v>
+      </c>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18">
+        <v>2287</v>
+      </c>
+      <c r="E18">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19">
+        <v>1304</v>
+      </c>
+      <c r="E19">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20">
+        <v>375</v>
+      </c>
+      <c r="E20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21">
+        <v>1605</v>
+      </c>
+      <c r="E21">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22">
+        <v>1545</v>
+      </c>
+      <c r="E22">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="12">
+        <v>193</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23">
+        <v>1391</v>
+      </c>
+      <c r="E23">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="12">
+        <v>162</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24">
+        <v>1077</v>
+      </c>
+      <c r="E24">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="12">
+        <v>213</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25">
+        <v>844</v>
+      </c>
+      <c r="E25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26">
+        <v>375</v>
+      </c>
+      <c r="E26">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D3:D16">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D26">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F16">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F26">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4:V16">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE63A85-7D93-4276-809E-D8DD4BB648B4}">
+  <dimension ref="A1:R26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="H3" s="24">
+        <v>0.95</v>
+      </c>
+      <c r="I3" s="24">
+        <v>0.98</v>
+      </c>
+      <c r="J3" s="24">
+        <v>0.99</v>
+      </c>
+      <c r="K3" s="25">
+        <v>0.995</v>
+      </c>
+      <c r="L3" s="24">
+        <v>0.99900000000000011</v>
+      </c>
+      <c r="M3" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="N3" s="24">
+        <v>0.95</v>
+      </c>
+      <c r="O3" s="24">
+        <v>0.98</v>
+      </c>
+      <c r="P3" s="24">
+        <v>0.99</v>
+      </c>
+      <c r="Q3" s="25">
+        <v>0.995</v>
+      </c>
+      <c r="R3" s="24">
+        <v>0.99900000000000011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>31</v>
+      </c>
+      <c r="G4">
+        <v>24</v>
+      </c>
+      <c r="H4">
+        <v>25</v>
+      </c>
+      <c r="I4">
+        <v>26</v>
+      </c>
+      <c r="J4">
+        <v>26</v>
+      </c>
+      <c r="K4">
+        <v>26</v>
+      </c>
+      <c r="L4">
+        <v>31</v>
+      </c>
+      <c r="M4">
+        <f>G4/$F4</f>
+        <v>0.77419354838709675</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:R4" si="0">H4/$F4</f>
+        <v>0.80645161290322576</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>0.83870967741935487</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>0.83870967741935487</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>0.83870967741935487</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>37</v>
+      </c>
+      <c r="E5">
+        <v>68</v>
+      </c>
+      <c r="F5">
+        <v>74</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>31</v>
+      </c>
+      <c r="I5">
+        <v>64</v>
+      </c>
+      <c r="J5">
+        <v>65</v>
+      </c>
+      <c r="K5">
+        <v>66</v>
+      </c>
+      <c r="L5">
+        <v>69</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M16" si="1">G5/$F5</f>
+        <v>0.27027027027027029</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:N16" si="2">H5/$F5</f>
+        <v>0.41891891891891891</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5:O16" si="3">I5/$F5</f>
+        <v>0.86486486486486491</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5:P16" si="4">J5/$F5</f>
+        <v>0.8783783783783784</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ref="Q5:Q16" si="5">K5/$F5</f>
+        <v>0.89189189189189189</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5:R16" si="6">L5/$F5</f>
+        <v>0.93243243243243246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>39</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>132</v>
+      </c>
+      <c r="E7">
+        <v>92</v>
+      </c>
+      <c r="F7">
+        <v>119</v>
+      </c>
+      <c r="G7">
+        <v>78</v>
+      </c>
+      <c r="H7">
+        <v>103</v>
+      </c>
+      <c r="I7">
+        <v>114</v>
+      </c>
+      <c r="J7">
+        <v>116</v>
+      </c>
+      <c r="K7">
+        <v>116</v>
+      </c>
+      <c r="L7">
+        <v>117</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>0.65546218487394958</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>0.86554621848739499</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="3"/>
+        <v>0.95798319327731096</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="4"/>
+        <v>0.97478991596638653</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="5"/>
+        <v>0.97478991596638653</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="6"/>
+        <v>0.98319327731092432</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>4876</v>
+      </c>
+      <c r="E8">
+        <v>2355</v>
+      </c>
+      <c r="F8">
+        <v>5900</v>
+      </c>
+      <c r="G8">
+        <v>1822</v>
+      </c>
+      <c r="H8">
+        <v>4225</v>
+      </c>
+      <c r="I8">
+        <v>5606</v>
+      </c>
+      <c r="J8">
+        <v>5810</v>
+      </c>
+      <c r="K8">
+        <v>5866</v>
+      </c>
+      <c r="L8">
+        <v>5898</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>0.30881355932203391</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>0.71610169491525422</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="3"/>
+        <v>0.95016949152542374</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="4"/>
+        <v>0.98474576271186443</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="5"/>
+        <v>0.9942372881355932</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="6"/>
+        <v>0.99966101694915255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>907</v>
+      </c>
+      <c r="E9">
+        <v>55</v>
+      </c>
+      <c r="F9">
+        <v>61</v>
+      </c>
+      <c r="G9">
+        <v>53</v>
+      </c>
+      <c r="H9">
+        <v>55</v>
+      </c>
+      <c r="I9">
+        <v>56</v>
+      </c>
+      <c r="J9">
+        <v>56</v>
+      </c>
+      <c r="K9">
+        <v>56</v>
+      </c>
+      <c r="L9">
+        <v>59</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>0.86885245901639341</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="2"/>
+        <v>0.90163934426229508</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="3"/>
+        <v>0.91803278688524592</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="4"/>
+        <v>0.91803278688524592</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="5"/>
+        <v>0.91803278688524592</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="6"/>
+        <v>0.96721311475409832</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>390</v>
+      </c>
+      <c r="E10">
+        <v>694</v>
+      </c>
+      <c r="F10">
+        <v>729</v>
+      </c>
+      <c r="G10">
+        <v>516</v>
+      </c>
+      <c r="H10">
+        <v>723</v>
+      </c>
+      <c r="I10">
+        <v>724</v>
+      </c>
+      <c r="J10">
+        <v>724</v>
+      </c>
+      <c r="K10">
+        <v>724</v>
+      </c>
+      <c r="L10">
+        <v>724</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>0.70781893004115226</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="2"/>
+        <v>0.99176954732510292</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="3"/>
+        <v>0.99314128943758573</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="4"/>
+        <v>0.99314128943758573</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="5"/>
+        <v>0.99314128943758573</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="6"/>
+        <v>0.99314128943758573</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6">
+        <v>17</v>
+      </c>
+      <c r="D11" s="6">
+        <v>2998</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1379</v>
+      </c>
+      <c r="F11" s="17">
+        <v>2567</v>
+      </c>
+      <c r="G11" s="17">
+        <v>2128</v>
+      </c>
+      <c r="H11" s="17">
+        <v>2423</v>
+      </c>
+      <c r="I11" s="17">
+        <v>2561</v>
+      </c>
+      <c r="J11" s="17">
+        <v>2564</v>
+      </c>
+      <c r="K11" s="17">
+        <v>2565</v>
+      </c>
+      <c r="L11" s="17">
+        <v>2567</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>0.82898324892871056</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="2"/>
+        <v>0.94390338917023764</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="3"/>
+        <v>0.99766264121542658</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="4"/>
+        <v>0.99883132060771329</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="5"/>
+        <v>0.99922088040514223</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="17">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>1255</v>
+      </c>
+      <c r="E12">
+        <v>868</v>
+      </c>
+      <c r="F12" s="17">
+        <v>1975</v>
+      </c>
+      <c r="G12" s="17">
+        <v>192</v>
+      </c>
+      <c r="H12" s="17">
+        <v>256</v>
+      </c>
+      <c r="I12" s="17">
+        <v>986</v>
+      </c>
+      <c r="J12" s="17">
+        <v>1384</v>
+      </c>
+      <c r="K12" s="17">
+        <v>1962</v>
+      </c>
+      <c r="L12" s="17">
+        <v>1975</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>9.7215189873417721E-2</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="2"/>
+        <v>0.12962025316455697</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="3"/>
+        <v>0.49924050632911393</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="4"/>
+        <v>0.70075949367088608</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="5"/>
+        <v>0.99341772151898733</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>22</v>
+      </c>
+      <c r="D13">
+        <v>6058</v>
+      </c>
+      <c r="E13">
+        <v>3891</v>
+      </c>
+      <c r="F13" s="17">
+        <v>6328</v>
+      </c>
+      <c r="G13" s="17">
+        <v>1353</v>
+      </c>
+      <c r="H13" s="17">
+        <v>3393</v>
+      </c>
+      <c r="I13" s="17">
+        <v>5868</v>
+      </c>
+      <c r="J13" s="17">
+        <v>6188</v>
+      </c>
+      <c r="K13" s="17">
+        <v>6277</v>
+      </c>
+      <c r="L13" s="17">
+        <v>6324</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>0.21381163084702909</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="2"/>
+        <v>0.53618836915297097</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="3"/>
+        <v>0.927307206068268</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="4"/>
+        <v>0.97787610619469023</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="5"/>
+        <v>0.99194058154235143</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="6"/>
+        <v>0.99936788874841975</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="6">
+        <v>19</v>
+      </c>
+      <c r="D14" s="6">
+        <v>4888</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1384</v>
+      </c>
+      <c r="F14" s="17">
+        <v>3056</v>
+      </c>
+      <c r="G14" s="17">
+        <v>2037</v>
+      </c>
+      <c r="H14" s="17">
+        <v>2583</v>
+      </c>
+      <c r="I14" s="17">
+        <v>2976</v>
+      </c>
+      <c r="J14" s="17">
+        <v>3037</v>
+      </c>
+      <c r="K14" s="17">
+        <v>3051</v>
+      </c>
+      <c r="L14" s="17">
+        <v>3056</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>0.66655759162303663</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="2"/>
+        <v>0.8452225130890052</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="3"/>
+        <v>0.97382198952879584</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="4"/>
+        <v>0.99378272251308897</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="5"/>
+        <v>0.99836387434554974</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>1282</v>
+      </c>
+      <c r="E15">
+        <v>332</v>
+      </c>
+      <c r="F15" s="17">
+        <v>1041</v>
+      </c>
+      <c r="G15" s="17">
+        <v>767</v>
+      </c>
+      <c r="H15" s="17">
+        <v>999</v>
+      </c>
+      <c r="I15" s="17">
+        <v>1018</v>
+      </c>
+      <c r="J15" s="17">
+        <v>1037</v>
+      </c>
+      <c r="K15" s="17">
+        <v>1040</v>
+      </c>
+      <c r="L15" s="17">
+        <v>1041</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>0.73679154658981749</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>0.95965417867435154</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="3"/>
+        <v>0.97790585975024014</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="4"/>
+        <v>0.99615754082612873</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="5"/>
+        <v>0.99903938520653213</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>21</v>
+      </c>
+      <c r="D16">
+        <v>2596</v>
+      </c>
+      <c r="E16">
+        <v>1470</v>
+      </c>
+      <c r="F16" s="17">
+        <v>1820</v>
+      </c>
+      <c r="G16" s="17">
+        <v>25</v>
+      </c>
+      <c r="H16" s="17">
+        <v>795</v>
+      </c>
+      <c r="I16" s="17">
+        <v>1620</v>
+      </c>
+      <c r="J16" s="17">
+        <v>1734</v>
+      </c>
+      <c r="K16" s="17">
+        <v>1808</v>
+      </c>
+      <c r="L16" s="17">
+        <v>1816</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>1.3736263736263736E-2</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="2"/>
+        <v>0.43681318681318682</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="3"/>
+        <v>0.89010989010989006</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="4"/>
+        <v>0.95274725274725269</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="5"/>
+        <v>0.99340659340659343</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="6"/>
+        <v>0.99780219780219781</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="6">
+        <v>907</v>
+      </c>
+      <c r="E17" s="6">
+        <v>55</v>
+      </c>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18">
+        <v>2287</v>
+      </c>
+      <c r="E18">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19">
+        <v>1304</v>
+      </c>
+      <c r="E19">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20">
+        <v>375</v>
+      </c>
+      <c r="E20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21">
+        <v>1605</v>
+      </c>
+      <c r="E21">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22">
+        <v>1545</v>
+      </c>
+      <c r="E22">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="12">
+        <v>193</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23">
+        <v>1391</v>
+      </c>
+      <c r="E23">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="12">
+        <v>162</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24">
+        <v>1077</v>
+      </c>
+      <c r="E24">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="12">
+        <v>213</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25">
+        <v>844</v>
+      </c>
+      <c r="E25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26">
+        <v>375</v>
+      </c>
+      <c r="E26">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D3:D16">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D26">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F16 G4:L5 G7:L16">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F26 G4:L5 G7:L16">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4:R16">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABCEEC2-D4D8-41AA-8F98-E40E7997937F}">
+  <dimension ref="A1:N26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="24">
+        <v>0.99</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3" s="24">
+        <v>0.99</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="N3" s="24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>31</v>
+      </c>
+      <c r="G4">
+        <v>26</v>
+      </c>
+      <c r="H4">
+        <v>11</v>
+      </c>
+      <c r="I4">
+        <v>18</v>
+      </c>
+      <c r="J4">
+        <v>19</v>
+      </c>
+      <c r="K4">
+        <f>G4/$F4</f>
+        <v>0.83870967741935487</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:N16" si="0">H4/$F4</f>
+        <v>0.35483870967741937</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>0.58064516129032262</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>0.61290322580645162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>37</v>
+      </c>
+      <c r="E5">
+        <v>68</v>
+      </c>
+      <c r="F5">
+        <v>74</v>
+      </c>
+      <c r="G5">
+        <v>65</v>
+      </c>
+      <c r="H5">
+        <v>24</v>
+      </c>
+      <c r="I5">
+        <v>27</v>
+      </c>
+      <c r="J5">
+        <v>31</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K16" si="1">G5/$F5</f>
+        <v>0.8783783783783784</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>0.32432432432432434</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>0.36486486486486486</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>0.41891891891891891</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>39</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>132</v>
+      </c>
+      <c r="E7">
+        <v>92</v>
+      </c>
+      <c r="F7">
+        <v>119</v>
+      </c>
+      <c r="G7">
+        <v>116</v>
+      </c>
+      <c r="H7">
+        <v>53</v>
+      </c>
+      <c r="I7">
+        <v>67</v>
+      </c>
+      <c r="J7">
+        <v>76</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>0.97478991596638653</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>0.44537815126050423</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>0.56302521008403361</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>0.6386554621848739</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>4876</v>
+      </c>
+      <c r="E8">
+        <v>2355</v>
+      </c>
+      <c r="F8">
+        <v>5900</v>
+      </c>
+      <c r="G8">
+        <v>5810</v>
+      </c>
+      <c r="H8">
+        <v>4149</v>
+      </c>
+      <c r="I8">
+        <v>4631</v>
+      </c>
+      <c r="J8">
+        <v>4760</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>0.98474576271186443</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0.70322033898305081</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0.78491525423728814</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0.8067796610169492</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>907</v>
+      </c>
+      <c r="E9">
+        <v>55</v>
+      </c>
+      <c r="F9">
+        <v>61</v>
+      </c>
+      <c r="G9">
+        <v>56</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>19</v>
+      </c>
+      <c r="J9">
+        <v>25</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>0.91803278688524592</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>0.16393442622950818</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>0.31147540983606559</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>0.4098360655737705</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>390</v>
+      </c>
+      <c r="E10">
+        <v>694</v>
+      </c>
+      <c r="F10">
+        <v>729</v>
+      </c>
+      <c r="G10">
+        <v>724</v>
+      </c>
+      <c r="H10">
+        <v>276</v>
+      </c>
+      <c r="I10">
+        <v>415</v>
+      </c>
+      <c r="J10">
+        <v>444</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>0.99314128943758573</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>0.37860082304526749</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>0.56927297668038412</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>0.60905349794238683</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6">
+        <v>17</v>
+      </c>
+      <c r="D11" s="6">
+        <v>2998</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1379</v>
+      </c>
+      <c r="F11" s="17">
+        <v>2567</v>
+      </c>
+      <c r="G11" s="17">
+        <v>2564</v>
+      </c>
+      <c r="H11" s="17">
+        <v>1547</v>
+      </c>
+      <c r="I11" s="17">
+        <v>1871</v>
+      </c>
+      <c r="J11" s="17">
+        <v>1928</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>0.99883132060771329</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>0.60264900662251653</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>0.72886638098948187</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>0.75107128944292945</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="17">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>1255</v>
+      </c>
+      <c r="E12">
+        <v>868</v>
+      </c>
+      <c r="F12" s="17">
+        <v>1975</v>
+      </c>
+      <c r="G12" s="17">
+        <v>1384</v>
+      </c>
+      <c r="H12" s="17">
+        <v>1160</v>
+      </c>
+      <c r="I12" s="17">
+        <v>1179</v>
+      </c>
+      <c r="J12" s="17">
+        <v>1196</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>0.70075949367088608</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>0.58734177215189876</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>0.5969620253164557</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>0.60556962025316452</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>22</v>
+      </c>
+      <c r="D13">
+        <v>6058</v>
+      </c>
+      <c r="E13">
+        <v>3891</v>
+      </c>
+      <c r="F13" s="17">
+        <v>6328</v>
+      </c>
+      <c r="G13" s="17">
+        <v>6188</v>
+      </c>
+      <c r="H13" s="17">
+        <v>4809</v>
+      </c>
+      <c r="I13" s="17">
+        <v>5091</v>
+      </c>
+      <c r="J13" s="17">
+        <v>5233</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>0.97787610619469023</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>0.75995575221238942</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>0.80451959544879903</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>0.82695954487989887</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="6">
+        <v>19</v>
+      </c>
+      <c r="D14" s="6">
+        <v>4888</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1384</v>
+      </c>
+      <c r="F14" s="17">
+        <v>3056</v>
+      </c>
+      <c r="G14" s="17">
+        <v>3037</v>
+      </c>
+      <c r="H14" s="17">
+        <v>1559</v>
+      </c>
+      <c r="I14" s="17">
+        <v>1937</v>
+      </c>
+      <c r="J14" s="17">
+        <v>2132</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>0.99378272251308897</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>0.51014397905759157</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>0.63383507853403143</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0.69764397905759157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>1282</v>
+      </c>
+      <c r="E15">
+        <v>332</v>
+      </c>
+      <c r="F15" s="17">
+        <v>1041</v>
+      </c>
+      <c r="G15" s="17">
+        <v>1037</v>
+      </c>
+      <c r="H15" s="17">
+        <v>460</v>
+      </c>
+      <c r="I15" s="17">
+        <v>606</v>
+      </c>
+      <c r="J15" s="17">
+        <v>666</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>0.99615754082612873</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>0.44188280499519694</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>0.58213256484149856</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>0.63976945244956773</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>21</v>
+      </c>
+      <c r="D16">
+        <v>2596</v>
+      </c>
+      <c r="E16">
+        <v>1470</v>
+      </c>
+      <c r="F16" s="17">
+        <v>1820</v>
+      </c>
+      <c r="G16" s="17">
+        <v>1734</v>
+      </c>
+      <c r="H16" s="17">
+        <v>1300</v>
+      </c>
+      <c r="I16" s="17">
+        <v>1623</v>
+      </c>
+      <c r="J16" s="17">
+        <v>1639</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>0.95274725274725269</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>0.89175824175824181</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>0.90054945054945057</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="6">
+        <v>907</v>
+      </c>
+      <c r="E17" s="6">
+        <v>55</v>
+      </c>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18">
+        <v>2287</v>
+      </c>
+      <c r="E18">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19">
+        <v>1304</v>
+      </c>
+      <c r="E19">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20">
+        <v>375</v>
+      </c>
+      <c r="E20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21">
+        <v>1605</v>
+      </c>
+      <c r="E21">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22">
+        <v>1545</v>
+      </c>
+      <c r="E22">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="12">
+        <v>193</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23">
+        <v>1391</v>
+      </c>
+      <c r="E23">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="12">
+        <v>162</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24">
+        <v>1077</v>
+      </c>
+      <c r="E24">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="12">
+        <v>213</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25">
+        <v>844</v>
+      </c>
+      <c r="E25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26">
+        <v>375</v>
+      </c>
+      <c r="E26">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D3:D16">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D26">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F16 G4:J5 G7:J16">
+    <cfRule type="colorScale" priority="76">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F26 G4:J5 G7:J16">
+    <cfRule type="colorScale" priority="81">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:N16">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changing computers (minor changes: mainly fixing linear hosting capacity which was not working for 'fxd' tap on models)
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C346D2-61C5-4F0B-9435-A13BF505DEE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3798AD14-D6B2-4CC2-A905-AB785B230A41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -5645,8 +5645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11FE248-93EC-498A-B149-79239CF2A22B}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6895,7 +6895,7 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7924,8 +7924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABCEEC2-D4D8-41AA-8F98-E40E7997937F}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
First round of testing for linear models. Preliminary results suggest that small networks need a different set of parameters compared to the larger networks? Still need to automate processing the results to save.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3798AD14-D6B2-4CC2-A905-AB785B230A41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -16,7 +15,7 @@
     <sheet name="varStuff" sheetId="6" r:id="rId6"/>
     <sheet name="varV2stuff" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="105">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -337,12 +336,21 @@
   </si>
   <si>
     <t>99%, 95%</t>
+  </si>
+  <si>
+    <t>90%, 95%</t>
+  </si>
+  <si>
+    <t>90%, 98%</t>
+  </si>
+  <si>
+    <t>90%, 99%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2210,11 +2218,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E1:E1048576"/>
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2223,25 +2231,25 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" customWidth="1"/>
     <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.42578125" customWidth="1"/>
-    <col min="21" max="21" width="23" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.42578125" customWidth="1"/>
+    <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -2254,47 +2262,48 @@
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="F1" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="N1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="N1" s="27" t="s">
         <v>25</v>
       </c>
+      <c r="O1" s="27"/>
       <c r="P1" s="27"/>
       <c r="Q1" s="27"/>
       <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="23"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S1" s="23"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
@@ -2302,38 +2311,37 @@
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="O2" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="T2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="U2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="V2" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="X2" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -2346,31 +2354,34 @@
       <c r="D3" s="6">
         <v>4</v>
       </c>
-      <c r="F3" s="6">
+      <c r="E3" s="6">
         <f>LOG(svdStuff!E3*D3)</f>
         <v>0.6020599913279624</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
       <c r="I3" s="6">
         <v>0</v>
       </c>
-      <c r="J3" s="6">
-        <v>0</v>
-      </c>
-      <c r="K3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>19</v>
+      </c>
+      <c r="K3" s="6">
+        <v>5.4</v>
       </c>
       <c r="L3" s="6">
         <v>5.4</v>
       </c>
-      <c r="M3" s="6">
-        <v>5.4</v>
-      </c>
-      <c r="N3" s="21" t="s">
+      <c r="M3" s="21" t="s">
         <v>26</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="O3" s="8" t="s">
         <v>27</v>
@@ -2387,11 +2398,8 @@
       <c r="S3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="T3" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -2401,35 +2409,38 @@
       <c r="D4">
         <v>16</v>
       </c>
-      <c r="F4" s="13">
+      <c r="E4" s="13">
         <f>LOG(svdStuff!E4*D4)</f>
         <v>2.3802112417116059</v>
       </c>
-      <c r="G4" t="s">
+      <c r="F4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="2">
+      <c r="G4" s="2">
         <v>4.16</v>
       </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
       <c r="I4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K4">
-        <v>1.5</v>
+        <v>3.6</v>
       </c>
       <c r="L4">
         <v>3.6</v>
       </c>
       <c r="M4">
-        <v>3.6</v>
-      </c>
-      <c r="N4">
         <f>LOG10(703)</f>
         <v>2.8469553250198238</v>
       </c>
+      <c r="N4" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O4" s="1" t="s">
         <v>26</v>
       </c>
@@ -2445,23 +2456,20 @@
       <c r="S4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V4">
+      <c r="U4">
         <f>18/60</f>
         <v>0.3</v>
       </c>
+      <c r="V4">
+        <f>(10^M4)*9000*0.000001/60</f>
+        <v>0.10545000000000002</v>
+      </c>
       <c r="W4">
-        <f>(10^N4)*9000*0.000001/60</f>
-        <v>0.10545000000000002</v>
-      </c>
-      <c r="X4">
         <f>18/60</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -2471,35 +2479,38 @@
       <c r="D5">
         <v>37</v>
       </c>
-      <c r="F5" s="13">
+      <c r="E5" s="13">
         <f>LOG(svdStuff!E5*D5)</f>
         <v>3.4007106367732312</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F5" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="2">
+      <c r="G5" s="2">
         <v>24.9</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
       </c>
       <c r="I5">
         <v>2</v>
       </c>
       <c r="J5">
+        <v>50</v>
+      </c>
+      <c r="K5">
         <v>2</v>
-      </c>
-      <c r="K5">
-        <v>50</v>
       </c>
       <c r="L5">
         <v>2</v>
       </c>
       <c r="M5">
-        <v>2</v>
-      </c>
-      <c r="N5">
         <f>LOG10(4000)</f>
         <v>3.6020599913279625</v>
       </c>
+      <c r="N5" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O5" s="1" t="s">
         <v>26</v>
       </c>
@@ -2515,23 +2526,20 @@
       <c r="S5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V5">
+      <c r="U5">
         <f>53.7/60</f>
         <v>0.89500000000000002</v>
       </c>
+      <c r="V5">
+        <f t="shared" ref="V5:V26" si="0">(10^M5)*9000*0.000001/60</f>
+        <v>0.60000000000000098</v>
+      </c>
       <c r="W5">
-        <f t="shared" ref="W5:W26" si="0">(10^N5)*9000*0.000001/60</f>
-        <v>0.60000000000000098</v>
-      </c>
-      <c r="X5">
         <f>19/60</f>
         <v>0.31666666666666665</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -2541,40 +2549,43 @@
       <c r="D6">
         <v>39</v>
       </c>
-      <c r="F6" s="13">
+      <c r="E6" s="13">
         <f>LOG(svdStuff!E6*D6)</f>
         <v>3.0681858617461617</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="2">
+      <c r="G6" s="2">
         <v>4.8</v>
       </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K6">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="L6">
         <v>2.6</v>
       </c>
       <c r="M6">
-        <v>2.6</v>
-      </c>
-      <c r="N6">
         <f>LOG10(2907)</f>
         <v>3.4634450317704277</v>
       </c>
+      <c r="N6" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="O6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>27</v>
@@ -2585,15 +2596,12 @@
       <c r="S6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="T6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W6">
+      <c r="V6">
         <f t="shared" si="0"/>
         <v>0.43605000000000016</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -2603,37 +2611,40 @@
       <c r="D7">
         <v>132</v>
       </c>
-      <c r="F7" s="13">
+      <c r="E7" s="13">
         <f>LOG(svdStuff!E7*D7)</f>
         <v>4.0843617585514052</v>
       </c>
-      <c r="G7" t="s">
+      <c r="F7" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="2">
+      <c r="G7" s="2">
         <v>2.4</v>
       </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
       <c r="I7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K7">
-        <v>6</v>
+        <v>3.6</v>
       </c>
       <c r="L7">
         <v>3.6</v>
       </c>
       <c r="M7">
-        <v>3.6</v>
-      </c>
-      <c r="N7">
         <f>LOG10(4965)</f>
         <v>3.6959192528313998</v>
       </c>
+      <c r="N7" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="O7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>26</v>
@@ -2647,23 +2658,20 @@
       <c r="S7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V7">
+      <c r="U7">
         <f>72/60</f>
         <v>1.2</v>
       </c>
+      <c r="V7">
+        <f t="shared" si="0"/>
+        <v>0.74475000000000013</v>
+      </c>
       <c r="W7">
-        <f t="shared" si="0"/>
-        <v>0.74475000000000013</v>
-      </c>
-      <c r="X7">
         <f>33/60</f>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -2673,63 +2681,63 @@
       <c r="D8">
         <v>4876</v>
       </c>
-      <c r="F8" s="13">
+      <c r="E8" s="13">
         <f>LOG(svdStuff!E8*D8)</f>
         <v>7.0600546084112592</v>
       </c>
-      <c r="G8" t="s">
+      <c r="F8" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="2">
+      <c r="G8" s="2">
         <v>7.2</v>
       </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
       <c r="I8">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J8">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="K8">
-        <v>17</v>
+        <v>12.05</v>
       </c>
       <c r="L8">
         <v>12.05</v>
       </c>
       <c r="M8">
-        <v>12.05</v>
-      </c>
-      <c r="N8">
         <f>LOG10(275763)</f>
         <v>5.4405359950748213</v>
       </c>
+      <c r="N8" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="O8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="Q8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R8" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="1" t="s">
-        <v>26</v>
+      <c r="V8">
+        <f t="shared" si="0"/>
+        <v>41.364450000000069</v>
       </c>
       <c r="W8">
-        <f t="shared" si="0"/>
-        <v>41.364450000000069</v>
-      </c>
-      <c r="X8">
         <f>958/60</f>
         <v>15.966666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -2739,63 +2747,63 @@
       <c r="D9">
         <v>907</v>
       </c>
-      <c r="F9" s="13">
+      <c r="E9" s="13">
         <f>LOG(svdStuff!E9*D9)</f>
         <v>4.6979699765543392</v>
       </c>
-      <c r="G9" t="s">
+      <c r="F9" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="2">
+      <c r="G9" s="2">
         <v>0.41599999999999998</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="K9">
-        <v>0.3</v>
+        <v>5.5E-2</v>
       </c>
       <c r="L9">
         <v>5.5E-2</v>
       </c>
       <c r="M9">
-        <v>5.5E-2</v>
-      </c>
-      <c r="N9">
         <f>LOG10(5144)</f>
         <v>3.7113009599161657</v>
       </c>
+      <c r="N9" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="1" t="s">
-        <v>26</v>
+      <c r="V9">
+        <f t="shared" si="0"/>
+        <v>0.77160000000000128</v>
       </c>
       <c r="W9">
-        <f t="shared" si="0"/>
-        <v>0.77160000000000128</v>
-      </c>
-      <c r="X9">
         <f>59/60</f>
         <v>0.98333333333333328</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -2805,60 +2813,60 @@
       <c r="D10">
         <v>390</v>
       </c>
-      <c r="F10" s="13">
+      <c r="E10" s="13">
         <f>LOG(svdStuff!E10*D10)</f>
         <v>5.4324240774813539</v>
       </c>
-      <c r="G10" t="s">
+      <c r="F10" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="2">
+      <c r="G10" s="2">
         <v>13.8</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
-      <c r="J10">
-        <v>0</v>
+      <c r="K10">
+        <v>42.8</v>
       </c>
       <c r="L10">
         <v>42.8</v>
       </c>
-      <c r="M10">
-        <v>42.8</v>
-      </c>
-      <c r="N10" s="15">
+      <c r="M10" s="15">
         <f>LOG10(12061)</f>
         <v>4.0813833174622856</v>
       </c>
+      <c r="N10" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>27</v>
+      <c r="V10">
+        <f t="shared" si="0"/>
+        <v>1.8091500000000034</v>
       </c>
       <c r="W10">
-        <f t="shared" si="0"/>
-        <v>1.8091500000000034</v>
-      </c>
-      <c r="X10">
         <f>145/60</f>
         <v>2.4166666666666665</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -2871,67 +2879,67 @@
       <c r="D11" s="6">
         <v>2998</v>
       </c>
-      <c r="F11" s="6">
+      <c r="E11" s="6">
         <f>LOG(svdStuff!E11*D11)</f>
         <v>6.6163958946881101</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="7">
+      <c r="G11" s="7">
         <v>12.47</v>
       </c>
+      <c r="H11" s="6">
+        <v>4</v>
+      </c>
       <c r="I11" s="6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J11" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K11" s="6">
-        <v>5</v>
+        <v>16.3</v>
       </c>
       <c r="L11" s="6">
         <v>16.3</v>
       </c>
-      <c r="M11" s="6">
-        <v>16.3</v>
-      </c>
-      <c r="N11">
+      <c r="M11">
         <f>LOG10(32321)</f>
         <v>4.50948478922394</v>
       </c>
+      <c r="N11" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="O11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="P11" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="Q11" s="8" t="s">
         <v>27</v>
       </c>
       <c r="R11" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="T11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="V11">
+      <c r="U11">
         <f>637/60</f>
         <v>10.616666666666667</v>
       </c>
+      <c r="V11">
+        <f t="shared" si="0"/>
+        <v>4.8481500000000013</v>
+      </c>
       <c r="W11">
-        <f t="shared" si="0"/>
-        <v>4.8481500000000013</v>
-      </c>
-      <c r="X11">
         <f>371/60</f>
         <v>6.1833333333333336</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -2941,69 +2949,69 @@
       <c r="D12">
         <v>1255</v>
       </c>
-      <c r="F12" s="13">
+      <c r="E12" s="13">
         <f>LOG(svdStuff!E12*D12)</f>
         <v>6.0371634509935488</v>
       </c>
-      <c r="G12" t="s">
+      <c r="F12" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="2">
+      <c r="G12" s="2">
         <v>12.47</v>
       </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
       <c r="I12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K12">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="L12">
-        <v>78</v>
+        <v>19.3</v>
       </c>
       <c r="M12">
-        <v>19.3</v>
-      </c>
-      <c r="N12">
         <f>LOG10(17450)</f>
         <v>4.2417954312951984</v>
       </c>
+      <c r="N12" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T12" s="1" t="s">
-        <v>26</v>
+      <c r="T12" t="s">
+        <v>78</v>
       </c>
       <c r="U12" t="s">
-        <v>78</v>
-      </c>
-      <c r="V12" t="s">
         <v>90</v>
       </c>
+      <c r="V12">
+        <f t="shared" si="0"/>
+        <v>2.6175000000000002</v>
+      </c>
       <c r="W12">
-        <f t="shared" si="0"/>
-        <v>2.6175000000000002</v>
-      </c>
-      <c r="X12">
         <f>367/60</f>
         <v>6.1166666666666663</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -3013,35 +3021,38 @@
       <c r="D13">
         <v>6058</v>
       </c>
-      <c r="F13" s="13">
+      <c r="E13" s="13">
         <f>LOG(svdStuff!E13*D13)</f>
         <v>7.3723904998005798</v>
       </c>
-      <c r="G13" t="s">
+      <c r="F13" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="2">
+      <c r="G13" s="2">
         <v>34.5</v>
       </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
       <c r="I13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J13">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K13">
-        <v>10</v>
+        <v>52.2</v>
       </c>
       <c r="L13">
-        <v>52.2</v>
-      </c>
-      <c r="M13">
         <v>69.400000000000006</v>
       </c>
-      <c r="N13" s="15">
+      <c r="M13" s="15">
         <f>LOG10(87955)</f>
         <v>4.9442605329428515</v>
       </c>
+      <c r="N13" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O13" s="1" t="s">
         <v>26</v>
       </c>
@@ -3049,30 +3060,27 @@
         <v>26</v>
       </c>
       <c r="Q13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="S13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V13" t="s">
+      <c r="U13" t="s">
         <v>89</v>
       </c>
+      <c r="V13">
+        <f t="shared" si="0"/>
+        <v>13.193250000000001</v>
+      </c>
       <c r="W13">
-        <f t="shared" si="0"/>
-        <v>13.193250000000001</v>
-      </c>
-      <c r="X13">
         <f>1996/60</f>
         <v>33.266666666666666</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
@@ -3085,33 +3093,36 @@
       <c r="D14" s="6">
         <v>4888</v>
       </c>
-      <c r="F14" s="6">
+      <c r="E14" s="6">
         <f>LOG(svdStuff!E14*D14)</f>
         <v>6.8302672873552366</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="7">
+      <c r="G14" s="7">
         <v>12.47</v>
       </c>
+      <c r="H14" s="6">
+        <v>5</v>
+      </c>
       <c r="I14" s="6">
-        <v>5</v>
-      </c>
-      <c r="J14" s="6">
         <v>9</v>
       </c>
-      <c r="K14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6">
+        <v>11.6</v>
+      </c>
       <c r="L14" s="6">
         <v>11.6</v>
       </c>
-      <c r="M14" s="6">
-        <v>11.6</v>
-      </c>
-      <c r="N14">
+      <c r="M14">
         <f>LOG10(26279)</f>
         <v>4.4196088349081029</v>
       </c>
+      <c r="N14" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="O14" s="8" t="s">
         <v>26</v>
       </c>
@@ -3119,30 +3130,27 @@
         <v>26</v>
       </c>
       <c r="Q14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R14" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="R14" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="S14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="T14" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="U14" t="s">
+      <c r="T14" t="s">
         <v>62</v>
       </c>
+      <c r="V14">
+        <f t="shared" si="0"/>
+        <v>3.9418500000000019</v>
+      </c>
       <c r="W14">
-        <f t="shared" si="0"/>
-        <v>3.9418500000000019</v>
-      </c>
-      <c r="X14">
         <f>551/60</f>
         <v>9.1833333333333336</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -3152,32 +3160,35 @@
       <c r="D15">
         <v>1282</v>
       </c>
-      <c r="F15" s="13">
+      <c r="E15" s="13">
         <f>LOG(svdStuff!E15*D15)</f>
         <v>5.6290261088868352</v>
       </c>
-      <c r="G15" t="s">
+      <c r="F15" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="2">
+      <c r="G15" s="2">
         <v>13.2</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
-      <c r="J15">
-        <v>1</v>
+      <c r="K15">
+        <v>12.74</v>
       </c>
       <c r="L15">
         <v>12.74</v>
       </c>
       <c r="M15">
-        <v>12.74</v>
-      </c>
-      <c r="N15">
         <f>LOG10(20153)</f>
         <v>4.3043397048923389</v>
       </c>
+      <c r="N15" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O15" s="1" t="s">
         <v>26</v>
       </c>
@@ -3193,19 +3204,16 @@
       <c r="S15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T15" s="1" t="s">
-        <v>26</v>
+      <c r="V15">
+        <f t="shared" si="0"/>
+        <v>3.0229500000000038</v>
       </c>
       <c r="W15">
-        <f t="shared" si="0"/>
-        <v>3.0229500000000038</v>
-      </c>
-      <c r="X15">
         <f>107/60</f>
         <v>1.7833333333333334</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>23</v>
       </c>
@@ -3215,32 +3223,35 @@
       <c r="D16">
         <v>2596</v>
       </c>
-      <c r="F16" s="13">
+      <c r="E16" s="13">
         <f>LOG(svdStuff!E16*D16)</f>
         <v>6.5816220228765081</v>
       </c>
-      <c r="G16" t="s">
+      <c r="F16" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="2">
+      <c r="G16" s="2">
         <v>12.47</v>
       </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
       <c r="I16">
-        <v>3</v>
-      </c>
-      <c r="J16">
         <v>1</v>
+      </c>
+      <c r="K16">
+        <v>15.67</v>
       </c>
       <c r="L16">
         <v>15.67</v>
       </c>
-      <c r="M16">
-        <v>15.67</v>
-      </c>
-      <c r="N16" s="15">
+      <c r="M16" s="15">
         <f>LOG10(27688)</f>
         <v>4.4422915862860712</v>
       </c>
+      <c r="N16" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O16" s="1" t="s">
         <v>26</v>
       </c>
@@ -3248,27 +3259,24 @@
         <v>26</v>
       </c>
       <c r="Q16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R16" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="S16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T16" s="1" t="s">
-        <v>26</v>
+      <c r="V16">
+        <f t="shared" si="0"/>
+        <v>4.1532000000000036</v>
       </c>
       <c r="W16">
-        <f t="shared" si="0"/>
-        <v>4.1532000000000036</v>
-      </c>
-      <c r="X16">
         <f>445/60</f>
         <v>7.416666666666667</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>93</v>
       </c>
@@ -3281,56 +3289,56 @@
       <c r="D17" s="6">
         <v>907</v>
       </c>
-      <c r="F17" s="6">
+      <c r="E17" s="6">
         <f>LOG(svdStuff!E17*D17)</f>
         <v>4.6979699765543392</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="7">
+      <c r="G17" s="7">
         <v>0.41599999999999998</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0</v>
       </c>
       <c r="I17" s="6">
         <v>0</v>
       </c>
-      <c r="J17" s="6">
-        <v>0</v>
-      </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6">
+      <c r="J17" s="6"/>
+      <c r="K17" s="6">
         <f>svdStuff!E17*0.001</f>
         <v>5.5E-2</v>
       </c>
-      <c r="M17" s="6">
+      <c r="L17" s="6">
         <v>5.5E-2</v>
       </c>
-      <c r="N17">
+      <c r="M17">
         <f>LOG10(10388)</f>
         <v>4.0165319409572655</v>
       </c>
+      <c r="N17" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="O17" s="8" t="s">
         <v>26</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q17" s="8" t="s">
         <v>27</v>
       </c>
       <c r="R17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="T17" s="8"/>
-      <c r="W17">
+      <c r="S17" s="8"/>
+      <c r="V17">
         <f t="shared" si="0"/>
         <v>1.5582000000000018</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>39</v>
       </c>
@@ -3340,55 +3348,55 @@
       <c r="D18">
         <v>2287</v>
       </c>
-      <c r="F18" s="13">
+      <c r="E18" s="13">
         <f>LOG(svdStuff!E18*D18)</f>
         <v>5.602304213293043</v>
       </c>
-      <c r="G18" t="s">
+      <c r="F18" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="2">
+      <c r="G18" s="2">
         <v>0.41599999999999998</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="L18" s="13">
+      <c r="K18" s="13">
         <f>svdStuff!E18*0.001</f>
         <v>0.17500000000000002</v>
       </c>
-      <c r="M18" s="13">
+      <c r="L18" s="13">
         <v>0.17500000000000002</v>
       </c>
-      <c r="N18">
+      <c r="M18">
         <f>LOG10(24732)</f>
         <v>4.3932592378268378</v>
       </c>
+      <c r="N18" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T18" s="1"/>
-      <c r="W18">
+      <c r="S18" s="1"/>
+      <c r="V18">
         <f t="shared" si="0"/>
         <v>3.7098000000000053</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>40</v>
       </c>
@@ -3398,55 +3406,55 @@
       <c r="D19">
         <v>1304</v>
       </c>
-      <c r="F19" s="13">
+      <c r="E19" s="13">
         <f>LOG(svdStuff!E19*D19)</f>
         <v>5.0884054449956002</v>
       </c>
-      <c r="G19" t="s">
+      <c r="F19" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="2">
+      <c r="G19" s="2">
         <v>0.41599999999999998</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="L19" s="13">
+      <c r="K19" s="13">
         <f>svdStuff!E19*0.001</f>
         <v>9.4E-2</v>
       </c>
-      <c r="M19" s="13">
+      <c r="L19" s="13">
         <v>9.4E-2</v>
       </c>
-      <c r="N19">
+      <c r="M19">
         <f>LOG10(24431)</f>
         <v>4.3879412437066989</v>
       </c>
+      <c r="N19" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O19" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T19" s="1"/>
-      <c r="W19">
+      <c r="S19" s="1"/>
+      <c r="V19">
         <f t="shared" si="0"/>
         <v>3.6646500000000035</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>36</v>
       </c>
@@ -3456,55 +3464,55 @@
       <c r="D20">
         <v>375</v>
       </c>
-      <c r="F20" s="13">
+      <c r="E20" s="13">
         <f>LOG(svdStuff!E20*D20)</f>
         <v>3.9542425094393248</v>
       </c>
-      <c r="G20" t="s">
+      <c r="F20" t="s">
         <v>30</v>
       </c>
-      <c r="H20" s="2">
+      <c r="G20" s="2">
         <v>0.41599999999999998</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="L20" s="13">
+      <c r="K20" s="13">
         <f>svdStuff!E20*0.001</f>
         <v>2.4E-2</v>
       </c>
-      <c r="M20" s="13">
+      <c r="L20" s="13">
         <v>2.4E-2</v>
       </c>
-      <c r="N20">
+      <c r="M20">
         <f>LOG10(6773)</f>
         <v>3.8307810756063612</v>
       </c>
+      <c r="N20" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O20" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T20" s="1"/>
-      <c r="W20">
+      <c r="S20" s="1"/>
+      <c r="V20">
         <f t="shared" si="0"/>
         <v>1.0159500000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>34</v>
       </c>
@@ -3514,55 +3522,55 @@
       <c r="D21">
         <v>1605</v>
       </c>
-      <c r="F21" s="13">
+      <c r="E21" s="13">
         <f>LOG(svdStuff!E21*D21)</f>
         <v>5.2661728770945029</v>
       </c>
-      <c r="G21" t="s">
+      <c r="F21" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="2">
+      <c r="G21" s="2">
         <v>0.41599999999999998</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
       </c>
       <c r="I21">
         <v>0</v>
       </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="L21" s="13">
+      <c r="K21" s="13">
         <f>svdStuff!E21*0.001</f>
         <v>0.115</v>
       </c>
-      <c r="M21" s="13">
+      <c r="L21" s="13">
         <v>0.115</v>
       </c>
-      <c r="N21">
+      <c r="M21">
         <f>LOG10(26276)</f>
         <v>4.4195592531957208</v>
       </c>
+      <c r="N21" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O21" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T21" s="1"/>
-      <c r="W21">
+      <c r="S21" s="1"/>
+      <c r="V21">
         <f t="shared" si="0"/>
         <v>3.9414000000000047</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>35</v>
       </c>
@@ -3572,55 +3580,55 @@
       <c r="D22">
         <v>1545</v>
       </c>
-      <c r="F22" s="13">
+      <c r="E22" s="13">
         <f>LOG(svdStuff!E22*D22)</f>
         <v>5.4584414279787694</v>
       </c>
-      <c r="G22" t="s">
+      <c r="F22" t="s">
         <v>30</v>
       </c>
-      <c r="H22" s="2">
+      <c r="G22" s="2">
         <v>0.41599999999999998</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="L22" s="13">
+      <c r="K22" s="13">
         <f>svdStuff!E22*0.001</f>
         <v>0.186</v>
       </c>
-      <c r="M22" s="13">
+      <c r="L22" s="13">
         <v>0.186</v>
       </c>
-      <c r="N22">
+      <c r="M22">
         <f>LOG10(20720)</f>
         <v>4.3163897510731957</v>
       </c>
+      <c r="N22" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T22" s="1"/>
-      <c r="W22">
+      <c r="S22" s="1"/>
+      <c r="V22">
         <f t="shared" si="0"/>
         <v>3.1080000000000032</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <v>193</v>
       </c>
@@ -3630,55 +3638,55 @@
       <c r="D23">
         <v>1391</v>
       </c>
-      <c r="F23" s="13">
+      <c r="E23" s="13">
         <f>LOG(svdStuff!E23*D23)</f>
         <v>4.9562404866349024</v>
       </c>
-      <c r="G23" t="s">
+      <c r="F23" t="s">
         <v>30</v>
       </c>
-      <c r="H23" s="2">
+      <c r="G23" s="2">
         <v>0.41599999999999998</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
       </c>
       <c r="I23">
         <v>0</v>
       </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="L23" s="13">
+      <c r="K23" s="13">
         <f>svdStuff!E23*0.001</f>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="M23" s="13">
+      <c r="L23" s="13">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="N23">
+      <c r="M23">
         <f>LOG10(16241)</f>
         <v>4.2106127663528978</v>
       </c>
+      <c r="N23" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T23" s="1"/>
-      <c r="W23">
+      <c r="S23" s="1"/>
+      <c r="V23">
         <f t="shared" si="0"/>
         <v>2.4361500000000018</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>162</v>
       </c>
@@ -3688,55 +3696,55 @@
       <c r="D24">
         <v>1077</v>
       </c>
-      <c r="F24" s="13">
+      <c r="E24" s="13">
         <f>LOG(svdStuff!E24*D24)</f>
         <v>4.8955385634184374</v>
       </c>
-      <c r="G24" t="s">
+      <c r="F24" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="2">
+      <c r="G24" s="2">
         <v>0.41599999999999998</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
       </c>
       <c r="I24">
         <v>0</v>
       </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="L24" s="13">
+      <c r="K24" s="13">
         <f>svdStuff!E24*0.001</f>
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="M24" s="13">
+      <c r="L24" s="13">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="N24">
+      <c r="M24">
         <f>LOG10(10072)</f>
         <v>4.0031157170998064</v>
       </c>
+      <c r="N24" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O24" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T24" s="1"/>
-      <c r="W24">
+      <c r="S24" s="1"/>
+      <c r="V24">
         <f t="shared" si="0"/>
         <v>1.5108000000000019</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B25" s="12">
         <v>213</v>
       </c>
@@ -3746,55 +3754,55 @@
       <c r="D25">
         <v>844</v>
       </c>
-      <c r="F25" s="13">
+      <c r="E25" s="13">
         <f>LOG(svdStuff!E25*D25)</f>
         <v>4.7524172493264816</v>
       </c>
-      <c r="G25" t="s">
+      <c r="F25" t="s">
         <v>30</v>
       </c>
-      <c r="H25" s="2">
+      <c r="G25" s="2">
         <v>0.41599999999999998</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="L25" s="13">
+      <c r="K25" s="13">
         <f>svdStuff!E25*0.001</f>
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="M25" s="13">
+      <c r="L25" s="13">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="N25">
+      <c r="M25">
         <f>LOG10(7623)</f>
         <v>3.882125919770032</v>
       </c>
+      <c r="N25" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O25" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T25" s="1"/>
-      <c r="W25">
+      <c r="S25" s="1"/>
+      <c r="V25">
         <f t="shared" si="0"/>
         <v>1.1434500000000012</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>36</v>
       </c>
@@ -3804,64 +3812,64 @@
       <c r="D26">
         <v>375</v>
       </c>
-      <c r="F26" s="13">
+      <c r="E26" s="13">
         <f>LOG(svdStuff!E26*D26)</f>
         <v>3.9542425094393248</v>
       </c>
-      <c r="G26" t="s">
+      <c r="F26" t="s">
         <v>30</v>
       </c>
-      <c r="H26" s="2">
+      <c r="G26" s="2">
         <v>0.41599999999999998</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
       </c>
       <c r="I26">
         <v>0</v>
       </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="L26" s="13">
+      <c r="K26" s="13">
         <f>svdStuff!E26*0.001</f>
         <v>2.4E-2</v>
       </c>
-      <c r="M26" s="13">
+      <c r="L26" s="13">
         <v>2.4E-2</v>
       </c>
-      <c r="N26">
+      <c r="M26">
         <f>LOG10(5757)</f>
         <v>3.7601962294551341</v>
       </c>
+      <c r="N26" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O26" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T26" s="1"/>
-      <c r="W26">
+      <c r="S26" s="1"/>
+      <c r="V26">
         <f t="shared" si="0"/>
         <v>0.86355000000000015</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="O1:S1"/>
+    <mergeCell ref="N1:R1"/>
   </mergeCells>
-  <conditionalFormatting sqref="O3:O16 R3:R16">
+  <conditionalFormatting sqref="N3:N16 Q3:Q16">
     <cfRule type="cellIs" dxfId="33" priority="45" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3884,7 +3892,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:G16 G17:G26 F4:F26">
+  <conditionalFormatting sqref="E3:F16 F17:F26 E4:E26">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -3896,7 +3904,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:J16 I18:J27">
+  <conditionalFormatting sqref="H3:I16 H18:I27">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -3908,7 +3916,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I16 I18:I27">
+  <conditionalFormatting sqref="H3:H16 H18:H27">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -3918,7 +3926,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J16 J18:J27">
+  <conditionalFormatting sqref="I3:I16 I18:I27">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -3928,7 +3936,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L16 N3:N26">
+  <conditionalFormatting sqref="K3:K16 M3:M26">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -3938,12 +3946,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G26">
+  <conditionalFormatting sqref="F3:F26">
     <cfRule type="cellIs" dxfId="30" priority="38" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R17:R26">
+  <conditionalFormatting sqref="Q17:Q26">
     <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3954,7 +3962,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O17:O26">
+  <conditionalFormatting sqref="N17:N26">
     <cfRule type="cellIs" dxfId="26" priority="32" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3965,7 +3973,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:J26">
+  <conditionalFormatting sqref="H3:I26">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -3975,7 +3983,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D26 F3:F26">
+  <conditionalFormatting sqref="D3:E26">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -3987,7 +3995,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L26 N3:N26">
+  <conditionalFormatting sqref="K3:K26 M3:M26">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -3997,7 +4005,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F26">
+  <conditionalFormatting sqref="E3:E26">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -4009,7 +4017,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S16">
+  <conditionalFormatting sqref="R3:R16">
     <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4020,7 +4028,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S17:S26">
+  <conditionalFormatting sqref="R17:R26">
     <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4031,7 +4039,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q16">
+  <conditionalFormatting sqref="P3:P16">
     <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4042,7 +4050,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q17:Q26">
+  <conditionalFormatting sqref="P17:P26">
     <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4053,7 +4061,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N26">
+  <conditionalFormatting sqref="M3:M26">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -4063,7 +4071,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P16">
+  <conditionalFormatting sqref="O3:O16">
     <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4074,7 +4082,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P17:P26">
+  <conditionalFormatting sqref="O17:O26">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4085,7 +4093,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M16">
+  <conditionalFormatting sqref="L3:L16">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -4095,7 +4103,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M26">
+  <conditionalFormatting sqref="L3:L26">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -4105,7 +4113,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T3:T16">
+  <conditionalFormatting sqref="S3:S16">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4116,7 +4124,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T17:T26">
+  <conditionalFormatting sqref="S17:S26">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4136,7 +4144,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4793,7 +4801,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5300,7 +5308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5635,14 +5643,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11FE248-93EC-498A-B149-79239CF2A22B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6891,11 +6899,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE63A85-7D93-4276-809E-D8DD4BB648B4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7921,11 +7929,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABCEEC2-D4D8-41AA-8F98-E40E7997937F}">
-  <dimension ref="A1:N26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7933,7 +7941,7 @@
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -7953,7 +7961,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -7961,7 +7969,7 @@
       <c r="E2" s="16"/>
       <c r="F2" s="26"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -8002,8 +8010,32 @@
       <c r="N3" s="24" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O3" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="P3" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q3" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="R3" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="S3" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="T3" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="U3" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="V3" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -8047,8 +8079,36 @@
         <f t="shared" si="0"/>
         <v>0.61290322580645162</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>24</v>
+      </c>
+      <c r="P4">
+        <v>9</v>
+      </c>
+      <c r="Q4">
+        <v>16</v>
+      </c>
+      <c r="R4">
+        <v>17</v>
+      </c>
+      <c r="S4">
+        <f>O4/$F4</f>
+        <v>0.77419354838709675</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ref="T4:T16" si="1">P4/$F4</f>
+        <v>0.29032258064516131</v>
+      </c>
+      <c r="U4">
+        <f t="shared" ref="U4:U16" si="2">Q4/$F4</f>
+        <v>0.5161290322580645</v>
+      </c>
+      <c r="V4">
+        <f t="shared" ref="V4:V16" si="3">R4/$F4</f>
+        <v>0.54838709677419351</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -8077,7 +8137,7 @@
         <v>31</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5:K16" si="1">G5/$F5</f>
+        <f t="shared" ref="K5:K16" si="4">G5/$F5</f>
         <v>0.8783783783783784</v>
       </c>
       <c r="L5">
@@ -8092,8 +8152,36 @@
         <f t="shared" si="0"/>
         <v>0.41891891891891891</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>20</v>
+      </c>
+      <c r="P5">
+        <v>11</v>
+      </c>
+      <c r="Q5">
+        <v>12</v>
+      </c>
+      <c r="R5">
+        <v>14</v>
+      </c>
+      <c r="S5">
+        <f t="shared" ref="S5:S16" si="5">O5/$F5</f>
+        <v>0.27027027027027029</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="1"/>
+        <v>0.14864864864864866</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="2"/>
+        <v>0.16216216216216217</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="3"/>
+        <v>0.1891891891891892</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -8107,7 +8195,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -8136,7 +8224,7 @@
         <v>76</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.97478991596638653</v>
       </c>
       <c r="L7">
@@ -8151,8 +8239,36 @@
         <f t="shared" si="0"/>
         <v>0.6386554621848739</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>78</v>
+      </c>
+      <c r="P7">
+        <v>28</v>
+      </c>
+      <c r="Q7">
+        <v>35</v>
+      </c>
+      <c r="R7">
+        <v>40</v>
+      </c>
+      <c r="S7">
+        <f t="shared" ref="S7:S16" si="6">O7/$F7</f>
+        <v>0.65546218487394958</v>
+      </c>
+      <c r="T7">
+        <f t="shared" ref="T7:T16" si="7">P7/$F7</f>
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="U7">
+        <f t="shared" ref="U7:U16" si="8">Q7/$F7</f>
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="V7">
+        <f t="shared" ref="V7:V16" si="9">R7/$F7</f>
+        <v>0.33613445378151263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -8181,7 +8297,7 @@
         <v>4760</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.98474576271186443</v>
       </c>
       <c r="L8">
@@ -8196,8 +8312,36 @@
         <f t="shared" si="0"/>
         <v>0.8067796610169492</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>1822</v>
+      </c>
+      <c r="P8">
+        <v>1670</v>
+      </c>
+      <c r="Q8">
+        <v>1789</v>
+      </c>
+      <c r="R8">
+        <v>1799</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="6"/>
+        <v>0.30881355932203391</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="7"/>
+        <v>0.2830508474576271</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="8"/>
+        <v>0.30322033898305084</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="9"/>
+        <v>0.30491525423728816</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -8226,7 +8370,7 @@
         <v>25</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.91803278688524592</v>
       </c>
       <c r="L9">
@@ -8241,8 +8385,36 @@
         <f t="shared" si="0"/>
         <v>0.4098360655737705</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <v>53</v>
+      </c>
+      <c r="P9">
+        <v>9</v>
+      </c>
+      <c r="Q9">
+        <v>18</v>
+      </c>
+      <c r="R9">
+        <v>24</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="6"/>
+        <v>0.86885245901639341</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="7"/>
+        <v>0.14754098360655737</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="8"/>
+        <v>0.29508196721311475</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="9"/>
+        <v>0.39344262295081966</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -8271,7 +8443,7 @@
         <v>444</v>
       </c>
       <c r="K10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.99314128943758573</v>
       </c>
       <c r="L10">
@@ -8286,8 +8458,36 @@
         <f t="shared" si="0"/>
         <v>0.60905349794238683</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O10">
+        <v>516</v>
+      </c>
+      <c r="P10">
+        <v>270</v>
+      </c>
+      <c r="Q10">
+        <v>403</v>
+      </c>
+      <c r="R10">
+        <v>417</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="6"/>
+        <v>0.70781893004115226</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="7"/>
+        <v>0.37037037037037035</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="8"/>
+        <v>0.55281207133058985</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="9"/>
+        <v>0.57201646090534974</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -8319,7 +8519,7 @@
         <v>1928</v>
       </c>
       <c r="K11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.99883132060771329</v>
       </c>
       <c r="L11">
@@ -8334,8 +8534,36 @@
         <f t="shared" si="0"/>
         <v>0.75107128944292945</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O11" s="17">
+        <v>2128</v>
+      </c>
+      <c r="P11" s="17">
+        <v>1515</v>
+      </c>
+      <c r="Q11" s="17">
+        <v>1815</v>
+      </c>
+      <c r="R11" s="17">
+        <v>1855</v>
+      </c>
+      <c r="S11">
+        <f>O11/$F11</f>
+        <v>0.82898324892871056</v>
+      </c>
+      <c r="T11">
+        <f>P11/$F11</f>
+        <v>0.59018309310479156</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="8"/>
+        <v>0.70705103233346323</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="9"/>
+        <v>0.72263342423061938</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -8364,7 +8592,7 @@
         <v>1196</v>
       </c>
       <c r="K12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.70075949367088608</v>
       </c>
       <c r="L12">
@@ -8379,8 +8607,36 @@
         <f t="shared" si="0"/>
         <v>0.60556962025316452</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="17">
+        <v>192</v>
+      </c>
+      <c r="P12" s="17">
+        <v>191</v>
+      </c>
+      <c r="Q12" s="17">
+        <v>191</v>
+      </c>
+      <c r="R12" s="17">
+        <v>191</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="6"/>
+        <v>9.7215189873417721E-2</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="7"/>
+        <v>9.670886075949367E-2</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="8"/>
+        <v>9.670886075949367E-2</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="9"/>
+        <v>9.670886075949367E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -8409,7 +8665,7 @@
         <v>5233</v>
       </c>
       <c r="K13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.97787610619469023</v>
       </c>
       <c r="L13">
@@ -8424,8 +8680,36 @@
         <f t="shared" si="0"/>
         <v>0.82695954487989887</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O13" s="17">
+        <v>1353</v>
+      </c>
+      <c r="P13" s="17">
+        <v>1247</v>
+      </c>
+      <c r="Q13" s="17">
+        <v>1291</v>
+      </c>
+      <c r="R13" s="17">
+        <v>1308</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="6"/>
+        <v>0.21381163084702909</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="7"/>
+        <v>0.1970606826801517</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="8"/>
+        <v>0.20401390644753475</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="9"/>
+        <v>0.20670037926675094</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
@@ -8457,7 +8741,7 @@
         <v>2132</v>
       </c>
       <c r="K14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.99378272251308897</v>
       </c>
       <c r="L14">
@@ -8472,8 +8756,36 @@
         <f t="shared" si="0"/>
         <v>0.69764397905759157</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O14" s="17">
+        <v>2037</v>
+      </c>
+      <c r="P14" s="17">
+        <v>1150</v>
+      </c>
+      <c r="Q14" s="17">
+        <v>1428</v>
+      </c>
+      <c r="R14" s="17">
+        <v>1566</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="6"/>
+        <v>0.66655759162303663</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="7"/>
+        <v>0.3763089005235602</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="8"/>
+        <v>0.46727748691099474</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="9"/>
+        <v>0.51243455497382195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -8502,7 +8814,7 @@
         <v>666</v>
       </c>
       <c r="K15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.99615754082612873</v>
       </c>
       <c r="L15">
@@ -8517,8 +8829,36 @@
         <f t="shared" si="0"/>
         <v>0.63976945244956773</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="17">
+        <v>767</v>
+      </c>
+      <c r="P15" s="17">
+        <v>407</v>
+      </c>
+      <c r="Q15" s="17">
+        <v>528</v>
+      </c>
+      <c r="R15" s="17">
+        <v>570</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="6"/>
+        <v>0.73679154658981749</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="7"/>
+        <v>0.39097022094140249</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="8"/>
+        <v>0.50720461095100866</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="9"/>
+        <v>0.54755043227665701</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>23</v>
       </c>
@@ -8547,7 +8887,7 @@
         <v>1639</v>
       </c>
       <c r="K16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.95274725274725269</v>
       </c>
       <c r="L16">
@@ -8561,6 +8901,34 @@
       <c r="N16">
         <f t="shared" si="0"/>
         <v>0.90054945054945057</v>
+      </c>
+      <c r="O16" s="17">
+        <v>25</v>
+      </c>
+      <c r="P16" s="17">
+        <v>17</v>
+      </c>
+      <c r="Q16" s="17">
+        <v>23</v>
+      </c>
+      <c r="R16" s="17">
+        <v>23</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="6"/>
+        <v>1.3736263736263736E-2</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="7"/>
+        <v>9.3406593406593404E-3</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="8"/>
+        <v>1.2637362637362638E-2</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="9"/>
+        <v>1.2637362637362638E-2</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8709,6 +9077,76 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D16">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D26">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F16 G4:J5 G7:J16">
+    <cfRule type="colorScale" priority="81">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F26 G4:J5 G7:J16">
+    <cfRule type="colorScale" priority="86">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:N16">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P4:R5 P7:R16">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P4:R5 P7:R16">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -8720,8 +9158,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D26">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="S4:V16 T17:V17">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4:O5 O7:O16">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -8732,8 +9180,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:F16 G4:J5 G7:J16">
-    <cfRule type="colorScale" priority="76">
+  <conditionalFormatting sqref="O4:O5 O7:O16">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -8744,28 +9192,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:F26 G4:J5 G7:J16">
-    <cfRule type="colorScale" priority="81">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4:N16">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
A bunch of changes from today. 1. load and voltage limit points chosen and most networks re-run; going to re-run the 24 bus overnight because it is a bit slow. 2. ckt24 and 8500 node updated to include fix annoying bugs 3. Different voltage limits considered for service and primary lines
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DF9788-C7CE-4A51-9D5C-125548EEC975}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
     <sheet name="varStuff" sheetId="6" r:id="rId6"/>
     <sheet name="varV2stuff" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="106">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -345,12 +346,15 @@
   </si>
   <si>
     <t>90%, 99%</t>
+  </si>
+  <si>
+    <t>HC2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -506,7 +510,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -561,6 +565,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -570,7 +577,67 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="3" builtinId="25"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -2218,11 +2285,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2244,12 +2311,12 @@
     <col min="16" max="16" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.42578125" customWidth="1"/>
-    <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="3.42578125" customWidth="1"/>
+    <col min="21" max="21" width="23" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -2289,16 +2356,17 @@
       <c r="M1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
       <c r="S1" s="23"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T1" s="27"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2330,18 +2398,21 @@
       <c r="S2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4" t="s">
+      <c r="T2" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -2398,8 +2469,11 @@
       <c r="S3" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="T3" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -2456,20 +2530,23 @@
       <c r="S4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U4">
+      <c r="T4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V4">
         <f>18/60</f>
         <v>0.3</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <f>(10^M4)*9000*0.000001/60</f>
         <v>0.10545000000000002</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <f>18/60</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -2526,20 +2603,23 @@
       <c r="S5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U5">
+      <c r="T5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V5">
         <f>53.7/60</f>
         <v>0.89500000000000002</v>
       </c>
-      <c r="V5">
-        <f t="shared" ref="V5:V26" si="0">(10^M5)*9000*0.000001/60</f>
+      <c r="W5">
+        <f t="shared" ref="W5:W26" si="0">(10^M5)*9000*0.000001/60</f>
         <v>0.60000000000000098</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <f>19/60</f>
         <v>0.31666666666666665</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -2596,12 +2676,15 @@
       <c r="S6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V6">
+      <c r="T6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W6">
         <f t="shared" si="0"/>
         <v>0.43605000000000016</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -2658,20 +2741,23 @@
       <c r="S7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U7">
+      <c r="T7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V7">
         <f>72/60</f>
         <v>1.2</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <f t="shared" si="0"/>
         <v>0.74475000000000013</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <f>33/60</f>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -2728,16 +2814,17 @@
       <c r="S8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="V8">
+      <c r="T8" s="1"/>
+      <c r="W8">
         <f t="shared" si="0"/>
         <v>41.364450000000069</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <f>958/60</f>
         <v>15.966666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -2794,16 +2881,19 @@
       <c r="S9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="V9">
+      <c r="T9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W9">
         <f t="shared" si="0"/>
         <v>0.77160000000000128</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <f>59/60</f>
         <v>0.98333333333333328</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -2857,16 +2947,19 @@
       <c r="S10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V10">
+      <c r="T10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W10">
         <f t="shared" si="0"/>
         <v>1.8091500000000034</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <f>145/60</f>
         <v>2.4166666666666665</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -2926,20 +3019,23 @@
       <c r="S11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="U11">
+      <c r="T11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="V11">
         <f>637/60</f>
         <v>10.616666666666667</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <f t="shared" si="0"/>
         <v>4.8481500000000013</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <f>371/60</f>
         <v>6.1833333333333336</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -2996,22 +3092,25 @@
       <c r="S12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U12" t="s">
         <v>78</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>90</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <f t="shared" si="0"/>
         <v>2.6175000000000002</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <f>367/60</f>
         <v>6.1166666666666663</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -3068,19 +3167,20 @@
       <c r="S13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U13" t="s">
+      <c r="T13" s="1"/>
+      <c r="V13" t="s">
         <v>89</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <f t="shared" si="0"/>
         <v>13.193250000000001</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <f>1996/60</f>
         <v>33.266666666666666</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
@@ -3138,19 +3238,20 @@
       <c r="S14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="T14" t="s">
+      <c r="T14" s="8"/>
+      <c r="U14" t="s">
         <v>62</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <f t="shared" si="0"/>
         <v>3.9418500000000019</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <f>551/60</f>
         <v>9.1833333333333336</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -3204,16 +3305,17 @@
       <c r="S15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="V15">
+      <c r="T15" s="1"/>
+      <c r="W15">
         <f t="shared" si="0"/>
         <v>3.0229500000000038</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <f>107/60</f>
         <v>1.7833333333333334</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>23</v>
       </c>
@@ -3267,16 +3369,17 @@
       <c r="S16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="V16">
+      <c r="T16" s="1"/>
+      <c r="W16">
         <f t="shared" si="0"/>
         <v>4.1532000000000036</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <f>445/60</f>
         <v>7.416666666666667</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>93</v>
       </c>
@@ -3333,12 +3436,13 @@
         <v>26</v>
       </c>
       <c r="S17" s="8"/>
-      <c r="V17">
+      <c r="T17" s="8"/>
+      <c r="W17">
         <f t="shared" si="0"/>
         <v>1.5582000000000018</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>39</v>
       </c>
@@ -3391,12 +3495,13 @@
         <v>26</v>
       </c>
       <c r="S18" s="1"/>
-      <c r="V18">
+      <c r="T18" s="1"/>
+      <c r="W18">
         <f t="shared" si="0"/>
         <v>3.7098000000000053</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>40</v>
       </c>
@@ -3449,12 +3554,13 @@
         <v>26</v>
       </c>
       <c r="S19" s="1"/>
-      <c r="V19">
+      <c r="T19" s="1"/>
+      <c r="W19">
         <f t="shared" si="0"/>
         <v>3.6646500000000035</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>36</v>
       </c>
@@ -3507,12 +3613,13 @@
         <v>26</v>
       </c>
       <c r="S20" s="1"/>
-      <c r="V20">
+      <c r="T20" s="1"/>
+      <c r="W20">
         <f t="shared" si="0"/>
         <v>1.0159500000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>34</v>
       </c>
@@ -3565,12 +3672,13 @@
         <v>26</v>
       </c>
       <c r="S21" s="1"/>
-      <c r="V21">
+      <c r="T21" s="1"/>
+      <c r="W21">
         <f t="shared" si="0"/>
         <v>3.9414000000000047</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>35</v>
       </c>
@@ -3623,12 +3731,13 @@
         <v>26</v>
       </c>
       <c r="S22" s="1"/>
-      <c r="V22">
+      <c r="T22" s="1"/>
+      <c r="W22">
         <f t="shared" si="0"/>
         <v>3.1080000000000032</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <v>193</v>
       </c>
@@ -3681,12 +3790,13 @@
         <v>26</v>
       </c>
       <c r="S23" s="1"/>
-      <c r="V23">
+      <c r="T23" s="1"/>
+      <c r="W23">
         <f t="shared" si="0"/>
         <v>2.4361500000000018</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>162</v>
       </c>
@@ -3739,12 +3849,13 @@
         <v>26</v>
       </c>
       <c r="S24" s="1"/>
-      <c r="V24">
+      <c r="T24" s="1"/>
+      <c r="W24">
         <f t="shared" si="0"/>
         <v>1.5108000000000019</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B25" s="12">
         <v>213</v>
       </c>
@@ -3797,12 +3908,13 @@
         <v>26</v>
       </c>
       <c r="S25" s="1"/>
-      <c r="V25">
+      <c r="T25" s="1"/>
+      <c r="W25">
         <f t="shared" si="0"/>
         <v>1.1434500000000012</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>36</v>
       </c>
@@ -3855,12 +3967,13 @@
         <v>26</v>
       </c>
       <c r="S26" s="1"/>
-      <c r="V26">
+      <c r="T26" s="1"/>
+      <c r="W26">
         <f t="shared" si="0"/>
         <v>0.86355000000000015</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -3870,18 +3983,18 @@
     <mergeCell ref="N1:R1"/>
   </mergeCells>
   <conditionalFormatting sqref="N3:N16 Q3:Q16">
-    <cfRule type="cellIs" dxfId="33" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="51" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="52" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="53" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D16">
-    <cfRule type="colorScale" priority="44">
+    <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3893,7 +4006,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:F16 F17:F26 E4:E26">
-    <cfRule type="colorScale" priority="43">
+    <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3905,7 +4018,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:I16 H18:I27">
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3917,7 +4030,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H16 H18:H27">
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3927,7 +4040,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I16 I18:I27">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3937,7 +4050,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K16 M3:M26">
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3947,34 +4060,34 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F26">
-    <cfRule type="cellIs" dxfId="30" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="44" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Q26">
-    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="42" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="43" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17:N26">
-    <cfRule type="cellIs" dxfId="26" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="38" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="39" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="40" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:I26">
-    <cfRule type="colorScale" priority="31">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3984,7 +4097,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E26">
-    <cfRule type="colorScale" priority="30">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3996,7 +4109,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K26 M3:M26">
-    <cfRule type="colorScale" priority="29">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4006,7 +4119,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E26">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4018,6 +4131,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R16">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R17:R26">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P16">
     <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4028,7 +4163,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R17:R26">
+  <conditionalFormatting sqref="P17:P26">
     <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4039,30 +4174,8 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P16">
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P17:P26">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="M3:M26">
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4072,29 +4185,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O16">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="20" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17:O26">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L16">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4104,7 +4217,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L26">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4114,6 +4227,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:S16">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S17:S26">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T3:T16">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4124,7 +4259,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S17:S26">
+  <conditionalFormatting sqref="T17:T26">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4144,7 +4279,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4801,11 +4936,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5308,7 +5443,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5643,14 +5778,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="D11" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6899,7 +7034,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7929,10 +8064,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
@@ -8096,15 +8231,15 @@
         <v>0.77419354838709675</v>
       </c>
       <c r="T4">
-        <f t="shared" ref="T4:T16" si="1">P4/$F4</f>
+        <f t="shared" ref="T4:T5" si="1">P4/$F4</f>
         <v>0.29032258064516131</v>
       </c>
       <c r="U4">
-        <f t="shared" ref="U4:U16" si="2">Q4/$F4</f>
+        <f t="shared" ref="U4:U5" si="2">Q4/$F4</f>
         <v>0.5161290322580645</v>
       </c>
       <c r="V4">
-        <f t="shared" ref="V4:V16" si="3">R4/$F4</f>
+        <f t="shared" ref="V4:V5" si="3">R4/$F4</f>
         <v>0.54838709677419351</v>
       </c>
     </row>
@@ -8165,7 +8300,7 @@
         <v>14</v>
       </c>
       <c r="S5">
-        <f t="shared" ref="S5:S16" si="5">O5/$F5</f>
+        <f t="shared" ref="S5" si="5">O5/$F5</f>
         <v>0.27027027027027029</v>
       </c>
       <c r="T5">

</xml_diff>

<commit_message>
Changes: - now am able to include regulators and sources (with/without regs) in plot figures for all circuit except 8500 node/ckt 24 - changed back to using all buses (from 'KtotCheck') and instead taking out zero covariance values where necessary
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DF9788-C7CE-4A51-9D5C-125548EEC975}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
-    <sheet name="sourceParams" sheetId="3" r:id="rId2"/>
-    <sheet name="plotTts" sheetId="2" r:id="rId3"/>
-    <sheet name="notes" sheetId="4" r:id="rId4"/>
-    <sheet name="svdStuff" sheetId="5" r:id="rId5"/>
-    <sheet name="varStuff" sheetId="6" r:id="rId6"/>
-    <sheet name="varV2stuff" sheetId="7" r:id="rId7"/>
+    <sheet name="plotting" sheetId="8" r:id="rId2"/>
+    <sheet name="sourceParams" sheetId="3" r:id="rId3"/>
+    <sheet name="plotTts" sheetId="2" r:id="rId4"/>
+    <sheet name="notes" sheetId="4" r:id="rId5"/>
+    <sheet name="svdStuff" sheetId="5" r:id="rId6"/>
+    <sheet name="varStuff" sheetId="6" r:id="rId7"/>
+    <sheet name="varV2stuff" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="115">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -349,12 +349,39 @@
   </si>
   <si>
     <t>HC2</t>
+  </si>
+  <si>
+    <t>Regulators</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>BUS ID</t>
+  </si>
+  <si>
+    <t>SRC Reg</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>SouthEast</t>
+  </si>
+  <si>
+    <t>NorthEast</t>
+  </si>
+  <si>
+    <t>NorthWest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1194,6 +1221,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1311,6 +1339,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2285,11 +2314,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4279,7 +4308,178 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9">
+        <v>318412</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>5964927408</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4935,8 +5135,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5442,12 +5642,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G26"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5455,9 +5655,10 @@
     <col min="3" max="3" width="5.28515625" customWidth="1"/>
     <col min="4" max="4" width="65.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -5473,13 +5674,16 @@
       <c r="G1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -5490,7 +5694,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -5500,8 +5704,11 @@
       <c r="F4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -5511,8 +5718,11 @@
       <c r="F5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -5520,7 +5730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -5533,8 +5743,11 @@
       <c r="G7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -5551,15 +5764,18 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -5567,7 +5783,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -5589,8 +5805,11 @@
       <c r="G11" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -5609,8 +5828,11 @@
       <c r="G12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -5630,7 +5852,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
@@ -5652,8 +5874,11 @@
       <c r="G14" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -5672,8 +5897,11 @@
       <c r="G15" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>23</v>
       </c>
@@ -5691,6 +5919,9 @@
       </c>
       <c r="G16" t="s">
         <v>76</v>
+      </c>
+      <c r="J16" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5778,14 +6009,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7033,12 +7264,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8063,8 +8294,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
A few odds and sods - chooseLinPoint plot made a bit more properly - better timing system added for measuring - a few plotting functions tweaked
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -1221,7 +1221,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1339,7 +1338,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4309,18 +4307,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F13"/>
+  <dimension ref="A2:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>107</v>
       </c>
@@ -4333,8 +4332,11 @@
       <c r="F2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -4347,8 +4349,11 @@
       <c r="D3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -4358,8 +4363,11 @@
       <c r="D4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -4372,13 +4380,16 @@
       <c r="F5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -4391,8 +4402,11 @@
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -4408,8 +4422,11 @@
       <c r="E8">
         <v>796</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -4422,13 +4439,16 @@
       <c r="E9">
         <v>318412</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
@@ -4444,8 +4464,11 @@
       <c r="E11">
         <v>5964927408</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>22</v>
       </c>
@@ -4458,8 +4481,11 @@
       <c r="F12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>23</v>
       </c>
@@ -4471,6 +4497,9 @@
       </c>
       <c r="F13" t="s">
         <v>30</v>
+      </c>
+      <c r="G13" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -5644,10 +5673,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J1:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5658,7 +5687,7 @@
     <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -5674,16 +5703,13 @@
       <c r="G1" t="s">
         <v>77</v>
       </c>
-      <c r="J1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -5694,7 +5720,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -5704,11 +5730,8 @@
       <c r="F4" t="s">
         <v>30</v>
       </c>
-      <c r="J4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -5718,11 +5741,8 @@
       <c r="F5" t="s">
         <v>30</v>
       </c>
-      <c r="J5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -5730,7 +5750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -5743,11 +5763,8 @@
       <c r="G7" t="s">
         <v>75</v>
       </c>
-      <c r="J7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -5764,18 +5781,15 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="J9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -5783,7 +5797,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -5805,11 +5819,8 @@
       <c r="G11" t="s">
         <v>76</v>
       </c>
-      <c r="J11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -5828,11 +5839,8 @@
       <c r="G12" t="s">
         <v>75</v>
       </c>
-      <c r="J12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -5852,7 +5860,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
@@ -5874,11 +5882,8 @@
       <c r="G14" t="s">
         <v>76</v>
       </c>
-      <c r="J14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -5897,11 +5902,8 @@
       <c r="G15" t="s">
         <v>76</v>
       </c>
-      <c r="J15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>23</v>
       </c>
@@ -5919,9 +5921,6 @@
       </c>
       <c r="G16" t="s">
         <v>76</v>
-      </c>
-      <c r="J16" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Plotting now works with all 11x feeders (no uslv).
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="115">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -2315,8 +2315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4309,8 +4309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4388,6 +4388,18 @@
       <c r="B6" t="s">
         <v>17</v>
       </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -4446,6 +4458,9 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
A number of changes: - plotting has been made much faster by plotting everything in one call to plt and using 'LineCollection' object (or something) - secondary buses can now be plotted using the 'augmented' buscoords set - tidied up linearise_manc so that it doesn't always rerun the bit where it finds the buses - still working through linSvdCalcs; can not plot the number of standard deviations from a node to the limit.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="115">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -604,7 +604,404 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="3" builtinId="25"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="80">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -2313,10 +2710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X29"/>
+  <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,26 +2721,27 @@
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
-    <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="3.42578125" customWidth="1"/>
-    <col min="21" max="21" width="23" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="3.42578125" customWidth="1"/>
+    <col min="22" max="22" width="23" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -2354,46 +2752,49 @@
         <v>47</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="O1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="28"/>
       <c r="P1" s="28"/>
       <c r="Q1" s="28"/>
       <c r="R1" s="28"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="27"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S1" s="28"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="27"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2406,40 +2807,41 @@
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" s="16"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="4" t="s">
+      <c r="M2" s="16"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="4"/>
+      <c r="W2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -2450,36 +2852,36 @@
         <v>61</v>
       </c>
       <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
         <v>4</v>
       </c>
-      <c r="E3" s="6">
-        <f>LOG(svdStuff!E3*D3)</f>
+      <c r="F3" s="6">
+        <f>LOG(svdStuff!E3*E3)</f>
         <v>0.6020599913279624</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
+      <c r="H3" s="7"/>
       <c r="I3" s="6">
         <v>0</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="K3" s="6">
-        <v>5.4</v>
       </c>
       <c r="L3" s="6">
         <v>5.4</v>
       </c>
-      <c r="M3" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>27</v>
+      <c r="M3" s="6">
+        <v>5.4</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>26</v>
       </c>
       <c r="O3" s="8" t="s">
         <v>27</v>
@@ -2499,8 +2901,11 @@
       <c r="T3" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="U3" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -2508,40 +2913,40 @@
         <v>5</v>
       </c>
       <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4">
         <v>16</v>
       </c>
-      <c r="E4" s="13">
-        <f>LOG(svdStuff!E4*D4)</f>
+      <c r="F4" s="13">
+        <f>LOG(svdStuff!E4*E4)</f>
         <v>2.3802112417116059</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>4.16</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1.5</v>
-      </c>
-      <c r="K4">
-        <v>3.6</v>
       </c>
       <c r="L4">
         <v>3.6</v>
       </c>
       <c r="M4">
+        <v>3.6</v>
+      </c>
+      <c r="N4">
         <f>LOG10(703)</f>
         <v>2.8469553250198238</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O4" s="1" t="s">
         <v>26</v>
       </c>
@@ -2560,20 +2965,23 @@
       <c r="T4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="V4">
+      <c r="U4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4">
         <f>18/60</f>
         <v>0.3</v>
       </c>
-      <c r="W4">
-        <f>(10^M4)*9000*0.000001/60</f>
+      <c r="X4">
+        <f>(10^N4)*9000*0.000001/60</f>
         <v>0.10545000000000002</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <f>18/60</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -2581,40 +2989,40 @@
         <v>6</v>
       </c>
       <c r="D5">
+        <v>68</v>
+      </c>
+      <c r="E5">
         <v>37</v>
       </c>
-      <c r="E5" s="13">
-        <f>LOG(svdStuff!E5*D5)</f>
+      <c r="F5" s="13">
+        <f>LOG(svdStuff!E5*E5)</f>
         <v>3.4007106367732312</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>24.9</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
       </c>
       <c r="I5">
         <v>2</v>
       </c>
       <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
         <v>50</v>
-      </c>
-      <c r="K5">
-        <v>2</v>
       </c>
       <c r="L5">
         <v>2</v>
       </c>
       <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
         <f>LOG10(4000)</f>
         <v>3.6020599913279625</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O5" s="1" t="s">
         <v>26</v>
       </c>
@@ -2633,20 +3041,23 @@
       <c r="T5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="V5">
+      <c r="U5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W5">
         <f>53.7/60</f>
         <v>0.89500000000000002</v>
       </c>
-      <c r="W5">
-        <f t="shared" ref="W5:W26" si="0">(10^M5)*9000*0.000001/60</f>
+      <c r="X5">
+        <f t="shared" ref="X5:X26" si="0">(10^N5)*9000*0.000001/60</f>
         <v>0.60000000000000098</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <f>19/60</f>
         <v>0.31666666666666665</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -2654,45 +3065,45 @@
         <v>7</v>
       </c>
       <c r="D6">
+        <v>30</v>
+      </c>
+      <c r="E6">
         <v>39</v>
       </c>
-      <c r="E6" s="13">
-        <f>LOG(svdStuff!E6*D6)</f>
+      <c r="F6" s="13">
+        <f>LOG(svdStuff!E6*E6)</f>
         <v>3.0681858617461617</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>4.8</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>1</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>3</v>
-      </c>
-      <c r="K6">
-        <v>2.6</v>
       </c>
       <c r="L6">
         <v>2.6</v>
       </c>
       <c r="M6">
+        <v>2.6</v>
+      </c>
+      <c r="N6">
         <f>LOG10(2907)</f>
         <v>3.4634450317704277</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="P6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>27</v>
@@ -2706,12 +3117,15 @@
       <c r="T6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="W6">
+      <c r="U6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X6">
         <f t="shared" si="0"/>
         <v>0.43605000000000016</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -2719,43 +3133,43 @@
         <v>8</v>
       </c>
       <c r="D7">
+        <v>92</v>
+      </c>
+      <c r="E7">
         <v>132</v>
       </c>
-      <c r="E7" s="13">
-        <f>LOG(svdStuff!E7*D7)</f>
+      <c r="F7" s="13">
+        <f>LOG(svdStuff!E7*E7)</f>
         <v>4.0843617585514052</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>2.4</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>4</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>3</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>6</v>
-      </c>
-      <c r="K7">
-        <v>3.6</v>
       </c>
       <c r="L7">
         <v>3.6</v>
       </c>
       <c r="M7">
+        <v>3.6</v>
+      </c>
+      <c r="N7">
         <f>LOG10(4965)</f>
         <v>3.6959192528313998</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="P7" s="1" t="s">
         <v>26</v>
       </c>
@@ -2771,20 +3185,23 @@
       <c r="T7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="V7">
+      <c r="U7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W7">
         <f>72/60</f>
         <v>1.2</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <f t="shared" si="0"/>
         <v>0.74475000000000013</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <f>33/60</f>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -2792,66 +3209,69 @@
         <v>9</v>
       </c>
       <c r="D8">
+        <v>2355</v>
+      </c>
+      <c r="E8">
         <v>4876</v>
       </c>
-      <c r="E8" s="13">
-        <f>LOG(svdStuff!E8*D8)</f>
+      <c r="F8" s="13">
+        <f>LOG(svdStuff!E8*E8)</f>
         <v>7.0600546084112592</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>7.2</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>4</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>12</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>17</v>
-      </c>
-      <c r="K8">
-        <v>12.05</v>
       </c>
       <c r="L8">
         <v>12.05</v>
       </c>
       <c r="M8">
+        <v>12.05</v>
+      </c>
+      <c r="N8">
         <f>LOG10(275763)</f>
         <v>5.4405359950748213</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="P8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="Q8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="R8" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="S8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="1"/>
-      <c r="W8">
+      <c r="T8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" s="1"/>
+      <c r="X8">
         <f t="shared" si="0"/>
         <v>41.364450000000069</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <f>958/60</f>
         <v>15.966666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -2859,51 +3279,51 @@
         <v>0</v>
       </c>
       <c r="D9">
+        <v>55</v>
+      </c>
+      <c r="E9">
         <v>907</v>
       </c>
-      <c r="E9" s="13">
-        <f>LOG(svdStuff!E9*D9)</f>
+      <c r="F9" s="13">
+        <f>LOG(svdStuff!E9*E9)</f>
         <v>4.6979699765543392</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>0.41599999999999998</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
         <v>0.3</v>
-      </c>
-      <c r="K9">
-        <v>5.5E-2</v>
       </c>
       <c r="L9">
         <v>5.5E-2</v>
       </c>
       <c r="M9">
+        <v>5.5E-2</v>
+      </c>
+      <c r="N9">
         <f>LOG10(5144)</f>
         <v>3.7113009599161657</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S9" s="1" t="s">
         <v>26</v>
@@ -2911,16 +3331,19 @@
       <c r="T9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W9">
+      <c r="U9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X9">
         <f t="shared" si="0"/>
         <v>0.77160000000000128</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <f>59/60</f>
         <v>0.98333333333333328</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -2928,65 +3351,68 @@
         <v>14</v>
       </c>
       <c r="D10">
+        <v>624</v>
+      </c>
+      <c r="E10">
         <v>390</v>
       </c>
-      <c r="E10" s="13">
-        <f>LOG(svdStuff!E10*D10)</f>
+      <c r="F10" s="13">
+        <f>LOG(svdStuff!E10*E10)</f>
         <v>5.4324240774813539</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>13.8</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
-      <c r="K10">
-        <v>42.8</v>
+      <c r="J10">
+        <v>0</v>
       </c>
       <c r="L10">
         <v>42.8</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10">
+        <v>42.8</v>
+      </c>
+      <c r="N10" s="15">
         <f>LOG10(12061)</f>
         <v>4.0813833174622856</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="T10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W10">
+      <c r="U10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X10">
         <f t="shared" si="0"/>
         <v>1.8091500000000034</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <f>145/60</f>
         <v>2.4166666666666665</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -2997,51 +3423,51 @@
         <v>17</v>
       </c>
       <c r="D11" s="6">
+        <v>1379</v>
+      </c>
+      <c r="E11" s="6">
         <v>2998</v>
       </c>
-      <c r="E11" s="6">
-        <f>LOG(svdStuff!E11*D11)</f>
+      <c r="F11" s="6">
+        <f>LOG(svdStuff!E11*E11)</f>
         <v>6.6163958946881101</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="7">
+      <c r="H11" s="7">
         <v>12.47</v>
       </c>
-      <c r="H11" s="6">
+      <c r="I11" s="6">
         <v>4</v>
       </c>
-      <c r="I11" s="6">
+      <c r="J11" s="6">
         <v>0</v>
       </c>
-      <c r="J11" s="6">
+      <c r="K11" s="6">
         <v>5</v>
-      </c>
-      <c r="K11" s="6">
-        <v>16.3</v>
       </c>
       <c r="L11" s="6">
         <v>16.3</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="6">
+        <v>16.3</v>
+      </c>
+      <c r="N11">
         <f>LOG10(32321)</f>
         <v>4.50948478922394</v>
       </c>
-      <c r="N11" s="8" t="s">
+      <c r="O11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O11" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="P11" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q11" s="8" t="s">
         <v>27</v>
       </c>
       <c r="R11" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S11" s="8" t="s">
         <v>26</v>
@@ -3049,20 +3475,23 @@
       <c r="T11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="V11">
+      <c r="U11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="W11">
         <f>637/60</f>
         <v>10.616666666666667</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <f t="shared" si="0"/>
         <v>4.8481500000000013</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <f>371/60</f>
         <v>6.1833333333333336</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -3070,51 +3499,51 @@
         <v>18</v>
       </c>
       <c r="D12">
+        <v>868</v>
+      </c>
+      <c r="E12">
         <v>1255</v>
       </c>
-      <c r="E12" s="13">
-        <f>LOG(svdStuff!E12*D12)</f>
+      <c r="F12" s="13">
+        <f>LOG(svdStuff!E12*E12)</f>
         <v>6.0371634509935488</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>12.47</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>2</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>4</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>78</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>19.3</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <f>LOG10(17450)</f>
         <v>4.2417954312951984</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S12" s="1" t="s">
         <v>26</v>
@@ -3122,22 +3551,25 @@
       <c r="T12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U12" t="s">
+      <c r="U12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V12" t="s">
         <v>78</v>
       </c>
-      <c r="V12" t="s">
+      <c r="W12" t="s">
         <v>90</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <f t="shared" si="0"/>
         <v>2.6175000000000002</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <f>367/60</f>
         <v>6.1166666666666663</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -3145,40 +3577,40 @@
         <v>22</v>
       </c>
       <c r="D13">
+        <v>3891</v>
+      </c>
+      <c r="E13">
         <v>6058</v>
       </c>
-      <c r="E13" s="13">
-        <f>LOG(svdStuff!E13*D13)</f>
+      <c r="F13" s="13">
+        <f>LOG(svdStuff!E13*E13)</f>
         <v>7.3723904998005798</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>34.5</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>3</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>1</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>10</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>52.2</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>69.400000000000006</v>
       </c>
-      <c r="M13" s="15">
+      <c r="N13" s="15">
         <f>LOG10(87955)</f>
         <v>4.9442605329428515</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O13" s="1" t="s">
         <v>26</v>
       </c>
@@ -3186,28 +3618,31 @@
         <v>26</v>
       </c>
       <c r="Q13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="R13" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="S13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T13" s="1"/>
-      <c r="V13" t="s">
+      <c r="T13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U13" s="1"/>
+      <c r="W13" t="s">
         <v>89</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <f t="shared" si="0"/>
         <v>13.193250000000001</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <f>1996/60</f>
         <v>33.266666666666666</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
@@ -3218,38 +3653,38 @@
         <v>19</v>
       </c>
       <c r="D14" s="6">
+        <v>1384</v>
+      </c>
+      <c r="E14" s="6">
         <v>4888</v>
       </c>
-      <c r="E14" s="6">
-        <f>LOG(svdStuff!E14*D14)</f>
+      <c r="F14" s="6">
+        <f>LOG(svdStuff!E14*E14)</f>
         <v>6.8302672873552366</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="7">
+      <c r="H14" s="7">
         <v>12.47</v>
       </c>
-      <c r="H14" s="6">
+      <c r="I14" s="6">
         <v>5</v>
       </c>
-      <c r="I14" s="6">
+      <c r="J14" s="6">
         <v>9</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6">
-        <v>11.6</v>
-      </c>
+      <c r="K14" s="6"/>
       <c r="L14" s="6">
         <v>11.6</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="6">
+        <v>11.6</v>
+      </c>
+      <c r="N14">
         <f>LOG10(26279)</f>
         <v>4.4196088349081029</v>
       </c>
-      <c r="N14" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="O14" s="8" t="s">
         <v>26</v>
       </c>
@@ -3257,28 +3692,31 @@
         <v>26</v>
       </c>
       <c r="Q14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="R14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="R14" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="S14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="T14" s="8"/>
-      <c r="U14" t="s">
+      <c r="T14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="U14" s="8"/>
+      <c r="V14" t="s">
         <v>62</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <f t="shared" si="0"/>
         <v>3.9418500000000019</v>
       </c>
-      <c r="X14">
+      <c r="Y14">
         <f>551/60</f>
         <v>9.1833333333333336</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -3286,37 +3724,37 @@
         <v>20</v>
       </c>
       <c r="D15">
+        <v>332</v>
+      </c>
+      <c r="E15">
         <v>1282</v>
       </c>
-      <c r="E15" s="13">
-        <f>LOG(svdStuff!E15*D15)</f>
+      <c r="F15" s="13">
+        <f>LOG(svdStuff!E15*E15)</f>
         <v>5.6290261088868352</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>13.2</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
-      <c r="K15">
-        <v>12.74</v>
+      <c r="J15">
+        <v>1</v>
       </c>
       <c r="L15">
         <v>12.74</v>
       </c>
       <c r="M15">
+        <v>12.74</v>
+      </c>
+      <c r="N15">
         <f>LOG10(20153)</f>
         <v>4.3043397048923389</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O15" s="1" t="s">
         <v>26</v>
       </c>
@@ -3332,17 +3770,20 @@
       <c r="S15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T15" s="1"/>
-      <c r="W15">
+      <c r="T15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U15" s="1"/>
+      <c r="X15">
         <f t="shared" si="0"/>
         <v>3.0229500000000038</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <f>107/60</f>
         <v>1.7833333333333334</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>23</v>
       </c>
@@ -3350,37 +3791,37 @@
         <v>21</v>
       </c>
       <c r="D16">
+        <v>1470</v>
+      </c>
+      <c r="E16">
         <v>2596</v>
       </c>
-      <c r="E16" s="13">
-        <f>LOG(svdStuff!E16*D16)</f>
+      <c r="F16" s="13">
+        <f>LOG(svdStuff!E16*E16)</f>
         <v>6.5816220228765081</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>12.47</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>3</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>1</v>
-      </c>
-      <c r="K16">
-        <v>15.67</v>
       </c>
       <c r="L16">
         <v>15.67</v>
       </c>
-      <c r="M16" s="15">
+      <c r="M16">
+        <v>15.67</v>
+      </c>
+      <c r="N16" s="15">
         <f>LOG10(27688)</f>
         <v>4.4422915862860712</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O16" s="1" t="s">
         <v>26</v>
       </c>
@@ -3388,25 +3829,28 @@
         <v>26</v>
       </c>
       <c r="Q16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="R16" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="S16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T16" s="1"/>
-      <c r="W16">
+      <c r="T16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U16" s="1"/>
+      <c r="X16">
         <f t="shared" si="0"/>
         <v>4.1532000000000036</v>
       </c>
-      <c r="X16">
+      <c r="Y16">
         <f>445/60</f>
         <v>7.416666666666667</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>93</v>
       </c>
@@ -3417,59 +3861,62 @@
         <v>61</v>
       </c>
       <c r="D17" s="6">
+        <v>55</v>
+      </c>
+      <c r="E17" s="6">
         <v>907</v>
       </c>
-      <c r="E17" s="6">
-        <f>LOG(svdStuff!E17*D17)</f>
+      <c r="F17" s="6">
+        <f>LOG(svdStuff!E17*E17)</f>
         <v>4.6979699765543392</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="7">
+      <c r="H17" s="7">
         <v>0.41599999999999998</v>
-      </c>
-      <c r="H17" s="6">
-        <v>0</v>
       </c>
       <c r="I17" s="6">
         <v>0</v>
       </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6">
+      <c r="J17" s="6">
+        <v>0</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6">
         <f>svdStuff!E17*0.001</f>
         <v>5.5E-2</v>
       </c>
-      <c r="L17" s="6">
+      <c r="M17" s="6">
         <v>5.5E-2</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <f>LOG10(10388)</f>
         <v>4.0165319409572655</v>
       </c>
-      <c r="N17" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="O17" s="8" t="s">
         <v>26</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q17" s="8" t="s">
         <v>27</v>
       </c>
       <c r="R17" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="S17" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="S17" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="T17" s="8"/>
-      <c r="W17">
+      <c r="U17" s="8"/>
+      <c r="X17">
         <f t="shared" si="0"/>
         <v>1.5582000000000018</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>39</v>
       </c>
@@ -3477,58 +3924,61 @@
         <v>61</v>
       </c>
       <c r="D18">
+        <v>175</v>
+      </c>
+      <c r="E18">
         <v>2287</v>
       </c>
-      <c r="E18" s="13">
-        <f>LOG(svdStuff!E18*D18)</f>
+      <c r="F18" s="13">
+        <f>LOG(svdStuff!E18*E18)</f>
         <v>5.602304213293043</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>0.41599999999999998</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
-      <c r="K18" s="13">
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="L18" s="13">
         <f>svdStuff!E18*0.001</f>
         <v>0.17500000000000002</v>
       </c>
-      <c r="L18" s="13">
+      <c r="M18" s="13">
         <v>0.17500000000000002</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <f>LOG10(24732)</f>
         <v>4.3932592378268378</v>
       </c>
-      <c r="N18" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S18" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="T18" s="1"/>
-      <c r="W18">
+      <c r="U18" s="1"/>
+      <c r="X18">
         <f t="shared" si="0"/>
         <v>3.7098000000000053</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>40</v>
       </c>
@@ -3536,58 +3986,61 @@
         <v>61</v>
       </c>
       <c r="D19">
+        <v>94</v>
+      </c>
+      <c r="E19">
         <v>1304</v>
       </c>
-      <c r="E19" s="13">
-        <f>LOG(svdStuff!E19*D19)</f>
+      <c r="F19" s="13">
+        <f>LOG(svdStuff!E19*E19)</f>
         <v>5.0884054449956002</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>0.41599999999999998</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
-      <c r="K19" s="13">
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="L19" s="13">
         <f>svdStuff!E19*0.001</f>
         <v>9.4E-2</v>
       </c>
-      <c r="L19" s="13">
+      <c r="M19" s="13">
         <v>9.4E-2</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <f>LOG10(24431)</f>
         <v>4.3879412437066989</v>
       </c>
-      <c r="N19" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O19" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S19" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="T19" s="1"/>
-      <c r="W19">
+      <c r="U19" s="1"/>
+      <c r="X19">
         <f t="shared" si="0"/>
         <v>3.6646500000000035</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>36</v>
       </c>
@@ -3595,58 +4048,61 @@
         <v>61</v>
       </c>
       <c r="D20">
+        <v>24</v>
+      </c>
+      <c r="E20">
         <v>375</v>
       </c>
-      <c r="E20" s="13">
-        <f>LOG(svdStuff!E20*D20)</f>
+      <c r="F20" s="13">
+        <f>LOG(svdStuff!E20*E20)</f>
         <v>3.9542425094393248</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <v>0.41599999999999998</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
-      <c r="K20" s="13">
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="L20" s="13">
         <f>svdStuff!E20*0.001</f>
         <v>2.4E-2</v>
       </c>
-      <c r="L20" s="13">
+      <c r="M20" s="13">
         <v>2.4E-2</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <f>LOG10(6773)</f>
         <v>3.8307810756063612</v>
       </c>
-      <c r="N20" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O20" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S20" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="T20" s="1"/>
-      <c r="W20">
+      <c r="U20" s="1"/>
+      <c r="X20">
         <f t="shared" si="0"/>
         <v>1.0159500000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>34</v>
       </c>
@@ -3654,58 +4110,61 @@
         <v>61</v>
       </c>
       <c r="D21">
+        <v>115</v>
+      </c>
+      <c r="E21">
         <v>1605</v>
       </c>
-      <c r="E21" s="13">
-        <f>LOG(svdStuff!E21*D21)</f>
+      <c r="F21" s="13">
+        <f>LOG(svdStuff!E21*E21)</f>
         <v>5.2661728770945029</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H21" s="2">
         <v>0.41599999999999998</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
       </c>
       <c r="I21">
         <v>0</v>
       </c>
-      <c r="K21" s="13">
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="L21" s="13">
         <f>svdStuff!E21*0.001</f>
         <v>0.115</v>
       </c>
-      <c r="L21" s="13">
+      <c r="M21" s="13">
         <v>0.115</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <f>LOG10(26276)</f>
         <v>4.4195592531957208</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O21" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S21" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="T21" s="1"/>
-      <c r="W21">
+      <c r="U21" s="1"/>
+      <c r="X21">
         <f t="shared" si="0"/>
         <v>3.9414000000000047</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>35</v>
       </c>
@@ -3713,58 +4172,61 @@
         <v>61</v>
       </c>
       <c r="D22">
+        <v>186</v>
+      </c>
+      <c r="E22">
         <v>1545</v>
       </c>
-      <c r="E22" s="13">
-        <f>LOG(svdStuff!E22*D22)</f>
+      <c r="F22" s="13">
+        <f>LOG(svdStuff!E22*E22)</f>
         <v>5.4584414279787694</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <v>0.41599999999999998</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
-      <c r="K22" s="13">
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="L22" s="13">
         <f>svdStuff!E22*0.001</f>
         <v>0.186</v>
       </c>
-      <c r="L22" s="13">
+      <c r="M22" s="13">
         <v>0.186</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <f>LOG10(20720)</f>
         <v>4.3163897510731957</v>
       </c>
-      <c r="N22" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S22" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="T22" s="1"/>
-      <c r="W22">
+      <c r="U22" s="1"/>
+      <c r="X22">
         <f t="shared" si="0"/>
         <v>3.1080000000000032</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <v>193</v>
       </c>
@@ -3772,58 +4234,61 @@
         <v>61</v>
       </c>
       <c r="D23">
+        <v>65</v>
+      </c>
+      <c r="E23">
         <v>1391</v>
       </c>
-      <c r="E23" s="13">
-        <f>LOG(svdStuff!E23*D23)</f>
+      <c r="F23" s="13">
+        <f>LOG(svdStuff!E23*E23)</f>
         <v>4.9562404866349024</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>0.41599999999999998</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
       </c>
       <c r="I23">
         <v>0</v>
       </c>
-      <c r="K23" s="13">
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="L23" s="13">
         <f>svdStuff!E23*0.001</f>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="L23" s="13">
+      <c r="M23" s="13">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <f>LOG10(16241)</f>
         <v>4.2106127663528978</v>
       </c>
-      <c r="N23" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S23" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="T23" s="1"/>
-      <c r="W23">
+      <c r="U23" s="1"/>
+      <c r="X23">
         <f t="shared" si="0"/>
         <v>2.4361500000000018</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>162</v>
       </c>
@@ -3831,58 +4296,61 @@
         <v>61</v>
       </c>
       <c r="D24">
+        <v>73</v>
+      </c>
+      <c r="E24">
         <v>1077</v>
       </c>
-      <c r="E24" s="13">
-        <f>LOG(svdStuff!E24*D24)</f>
+      <c r="F24" s="13">
+        <f>LOG(svdStuff!E24*E24)</f>
         <v>4.8955385634184374</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>30</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>0.41599999999999998</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
       </c>
       <c r="I24">
         <v>0</v>
       </c>
-      <c r="K24" s="13">
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="L24" s="13">
         <f>svdStuff!E24*0.001</f>
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="L24" s="13">
+      <c r="M24" s="13">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <f>LOG10(10072)</f>
         <v>4.0031157170998064</v>
       </c>
-      <c r="N24" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O24" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S24" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="T24" s="1"/>
-      <c r="W24">
+      <c r="U24" s="1"/>
+      <c r="X24">
         <f t="shared" si="0"/>
         <v>1.5108000000000019</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B25" s="12">
         <v>213</v>
       </c>
@@ -3890,58 +4358,61 @@
         <v>61</v>
       </c>
       <c r="D25">
+        <v>67</v>
+      </c>
+      <c r="E25">
         <v>844</v>
       </c>
-      <c r="E25" s="13">
-        <f>LOG(svdStuff!E25*D25)</f>
+      <c r="F25" s="13">
+        <f>LOG(svdStuff!E25*E25)</f>
         <v>4.7524172493264816</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>30</v>
       </c>
-      <c r="G25" s="2">
+      <c r="H25" s="2">
         <v>0.41599999999999998</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
-      <c r="K25" s="13">
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="L25" s="13">
         <f>svdStuff!E25*0.001</f>
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="L25" s="13">
+      <c r="M25" s="13">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <f>LOG10(7623)</f>
         <v>3.882125919770032</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O25" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S25" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="T25" s="1"/>
-      <c r="W25">
+      <c r="U25" s="1"/>
+      <c r="X25">
         <f t="shared" si="0"/>
         <v>1.1434500000000012</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>36</v>
       </c>
@@ -3949,79 +4420,82 @@
         <v>61</v>
       </c>
       <c r="D26">
+        <v>24</v>
+      </c>
+      <c r="E26">
         <v>375</v>
       </c>
-      <c r="E26" s="13">
-        <f>LOG(svdStuff!E26*D26)</f>
+      <c r="F26" s="13">
+        <f>LOG(svdStuff!E26*E26)</f>
         <v>3.9542425094393248</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>30</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>0.41599999999999998</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
       </c>
       <c r="I26">
         <v>0</v>
       </c>
-      <c r="K26" s="13">
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="L26" s="13">
         <f>svdStuff!E26*0.001</f>
         <v>2.4E-2</v>
       </c>
-      <c r="L26" s="13">
+      <c r="M26" s="13">
         <v>2.4E-2</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <f>LOG10(5757)</f>
         <v>3.7601962294551341</v>
       </c>
-      <c r="N26" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O26" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S26" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="T26" s="1"/>
-      <c r="W26">
+      <c r="U26" s="1"/>
+      <c r="X26">
         <f t="shared" si="0"/>
         <v>0.86355000000000015</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="O1:S1"/>
   </mergeCells>
-  <conditionalFormatting sqref="N3:N16 Q3:Q16">
-    <cfRule type="cellIs" dxfId="39" priority="51" operator="equal">
+  <conditionalFormatting sqref="O3:O16 R3:R16">
+    <cfRule type="cellIs" dxfId="39" priority="54" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="55" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="56" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D16">
-    <cfRule type="colorScale" priority="50">
+  <conditionalFormatting sqref="E3:E16">
+    <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4032,8 +4506,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:F16 F17:F26 E4:E26">
-    <cfRule type="colorScale" priority="49">
+  <conditionalFormatting sqref="F3:G16 G17:G26 F4:F26">
+    <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4044,8 +4518,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:I16 H18:I27">
-    <cfRule type="colorScale" priority="48">
+  <conditionalFormatting sqref="I3:J16 I18:J27">
+    <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4056,8 +4530,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H16 H18:H27">
-    <cfRule type="colorScale" priority="47">
+  <conditionalFormatting sqref="I3:I16 I18:I27">
+    <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4066,8 +4540,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I16 I18:I27">
-    <cfRule type="colorScale" priority="46">
+  <conditionalFormatting sqref="J3:J16 J18:J27">
+    <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4076,8 +4550,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K16 M3:M26">
-    <cfRule type="colorScale" priority="45">
+  <conditionalFormatting sqref="L3:L16 N3:N26">
+    <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4086,35 +4560,35 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F26">
-    <cfRule type="cellIs" dxfId="36" priority="44" operator="equal">
+  <conditionalFormatting sqref="G3:G26">
+    <cfRule type="cellIs" dxfId="36" priority="47" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q17:Q26">
-    <cfRule type="cellIs" dxfId="35" priority="41" operator="equal">
+  <conditionalFormatting sqref="R17:R26">
+    <cfRule type="cellIs" dxfId="35" priority="44" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="45" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N17:N26">
-    <cfRule type="cellIs" dxfId="32" priority="38" operator="equal">
+  <conditionalFormatting sqref="O17:O26">
+    <cfRule type="cellIs" dxfId="32" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="42" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="43" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:I26">
-    <cfRule type="colorScale" priority="37">
+  <conditionalFormatting sqref="I3:J26">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4123,8 +4597,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:E26">
-    <cfRule type="colorScale" priority="36">
+  <conditionalFormatting sqref="E3:F26">
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4135,8 +4609,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K26 M3:M26">
-    <cfRule type="colorScale" priority="35">
+  <conditionalFormatting sqref="L3:L26 N3:N26">
+    <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4145,8 +4619,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E26">
-    <cfRule type="colorScale" priority="34">
+  <conditionalFormatting sqref="F3:F26">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4157,52 +4631,52 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3:R16">
-    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
+  <conditionalFormatting sqref="S3:S16">
+    <cfRule type="cellIs" dxfId="29" priority="34" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="35" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="36" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R17:R26">
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+  <conditionalFormatting sqref="S17:S26">
+    <cfRule type="cellIs" dxfId="26" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="32" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="33" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P16">
-    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
+  <conditionalFormatting sqref="Q3:Q16">
+    <cfRule type="cellIs" dxfId="23" priority="28" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="29" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="30" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P17:P26">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+  <conditionalFormatting sqref="Q17:Q26">
+    <cfRule type="cellIs" dxfId="20" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="27" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M26">
-    <cfRule type="colorScale" priority="21">
+  <conditionalFormatting sqref="N3:N26">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4211,30 +4685,30 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O16">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+  <conditionalFormatting sqref="P3:P16">
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="22" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="23" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O17:O26">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+  <conditionalFormatting sqref="P17:P26">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="20" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L16">
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="M3:M16">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4243,8 +4717,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L26">
-    <cfRule type="colorScale" priority="13">
+  <conditionalFormatting sqref="M3:M26">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4253,48 +4727,72 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S16">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+  <conditionalFormatting sqref="T3:T16">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S17:S26">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T3:T16">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T17:T26">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
       <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U3:U16">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U17:U26">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D16">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D26">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5691,7 +6189,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J1:J17"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6034,7 +6532,7 @@
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
A lot of exploring to investigate how the problem is working out and to try and get some better (?) analyses running that follows the literature a bit better. Main takeaway: - The california set does not work well for some of the networks. Therefore, proposed half-double sets for analysis to make the results a bit more interesting. Saved as a nice pickle file. - Also some updating of the scripts to make it run more easily with the gammaFrac MC analysis. Next step: get this up and running to see how the result come out.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5B37E0-DF7A-4BC9-826B-39A7978D8838}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -15,8 +16,9 @@
     <sheet name="svdStuff" sheetId="5" r:id="rId6"/>
     <sheet name="varStuff" sheetId="6" r:id="rId7"/>
     <sheet name="varV2stuff" sheetId="7" r:id="rId8"/>
+    <sheet name="quarterGenQuarterMax" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="136">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -376,12 +378,75 @@
   </si>
   <si>
     <t>NorthWest</t>
+  </si>
+  <si>
+    <t>theta</t>
+  </si>
+  <si>
+    <t>vp_pct(0.25)</t>
+  </si>
+  <si>
+    <t>mean(loads(loads&lt;100kW))</t>
+  </si>
+  <si>
+    <t>std(loads(loads&lt;100kW))</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>th</t>
+  </si>
+  <si>
+    <t>mu</t>
+  </si>
+  <si>
+    <t>sgm</t>
+  </si>
+  <si>
+    <t>Location?</t>
+  </si>
+  <si>
+    <t>NorthEast US</t>
+  </si>
+  <si>
+    <t>southeastern US</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>HC 5%</t>
+  </si>
+  <si>
+    <t>HC 75%</t>
+  </si>
+  <si>
+    <t>HC 5% new</t>
+  </si>
+  <si>
+    <t>HC 75% new</t>
+  </si>
+  <si>
+    <t>RULE</t>
+  </si>
+  <si>
+    <t>if HC 75% &lt; 10% -&gt; 0.5</t>
+  </si>
+  <si>
+    <t>if HC 5% &gt; 90% -&gt; 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -604,404 +669,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="3" builtinId="25"/>
   </cellStyles>
-  <dxfs count="80">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="40">
     <dxf>
       <font>
         <color auto="1"/>
@@ -2709,11 +2377,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2731,7 +2399,7 @@
     <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.140625" customWidth="1"/>
     <col min="16" max="16" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
@@ -4804,7 +4472,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5021,7 +4689,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5678,7 +5346,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6185,11 +5853,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6197,10 +5865,11 @@
     <col min="3" max="3" width="5.28515625" customWidth="1"/>
     <col min="4" max="4" width="65.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -6216,13 +5885,16 @@
       <c r="G1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -6233,7 +5905,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -6244,7 +5916,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -6255,7 +5927,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -6263,7 +5935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -6277,7 +5949,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -6294,7 +5966,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -6302,7 +5974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -6310,7 +5982,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -6332,8 +6004,11 @@
       <c r="G11" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -6352,8 +6027,11 @@
       <c r="G12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -6372,8 +6050,11 @@
       <c r="G13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
@@ -6395,8 +6076,11 @@
       <c r="G14" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -6415,8 +6099,11 @@
       <c r="G15" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>23</v>
       </c>
@@ -6434,6 +6121,9 @@
       </c>
       <c r="G16" t="s">
         <v>76</v>
+      </c>
+      <c r="H16" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6521,14 +6211,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="D11" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7777,7 +7467,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8807,11 +8497,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+      <selection activeCell="C8" activeCellId="1" sqref="A11:C16 A8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10072,4 +9762,556 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD199016-BA05-4465-A2F6-D08DD3A5E39B}">
+  <dimension ref="B2:P26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>122</v>
+      </c>
+      <c r="K2" t="s">
+        <v>123</v>
+      </c>
+      <c r="M2" t="s">
+        <v>120</v>
+      </c>
+      <c r="N2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>119</v>
+      </c>
+      <c r="J3">
+        <f>M3*N3</f>
+        <v>10.25</v>
+      </c>
+      <c r="K3">
+        <f>SQRT(M3)*N3</f>
+        <v>5.0621141828291458</v>
+      </c>
+      <c r="M3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H6" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" t="s">
+        <v>117</v>
+      </c>
+      <c r="K6" t="s">
+        <v>118</v>
+      </c>
+      <c r="M6" t="s">
+        <v>120</v>
+      </c>
+      <c r="N6" t="s">
+        <v>121</v>
+      </c>
+      <c r="P6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="G7">
+        <v>0.21</v>
+      </c>
+      <c r="H7">
+        <v>33.33</v>
+      </c>
+      <c r="J7">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="K7">
+        <v>1.86</v>
+      </c>
+      <c r="L7">
+        <f>K7/SQRT(2)</f>
+        <v>1.3152186130069783</v>
+      </c>
+      <c r="M7">
+        <f>(J7/L7)^2</f>
+        <v>3.0052029136316341</v>
+      </c>
+      <c r="N7">
+        <f>J7/M7</f>
+        <v>0.75868421052631563</v>
+      </c>
+      <c r="P7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="6">
+        <v>17</v>
+      </c>
+      <c r="G8">
+        <v>0.35</v>
+      </c>
+      <c r="H8">
+        <v>27</v>
+      </c>
+      <c r="J8">
+        <v>2.57</v>
+      </c>
+      <c r="K8">
+        <v>1.58</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ref="L8:L13" si="0">K8/SQRT(2)</f>
+        <v>1.117228714274745</v>
+      </c>
+      <c r="M8">
+        <f t="shared" ref="M8:M13" si="1">(J8/L8)^2</f>
+        <v>5.2915398173369654</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ref="N8:N13" si="2">J8/M8</f>
+        <v>0.48568093385214001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="17">
+        <v>18</v>
+      </c>
+      <c r="G9">
+        <v>0.34</v>
+      </c>
+      <c r="H9">
+        <v>23.3</v>
+      </c>
+      <c r="J9">
+        <v>2.48</v>
+      </c>
+      <c r="K9">
+        <v>3.01</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>2.1283914113715077</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>1.3576892087283809</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="2"/>
+        <v>1.8266330645161284</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <v>22</v>
+      </c>
+      <c r="G10">
+        <v>1.08</v>
+      </c>
+      <c r="H10">
+        <v>24</v>
+      </c>
+      <c r="J10">
+        <v>2.65</v>
+      </c>
+      <c r="K10">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>1.7748380207782339</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>2.2293296931794737</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="2"/>
+        <v>1.1886981132075469</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="6">
+        <v>19</v>
+      </c>
+      <c r="G11">
+        <v>0.17</v>
+      </c>
+      <c r="H11">
+        <v>25</v>
+      </c>
+      <c r="J11">
+        <v>1.71</v>
+      </c>
+      <c r="K11">
+        <v>1.68</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>1.1879393923933996</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>2.0720663265306127</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="2"/>
+        <v>0.82526315789473659</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>2.35</v>
+      </c>
+      <c r="H12">
+        <v>22.3</v>
+      </c>
+      <c r="J12">
+        <v>6.08</v>
+      </c>
+      <c r="K12">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>3.0829855659733472</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>3.889234912886121</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="2"/>
+        <v>1.5632894736842105</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13">
+        <v>21</v>
+      </c>
+      <c r="G13">
+        <v>1.5</v>
+      </c>
+      <c r="H13">
+        <v>24.3</v>
+      </c>
+      <c r="J13">
+        <v>1.94</v>
+      </c>
+      <c r="K13">
+        <v>1.5</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>1.0606601717798212</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>3.345422222222223</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="2"/>
+        <v>0.57989690721649467</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>129</v>
+      </c>
+      <c r="F14" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" t="s">
+        <v>131</v>
+      </c>
+      <c r="I14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>27</v>
+      </c>
+      <c r="F16">
+        <v>100</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="J17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <v>100</v>
+      </c>
+      <c r="F18">
+        <v>100</v>
+      </c>
+      <c r="G18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>93</v>
+      </c>
+      <c r="F19">
+        <v>100</v>
+      </c>
+      <c r="G19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20">
+        <v>14</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>6.6</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="6">
+        <v>17</v>
+      </c>
+      <c r="E21">
+        <v>100</v>
+      </c>
+      <c r="F21">
+        <v>100</v>
+      </c>
+      <c r="G21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="17">
+        <v>18</v>
+      </c>
+      <c r="E22">
+        <v>100</v>
+      </c>
+      <c r="F22">
+        <v>100</v>
+      </c>
+      <c r="G22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23">
+        <v>22</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>100</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="6">
+        <v>19</v>
+      </c>
+      <c r="E24">
+        <v>100</v>
+      </c>
+      <c r="F24">
+        <v>100</v>
+      </c>
+      <c r="G24">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25">
+        <v>20</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26">
+        <v>21</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>100</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tidied up the code and now have a bunch more examples working; still just trying to find a way to look at the matrices to decide a sensible regulator setpoint.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465E4DF5-4219-48F9-A43C-0A3D13BAB60C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
     <sheet name="notes" sheetId="4" r:id="rId2"/>
     <sheet name="caps" sheetId="11" r:id="rId3"/>
     <sheet name="regs" sheetId="12" r:id="rId4"/>
-    <sheet name="legacy&gt;&gt;&gt;" sheetId="10" r:id="rId5"/>
-    <sheet name="plotting" sheetId="8" r:id="rId6"/>
-    <sheet name="sourceParams" sheetId="3" r:id="rId7"/>
-    <sheet name="plotTts" sheetId="2" r:id="rId8"/>
-    <sheet name="svdStuff" sheetId="5" r:id="rId9"/>
-    <sheet name="varStuff" sheetId="6" r:id="rId10"/>
-    <sheet name="varV2stuff" sheetId="7" r:id="rId11"/>
-    <sheet name="quarterGenQuarterMax" sheetId="9" r:id="rId12"/>
+    <sheet name="workflow" sheetId="13" r:id="rId5"/>
+    <sheet name="legacy&gt;&gt;&gt;" sheetId="10" r:id="rId6"/>
+    <sheet name="plotting" sheetId="8" r:id="rId7"/>
+    <sheet name="sourceParams" sheetId="3" r:id="rId8"/>
+    <sheet name="plotTts" sheetId="2" r:id="rId9"/>
+    <sheet name="svdStuff" sheetId="5" r:id="rId10"/>
+    <sheet name="varStuff" sheetId="6" r:id="rId11"/>
+    <sheet name="varV2stuff" sheetId="7" r:id="rId12"/>
+    <sheet name="quarterGenQuarterMax" sheetId="9" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="184">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -549,13 +549,52 @@
   </si>
   <si>
     <t>R/X!=0 (?)</t>
+  </si>
+  <si>
+    <t>linearise_manc_py</t>
+  </si>
+  <si>
+    <t>if reg &gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>if ldc &gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>linHcCalcs</t>
+  </si>
+  <si>
+    <t>choose_lin_point</t>
+  </si>
+  <si>
+    <t>linSvdCalcs_run</t>
+  </si>
+  <si>
+    <t>linearise_regs</t>
+  </si>
+  <si>
+    <t>&lt;&lt;&lt;</t>
+  </si>
+  <si>
+    <t>vvv</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>fixed_voltage_testing</t>
+  </si>
+  <si>
+    <t>ltc_voltage_testing</t>
+  </si>
+  <si>
+    <t>Class: linSvdCalcs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,6 +629,15 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -710,7 +758,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -768,6 +816,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -1450,14 +1501,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:J16"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36:H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3548,7 +3599,1256 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="3.85546875" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="R1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="26"/>
+      <c r="H2" s="24">
+        <v>0.95</v>
+      </c>
+      <c r="I2" s="24">
+        <v>0.98</v>
+      </c>
+      <c r="J2" s="24">
+        <v>0.99</v>
+      </c>
+      <c r="K2" s="25">
+        <v>0.995</v>
+      </c>
+      <c r="L2" s="24">
+        <v>0.99900000000000011</v>
+      </c>
+      <c r="M2" s="24">
+        <v>0.95</v>
+      </c>
+      <c r="N2" s="24">
+        <v>0.98</v>
+      </c>
+      <c r="O2" s="24">
+        <v>0.99</v>
+      </c>
+      <c r="P2" s="25">
+        <v>0.995</v>
+      </c>
+      <c r="Q2" s="24">
+        <v>0.99900000000000011</v>
+      </c>
+      <c r="R2" s="24">
+        <v>0.95</v>
+      </c>
+      <c r="S2" s="24">
+        <v>0.98</v>
+      </c>
+      <c r="T2" s="24">
+        <v>0.99</v>
+      </c>
+      <c r="U2" s="25">
+        <v>0.995</v>
+      </c>
+      <c r="V2" s="24">
+        <v>0.99900000000000011</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>31</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <f>H4/$E4</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:Q16" si="0">I4/$E4</f>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="R4">
+        <f>MIN((H4*($F4+$E4))/($E4*$F4),1)</f>
+        <v>0.19784946236559139</v>
+      </c>
+      <c r="S4">
+        <f t="shared" ref="S4:V4" si="1">MIN((I4*($F4+$E4))/($E4*$F4),1)</f>
+        <v>0.39569892473118279</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="1"/>
+        <v>0.59354838709677415</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="1"/>
+        <v>0.79139784946236558</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="1"/>
+        <v>0.989247311827957</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>37</v>
+      </c>
+      <c r="E5">
+        <v>68</v>
+      </c>
+      <c r="F5">
+        <v>74</v>
+      </c>
+      <c r="H5">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>13</v>
+      </c>
+      <c r="J5">
+        <v>13</v>
+      </c>
+      <c r="K5">
+        <v>13</v>
+      </c>
+      <c r="L5">
+        <v>15</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M16" si="2">H5/$E5</f>
+        <v>0.17647058823529413</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>0.19117647058823528</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>0.19117647058823528</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>0.19117647058823528</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>0.22058823529411764</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5:R16" si="3">MIN((H5*($F5+$E5))/($E5*$F5),1)</f>
+        <v>0.33863275039745627</v>
+      </c>
+      <c r="S5">
+        <f t="shared" ref="S5:S16" si="4">MIN((I5*($F5+$E5))/($E5*$F5),1)</f>
+        <v>0.36685214626391099</v>
+      </c>
+      <c r="T5">
+        <f t="shared" ref="T5:T16" si="5">MIN((J5*($F5+$E5))/($E5*$F5),1)</f>
+        <v>0.36685214626391099</v>
+      </c>
+      <c r="U5">
+        <f t="shared" ref="U5:U16" si="6">MIN((K5*($F5+$E5))/($E5*$F5),1)</f>
+        <v>0.36685214626391099</v>
+      </c>
+      <c r="V5">
+        <f t="shared" ref="V5:V16" si="7">MIN((L5*($F5+$E5))/($E5*$F5),1)</f>
+        <v>0.42329093799682033</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>39</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R6" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S6" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T6" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U6" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V6" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>132</v>
+      </c>
+      <c r="E7">
+        <v>92</v>
+      </c>
+      <c r="F7">
+        <v>119</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>15</v>
+      </c>
+      <c r="K7">
+        <v>21</v>
+      </c>
+      <c r="L7">
+        <v>35</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>5.434782608695652E-2</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>0.10869565217391304</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>0.16304347826086957</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>0.22826086956521738</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>0.38043478260869568</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="3"/>
+        <v>9.6364632809645592E-2</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="4"/>
+        <v>0.19272926561929118</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="5"/>
+        <v>0.28909389842893679</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="6"/>
+        <v>0.40473145780051151</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="7"/>
+        <v>0.67455242966751916</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>4876</v>
+      </c>
+      <c r="E8">
+        <v>2355</v>
+      </c>
+      <c r="F8">
+        <v>5900</v>
+      </c>
+      <c r="G8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8">
+        <v>1214</v>
+      </c>
+      <c r="I8">
+        <v>1504</v>
+      </c>
+      <c r="J8">
+        <v>1676</v>
+      </c>
+      <c r="K8">
+        <v>1811</v>
+      </c>
+      <c r="L8">
+        <v>2034</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>0.51549893842887473</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0.63864118895966027</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>0.71167728237791927</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>0.76900212314225058</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>0.8636942675159236</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="3"/>
+        <v>0.72126165029328149</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="4"/>
+        <v>0.89355644319694838</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="5"/>
+        <v>0.99574507898808884</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>907</v>
+      </c>
+      <c r="E9">
+        <v>55</v>
+      </c>
+      <c r="F9">
+        <v>61</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>6</v>
+      </c>
+      <c r="K9">
+        <v>9</v>
+      </c>
+      <c r="L9">
+        <v>21</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>5.4545454545454543E-2</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>7.2727272727272724E-2</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>0.10909090909090909</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>0.16363636363636364</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>0.38181818181818183</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="3"/>
+        <v>0.10372578241430701</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="4"/>
+        <v>0.13830104321907602</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="5"/>
+        <v>0.20745156482861402</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="6"/>
+        <v>0.31117734724292101</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="7"/>
+        <v>0.72608047690014899</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>390</v>
+      </c>
+      <c r="E10">
+        <v>694</v>
+      </c>
+      <c r="F10">
+        <v>729</v>
+      </c>
+      <c r="H10">
+        <v>102</v>
+      </c>
+      <c r="I10">
+        <v>146</v>
+      </c>
+      <c r="J10">
+        <v>176</v>
+      </c>
+      <c r="K10">
+        <v>204</v>
+      </c>
+      <c r="L10">
+        <v>272</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>0.14697406340057637</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>0.21037463976945245</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>0.25360230547550433</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>0.29394812680115273</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>0.39193083573487031</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="3"/>
+        <v>0.2868917588738274</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="4"/>
+        <v>0.410648988191949</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="5"/>
+        <v>0.49502891727248649</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="6"/>
+        <v>0.57378351774765479</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="7"/>
+        <v>0.76504469033020639</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6">
+        <v>17</v>
+      </c>
+      <c r="D11" s="6">
+        <v>2998</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1379</v>
+      </c>
+      <c r="F11" s="17">
+        <v>2567</v>
+      </c>
+      <c r="H11">
+        <v>588</v>
+      </c>
+      <c r="I11">
+        <v>872</v>
+      </c>
+      <c r="J11">
+        <v>1031</v>
+      </c>
+      <c r="K11">
+        <v>1147</v>
+      </c>
+      <c r="L11">
+        <v>1299</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>0.42639593908629442</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>0.63234227701232781</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>0.74764321972443804</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>0.83176214648295865</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>0.94198694706308916</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="3"/>
+        <v>0.65545709997449075</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="4"/>
+        <v>0.97203842037033328</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="17">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>1255</v>
+      </c>
+      <c r="E12">
+        <v>868</v>
+      </c>
+      <c r="F12" s="17">
+        <v>1975</v>
+      </c>
+      <c r="H12">
+        <v>103</v>
+      </c>
+      <c r="I12">
+        <v>172</v>
+      </c>
+      <c r="J12">
+        <v>259</v>
+      </c>
+      <c r="K12">
+        <v>385</v>
+      </c>
+      <c r="L12">
+        <v>779</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>0.11866359447004608</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>0.19815668202764977</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>0.29838709677419356</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>0.44354838709677419</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>0.89746543778801846</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="3"/>
+        <v>0.17081549320422329</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="4"/>
+        <v>0.2852452896225865</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="5"/>
+        <v>0.42952633728052264</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="6"/>
+        <v>0.63848509595753367</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>22</v>
+      </c>
+      <c r="D13">
+        <v>6058</v>
+      </c>
+      <c r="E13">
+        <v>3891</v>
+      </c>
+      <c r="F13" s="17">
+        <v>6328</v>
+      </c>
+      <c r="G13" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13">
+        <v>1028</v>
+      </c>
+      <c r="I13">
+        <v>1681</v>
+      </c>
+      <c r="J13">
+        <v>2231</v>
+      </c>
+      <c r="K13">
+        <v>2743</v>
+      </c>
+      <c r="L13" t="s">
+        <v>94</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="2"/>
+        <v>0.26419943459264972</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>0.43202261629401184</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>0.57337445386790031</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>0.70496016448213827</v>
+      </c>
+      <c r="Q13" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="3"/>
+        <v>0.42665202624878118</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="4"/>
+        <v>0.69766736977062371</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="5"/>
+        <v>0.92593450443680037</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V13" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="6">
+        <v>19</v>
+      </c>
+      <c r="D14" s="6">
+        <v>4888</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1384</v>
+      </c>
+      <c r="F14" s="17">
+        <v>3056</v>
+      </c>
+      <c r="H14">
+        <v>667</v>
+      </c>
+      <c r="I14">
+        <v>774</v>
+      </c>
+      <c r="J14">
+        <v>841</v>
+      </c>
+      <c r="K14">
+        <v>929</v>
+      </c>
+      <c r="L14">
+        <v>1144</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>0.48193641618497107</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0.55924855491329484</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>0.60765895953757221</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>0.67124277456647397</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>0.82658959537572252</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="3"/>
+        <v>0.70019557848863601</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="4"/>
+        <v>0.81252080622219536</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="5"/>
+        <v>0.88285529461610623</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="6"/>
+        <v>0.97523492116333266</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>1282</v>
+      </c>
+      <c r="E15">
+        <v>332</v>
+      </c>
+      <c r="F15" s="17">
+        <v>1041</v>
+      </c>
+      <c r="H15">
+        <v>226</v>
+      </c>
+      <c r="I15">
+        <v>261</v>
+      </c>
+      <c r="J15">
+        <v>277</v>
+      </c>
+      <c r="K15">
+        <v>290</v>
+      </c>
+      <c r="L15">
+        <v>308</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>0.68072289156626509</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>0.78614457831325302</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>0.83433734939759041</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>0.87349397590361444</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>0.92771084337349397</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="3"/>
+        <v>0.89782183488999223</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>21</v>
+      </c>
+      <c r="D16">
+        <v>2596</v>
+      </c>
+      <c r="E16">
+        <v>1470</v>
+      </c>
+      <c r="F16" s="17">
+        <v>1820</v>
+      </c>
+      <c r="H16">
+        <v>314</v>
+      </c>
+      <c r="I16">
+        <v>512</v>
+      </c>
+      <c r="J16">
+        <v>781</v>
+      </c>
+      <c r="K16">
+        <v>1037</v>
+      </c>
+      <c r="L16">
+        <v>1328</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>0.21360544217687075</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>0.34829931972789113</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>0.53129251700680269</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="0"/>
+        <v>0.70544217687074828</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>0.90340136054421771</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="3"/>
+        <v>0.3861329147043433</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="4"/>
+        <v>0.62961800104657251</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="5"/>
+        <v>0.96041339612768184</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="6">
+        <v>907</v>
+      </c>
+      <c r="E17" s="6">
+        <v>55</v>
+      </c>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18">
+        <v>2287</v>
+      </c>
+      <c r="E18">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19">
+        <v>1304</v>
+      </c>
+      <c r="E19">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20">
+        <v>375</v>
+      </c>
+      <c r="E20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21">
+        <v>1605</v>
+      </c>
+      <c r="E21">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22">
+        <v>1545</v>
+      </c>
+      <c r="E22">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="12">
+        <v>193</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23">
+        <v>1391</v>
+      </c>
+      <c r="E23">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="12">
+        <v>162</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24">
+        <v>1077</v>
+      </c>
+      <c r="E24">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="12">
+        <v>213</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25">
+        <v>844</v>
+      </c>
+      <c r="E25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26">
+        <v>375</v>
+      </c>
+      <c r="E26">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D3:D16">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D26">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F16">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F26">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4:V16">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4577,8 +5877,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5845,8 +7145,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD199016-BA05-4465-A2F6-D08DD3A5E39B}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6383,7 +7683,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -6744,14 +8044,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="D11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABF17D4-E643-4BD4-AE01-D544E53B2465}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7063,11 +8366,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8249C74E-FD9B-413A-8E0E-85E5AD777A3D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7231,6 +8537,9 @@
       <c r="J5" t="s">
         <v>26</v>
       </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -7403,6 +8712,9 @@
         <v>61</v>
       </c>
       <c r="J11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" t="s">
         <v>26</v>
       </c>
     </row>
@@ -7510,7 +8822,107 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F4EC55F-D879-4D6C-A0F2-C3D481B14807}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="F3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" t="s">
+        <v>179</v>
+      </c>
+      <c r="G4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -7526,8 +8938,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="2"/>
   </sheetPr>
@@ -7746,8 +9158,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8403,8 +9815,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8907,1253 +10319,4 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:V26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="3.85546875" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="R1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="26"/>
-      <c r="H2" s="24">
-        <v>0.95</v>
-      </c>
-      <c r="I2" s="24">
-        <v>0.98</v>
-      </c>
-      <c r="J2" s="24">
-        <v>0.99</v>
-      </c>
-      <c r="K2" s="25">
-        <v>0.995</v>
-      </c>
-      <c r="L2" s="24">
-        <v>0.99900000000000011</v>
-      </c>
-      <c r="M2" s="24">
-        <v>0.95</v>
-      </c>
-      <c r="N2" s="24">
-        <v>0.98</v>
-      </c>
-      <c r="O2" s="24">
-        <v>0.99</v>
-      </c>
-      <c r="P2" s="25">
-        <v>0.995</v>
-      </c>
-      <c r="Q2" s="24">
-        <v>0.99900000000000011</v>
-      </c>
-      <c r="R2" s="24">
-        <v>0.95</v>
-      </c>
-      <c r="S2" s="24">
-        <v>0.98</v>
-      </c>
-      <c r="T2" s="24">
-        <v>0.99</v>
-      </c>
-      <c r="U2" s="25">
-        <v>0.995</v>
-      </c>
-      <c r="V2" s="24">
-        <v>0.99900000000000011</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="6">
-        <v>4</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="F3" s="13"/>
-    </row>
-    <row r="4" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>16</v>
-      </c>
-      <c r="E4">
-        <v>15</v>
-      </c>
-      <c r="F4">
-        <v>31</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-      <c r="J4">
-        <v>6</v>
-      </c>
-      <c r="K4">
-        <v>8</v>
-      </c>
-      <c r="L4">
-        <v>10</v>
-      </c>
-      <c r="M4">
-        <f>H4/$E4</f>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="N4">
-        <f t="shared" ref="N4:Q16" si="0">I4/$E4</f>
-        <v>0.26666666666666666</v>
-      </c>
-      <c r="O4">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="P4">
-        <f t="shared" si="0"/>
-        <v>0.53333333333333333</v>
-      </c>
-      <c r="Q4">
-        <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="R4">
-        <f>MIN((H4*($F4+$E4))/($E4*$F4),1)</f>
-        <v>0.19784946236559139</v>
-      </c>
-      <c r="S4">
-        <f t="shared" ref="S4:V4" si="1">MIN((I4*($F4+$E4))/($E4*$F4),1)</f>
-        <v>0.39569892473118279</v>
-      </c>
-      <c r="T4">
-        <f t="shared" si="1"/>
-        <v>0.59354838709677415</v>
-      </c>
-      <c r="U4">
-        <f t="shared" si="1"/>
-        <v>0.79139784946236558</v>
-      </c>
-      <c r="V4">
-        <f t="shared" si="1"/>
-        <v>0.989247311827957</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>37</v>
-      </c>
-      <c r="E5">
-        <v>68</v>
-      </c>
-      <c r="F5">
-        <v>74</v>
-      </c>
-      <c r="H5">
-        <v>12</v>
-      </c>
-      <c r="I5">
-        <v>13</v>
-      </c>
-      <c r="J5">
-        <v>13</v>
-      </c>
-      <c r="K5">
-        <v>13</v>
-      </c>
-      <c r="L5">
-        <v>15</v>
-      </c>
-      <c r="M5">
-        <f t="shared" ref="M5:M16" si="2">H5/$E5</f>
-        <v>0.17647058823529413</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="0"/>
-        <v>0.19117647058823528</v>
-      </c>
-      <c r="O5">
-        <f t="shared" si="0"/>
-        <v>0.19117647058823528</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="0"/>
-        <v>0.19117647058823528</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="0"/>
-        <v>0.22058823529411764</v>
-      </c>
-      <c r="R5">
-        <f t="shared" ref="R5:R16" si="3">MIN((H5*($F5+$E5))/($E5*$F5),1)</f>
-        <v>0.33863275039745627</v>
-      </c>
-      <c r="S5">
-        <f t="shared" ref="S5:S16" si="4">MIN((I5*($F5+$E5))/($E5*$F5),1)</f>
-        <v>0.36685214626391099</v>
-      </c>
-      <c r="T5">
-        <f t="shared" ref="T5:T16" si="5">MIN((J5*($F5+$E5))/($E5*$F5),1)</f>
-        <v>0.36685214626391099</v>
-      </c>
-      <c r="U5">
-        <f t="shared" ref="U5:U16" si="6">MIN((K5*($F5+$E5))/($E5*$F5),1)</f>
-        <v>0.36685214626391099</v>
-      </c>
-      <c r="V5">
-        <f t="shared" ref="V5:V16" si="7">MIN((L5*($F5+$E5))/($E5*$F5),1)</f>
-        <v>0.42329093799682033</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>39</v>
-      </c>
-      <c r="E6">
-        <v>30</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R6" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S6" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T6" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U6" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V6" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>132</v>
-      </c>
-      <c r="E7">
-        <v>92</v>
-      </c>
-      <c r="F7">
-        <v>119</v>
-      </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-      <c r="I7">
-        <v>10</v>
-      </c>
-      <c r="J7">
-        <v>15</v>
-      </c>
-      <c r="K7">
-        <v>21</v>
-      </c>
-      <c r="L7">
-        <v>35</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="2"/>
-        <v>5.434782608695652E-2</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="0"/>
-        <v>0.10869565217391304</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="0"/>
-        <v>0.16304347826086957</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="0"/>
-        <v>0.22826086956521738</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="0"/>
-        <v>0.38043478260869568</v>
-      </c>
-      <c r="R7">
-        <f t="shared" si="3"/>
-        <v>9.6364632809645592E-2</v>
-      </c>
-      <c r="S7">
-        <f t="shared" si="4"/>
-        <v>0.19272926561929118</v>
-      </c>
-      <c r="T7">
-        <f t="shared" si="5"/>
-        <v>0.28909389842893679</v>
-      </c>
-      <c r="U7">
-        <f t="shared" si="6"/>
-        <v>0.40473145780051151</v>
-      </c>
-      <c r="V7">
-        <f t="shared" si="7"/>
-        <v>0.67455242966751916</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>9</v>
-      </c>
-      <c r="D8">
-        <v>4876</v>
-      </c>
-      <c r="E8">
-        <v>2355</v>
-      </c>
-      <c r="F8">
-        <v>5900</v>
-      </c>
-      <c r="G8" t="s">
-        <v>96</v>
-      </c>
-      <c r="H8">
-        <v>1214</v>
-      </c>
-      <c r="I8">
-        <v>1504</v>
-      </c>
-      <c r="J8">
-        <v>1676</v>
-      </c>
-      <c r="K8">
-        <v>1811</v>
-      </c>
-      <c r="L8">
-        <v>2034</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="2"/>
-        <v>0.51549893842887473</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="0"/>
-        <v>0.63864118895966027</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="0"/>
-        <v>0.71167728237791927</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="0"/>
-        <v>0.76900212314225058</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="0"/>
-        <v>0.8636942675159236</v>
-      </c>
-      <c r="R8">
-        <f t="shared" si="3"/>
-        <v>0.72126165029328149</v>
-      </c>
-      <c r="S8">
-        <f t="shared" si="4"/>
-        <v>0.89355644319694838</v>
-      </c>
-      <c r="T8">
-        <f t="shared" si="5"/>
-        <v>0.99574507898808884</v>
-      </c>
-      <c r="U8">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="V8">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>907</v>
-      </c>
-      <c r="E9">
-        <v>55</v>
-      </c>
-      <c r="F9">
-        <v>61</v>
-      </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9">
-        <v>4</v>
-      </c>
-      <c r="J9">
-        <v>6</v>
-      </c>
-      <c r="K9">
-        <v>9</v>
-      </c>
-      <c r="L9">
-        <v>21</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="2"/>
-        <v>5.4545454545454543E-2</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="0"/>
-        <v>7.2727272727272724E-2</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="0"/>
-        <v>0.10909090909090909</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>0.16363636363636364</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="0"/>
-        <v>0.38181818181818183</v>
-      </c>
-      <c r="R9">
-        <f t="shared" si="3"/>
-        <v>0.10372578241430701</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="4"/>
-        <v>0.13830104321907602</v>
-      </c>
-      <c r="T9">
-        <f t="shared" si="5"/>
-        <v>0.20745156482861402</v>
-      </c>
-      <c r="U9">
-        <f t="shared" si="6"/>
-        <v>0.31117734724292101</v>
-      </c>
-      <c r="V9">
-        <f t="shared" si="7"/>
-        <v>0.72608047690014899</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10">
-        <v>14</v>
-      </c>
-      <c r="D10">
-        <v>390</v>
-      </c>
-      <c r="E10">
-        <v>694</v>
-      </c>
-      <c r="F10">
-        <v>729</v>
-      </c>
-      <c r="H10">
-        <v>102</v>
-      </c>
-      <c r="I10">
-        <v>146</v>
-      </c>
-      <c r="J10">
-        <v>176</v>
-      </c>
-      <c r="K10">
-        <v>204</v>
-      </c>
-      <c r="L10">
-        <v>272</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="2"/>
-        <v>0.14697406340057637</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="0"/>
-        <v>0.21037463976945245</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="0"/>
-        <v>0.25360230547550433</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="0"/>
-        <v>0.29394812680115273</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="0"/>
-        <v>0.39193083573487031</v>
-      </c>
-      <c r="R10">
-        <f t="shared" si="3"/>
-        <v>0.2868917588738274</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="4"/>
-        <v>0.410648988191949</v>
-      </c>
-      <c r="T10">
-        <f t="shared" si="5"/>
-        <v>0.49502891727248649</v>
-      </c>
-      <c r="U10">
-        <f t="shared" si="6"/>
-        <v>0.57378351774765479</v>
-      </c>
-      <c r="V10">
-        <f t="shared" si="7"/>
-        <v>0.76504469033020639</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="6">
-        <v>17</v>
-      </c>
-      <c r="D11" s="6">
-        <v>2998</v>
-      </c>
-      <c r="E11" s="6">
-        <v>1379</v>
-      </c>
-      <c r="F11" s="17">
-        <v>2567</v>
-      </c>
-      <c r="H11">
-        <v>588</v>
-      </c>
-      <c r="I11">
-        <v>872</v>
-      </c>
-      <c r="J11">
-        <v>1031</v>
-      </c>
-      <c r="K11">
-        <v>1147</v>
-      </c>
-      <c r="L11">
-        <v>1299</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="2"/>
-        <v>0.42639593908629442</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="0"/>
-        <v>0.63234227701232781</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="0"/>
-        <v>0.74764321972443804</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="0"/>
-        <v>0.83176214648295865</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="0"/>
-        <v>0.94198694706308916</v>
-      </c>
-      <c r="R11">
-        <f t="shared" si="3"/>
-        <v>0.65545709997449075</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="4"/>
-        <v>0.97203842037033328</v>
-      </c>
-      <c r="T11">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="U11">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="V11">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="17">
-        <v>18</v>
-      </c>
-      <c r="D12">
-        <v>1255</v>
-      </c>
-      <c r="E12">
-        <v>868</v>
-      </c>
-      <c r="F12" s="17">
-        <v>1975</v>
-      </c>
-      <c r="H12">
-        <v>103</v>
-      </c>
-      <c r="I12">
-        <v>172</v>
-      </c>
-      <c r="J12">
-        <v>259</v>
-      </c>
-      <c r="K12">
-        <v>385</v>
-      </c>
-      <c r="L12">
-        <v>779</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="2"/>
-        <v>0.11866359447004608</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="0"/>
-        <v>0.19815668202764977</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="0"/>
-        <v>0.29838709677419356</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="0"/>
-        <v>0.44354838709677419</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="0"/>
-        <v>0.89746543778801846</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="3"/>
-        <v>0.17081549320422329</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="4"/>
-        <v>0.2852452896225865</v>
-      </c>
-      <c r="T12">
-        <f t="shared" si="5"/>
-        <v>0.42952633728052264</v>
-      </c>
-      <c r="U12">
-        <f t="shared" si="6"/>
-        <v>0.63848509595753367</v>
-      </c>
-      <c r="V12">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13">
-        <v>22</v>
-      </c>
-      <c r="D13">
-        <v>6058</v>
-      </c>
-      <c r="E13">
-        <v>3891</v>
-      </c>
-      <c r="F13" s="17">
-        <v>6328</v>
-      </c>
-      <c r="G13" t="s">
-        <v>97</v>
-      </c>
-      <c r="H13">
-        <v>1028</v>
-      </c>
-      <c r="I13">
-        <v>1681</v>
-      </c>
-      <c r="J13">
-        <v>2231</v>
-      </c>
-      <c r="K13">
-        <v>2743</v>
-      </c>
-      <c r="L13" t="s">
-        <v>94</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="2"/>
-        <v>0.26419943459264972</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="0"/>
-        <v>0.43202261629401184</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="0"/>
-        <v>0.57337445386790031</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="0"/>
-        <v>0.70496016448213827</v>
-      </c>
-      <c r="Q13" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R13">
-        <f t="shared" si="3"/>
-        <v>0.42665202624878118</v>
-      </c>
-      <c r="S13">
-        <f t="shared" si="4"/>
-        <v>0.69766736977062371</v>
-      </c>
-      <c r="T13">
-        <f t="shared" si="5"/>
-        <v>0.92593450443680037</v>
-      </c>
-      <c r="U13">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="V13" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="6">
-        <v>19</v>
-      </c>
-      <c r="D14" s="6">
-        <v>4888</v>
-      </c>
-      <c r="E14" s="6">
-        <v>1384</v>
-      </c>
-      <c r="F14" s="17">
-        <v>3056</v>
-      </c>
-      <c r="H14">
-        <v>667</v>
-      </c>
-      <c r="I14">
-        <v>774</v>
-      </c>
-      <c r="J14">
-        <v>841</v>
-      </c>
-      <c r="K14">
-        <v>929</v>
-      </c>
-      <c r="L14">
-        <v>1144</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="2"/>
-        <v>0.48193641618497107</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="0"/>
-        <v>0.55924855491329484</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="0"/>
-        <v>0.60765895953757221</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="0"/>
-        <v>0.67124277456647397</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="0"/>
-        <v>0.82658959537572252</v>
-      </c>
-      <c r="R14">
-        <f t="shared" si="3"/>
-        <v>0.70019557848863601</v>
-      </c>
-      <c r="S14">
-        <f t="shared" si="4"/>
-        <v>0.81252080622219536</v>
-      </c>
-      <c r="T14">
-        <f t="shared" si="5"/>
-        <v>0.88285529461610623</v>
-      </c>
-      <c r="U14">
-        <f t="shared" si="6"/>
-        <v>0.97523492116333266</v>
-      </c>
-      <c r="V14">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15">
-        <v>20</v>
-      </c>
-      <c r="D15">
-        <v>1282</v>
-      </c>
-      <c r="E15">
-        <v>332</v>
-      </c>
-      <c r="F15" s="17">
-        <v>1041</v>
-      </c>
-      <c r="H15">
-        <v>226</v>
-      </c>
-      <c r="I15">
-        <v>261</v>
-      </c>
-      <c r="J15">
-        <v>277</v>
-      </c>
-      <c r="K15">
-        <v>290</v>
-      </c>
-      <c r="L15">
-        <v>308</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="2"/>
-        <v>0.68072289156626509</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="0"/>
-        <v>0.78614457831325302</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="0"/>
-        <v>0.83433734939759041</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="0"/>
-        <v>0.87349397590361444</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="0"/>
-        <v>0.92771084337349397</v>
-      </c>
-      <c r="R15">
-        <f t="shared" si="3"/>
-        <v>0.89782183488999223</v>
-      </c>
-      <c r="S15">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="T15">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="U15">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="V15">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16">
-        <v>21</v>
-      </c>
-      <c r="D16">
-        <v>2596</v>
-      </c>
-      <c r="E16">
-        <v>1470</v>
-      </c>
-      <c r="F16" s="17">
-        <v>1820</v>
-      </c>
-      <c r="H16">
-        <v>314</v>
-      </c>
-      <c r="I16">
-        <v>512</v>
-      </c>
-      <c r="J16">
-        <v>781</v>
-      </c>
-      <c r="K16">
-        <v>1037</v>
-      </c>
-      <c r="L16">
-        <v>1328</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="2"/>
-        <v>0.21360544217687075</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="0"/>
-        <v>0.34829931972789113</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="0"/>
-        <v>0.53129251700680269</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="0"/>
-        <v>0.70544217687074828</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="0"/>
-        <v>0.90340136054421771</v>
-      </c>
-      <c r="R16">
-        <f t="shared" si="3"/>
-        <v>0.3861329147043433</v>
-      </c>
-      <c r="S16">
-        <f t="shared" si="4"/>
-        <v>0.62961800104657251</v>
-      </c>
-      <c r="T16">
-        <f t="shared" si="5"/>
-        <v>0.96041339612768184</v>
-      </c>
-      <c r="U16">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="V16">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="6">
-        <v>907</v>
-      </c>
-      <c r="E17" s="6">
-        <v>55</v>
-      </c>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18">
-        <v>2287</v>
-      </c>
-      <c r="E18">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19">
-        <v>1304</v>
-      </c>
-      <c r="E19">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20">
-        <v>375</v>
-      </c>
-      <c r="E20">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21">
-        <v>1605</v>
-      </c>
-      <c r="E21">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22">
-        <v>1545</v>
-      </c>
-      <c r="E22">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="12">
-        <v>193</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23">
-        <v>1391</v>
-      </c>
-      <c r="E23">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="12">
-        <v>162</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24">
-        <v>1077</v>
-      </c>
-      <c r="E24">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="12">
-        <v>213</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25">
-        <v>844</v>
-      </c>
-      <c r="E25">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26">
-        <v>375</v>
-      </c>
-      <c r="E26">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="D3:D16">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D26">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:F16">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:F26">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R4:V16">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
A few new sets of results: - J1 and epri 7 circuits now modified to take out problematic capacitors that has improved results somewhat (we had a bunch of undervoltages on epri7). - Comparisons run and plotted for linear models that have tap changers, going up and down one tap, to show sensitivity to tap - Metric chosen to compare changes to PDFs as a regularised 1-norm metric. - More plotting and shite to go in the paper.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="188">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -588,6 +588,18 @@
   </si>
   <si>
     <t>Class: linSvdCalcs</t>
+  </si>
+  <si>
+    <t>_Z</t>
+  </si>
+  <si>
+    <t>_Z_Y</t>
+  </si>
+  <si>
+    <t>pltHcResults</t>
+  </si>
+  <si>
+    <t>DSS SCRIPTS</t>
   </si>
 </sst>
 </file>
@@ -813,12 +825,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -1579,13 +1591,13 @@
       <c r="N1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
       <c r="T1" s="23"/>
       <c r="U1" s="27"/>
     </row>
@@ -8058,7 +8070,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8373,7 +8385,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8826,10 +8838,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8842,40 +8854,49 @@
     <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="K2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>171</v>
       </c>
       <c r="B3" t="s">
         <v>172</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="28" t="s">
         <v>181</v>
       </c>
       <c r="F3" t="s">
         <v>173</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="28" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>184</v>
+      </c>
+      <c r="L3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>179</v>
       </c>
@@ -8886,8 +8907,8 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
         <v>174</v>
       </c>
       <c r="B5" t="s">
@@ -8900,18 +8921,28 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
         <v>183</v>
       </c>
     </row>

</xml_diff>

<commit_message>
A bunch of changes. 1. Capacitor model updated so that capacitors do not change with loads in the models, to be rather more realistic (both linear and OpenDSS models) 2. A bunch of the model's CAPACITOR SETTINGS have been updated (!) to try and make the problem feasible again. 3. A new set of results have been created with a bandwidth of 1 with the idea that sensitivity analysis will perhaps (?) be a secondary set.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E83D7FF-D8FD-4957-AFBB-2AF382744B9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <sheet name="varV2stuff" sheetId="7" r:id="rId12"/>
     <sheet name="quarterGenQuarterMax" sheetId="9" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="191">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -600,12 +601,21 @@
   </si>
   <si>
     <t>DSS SCRIPTS</t>
+  </si>
+  <si>
+    <t>\</t>
+  </si>
+  <si>
+    <t>linHcCalcs Full</t>
+  </si>
+  <si>
+    <t>linHcCalcs Sns</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1513,14 +1523,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36:H37"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3611,7 +3621,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4860,7 +4870,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5890,7 +5900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7158,7 +7168,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="B2:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7695,7 +7705,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -8056,21 +8066,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="D11" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8378,7 +8388,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -8834,14 +8844,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8852,6 +8862,8 @@
     <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -8941,9 +8953,331 @@
         <v>186</v>
       </c>
     </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F10" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>186</v>
+      </c>
+    </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>183</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>188</v>
+      </c>
+      <c r="G11" t="s">
+        <v>188</v>
+      </c>
+      <c r="H11" t="s">
+        <v>188</v>
+      </c>
+      <c r="I11" t="s">
+        <v>188</v>
+      </c>
+      <c r="J11" t="s">
+        <v>188</v>
+      </c>
+      <c r="K11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" t="s">
+        <v>188</v>
+      </c>
+      <c r="J12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>188</v>
+      </c>
+      <c r="J13" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>188</v>
+      </c>
+      <c r="G14" t="s">
+        <v>188</v>
+      </c>
+      <c r="H14" t="s">
+        <v>188</v>
+      </c>
+      <c r="I14" t="s">
+        <v>188</v>
+      </c>
+      <c r="J14" t="s">
+        <v>188</v>
+      </c>
+      <c r="K14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" t="s">
+        <v>188</v>
+      </c>
+      <c r="J15" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" t="s">
+        <v>188</v>
+      </c>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" t="s">
+        <v>188</v>
+      </c>
+      <c r="H17" t="s">
+        <v>188</v>
+      </c>
+      <c r="I17" t="s">
+        <v>188</v>
+      </c>
+      <c r="J17" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" t="s">
+        <v>188</v>
+      </c>
+      <c r="H18" t="s">
+        <v>188</v>
+      </c>
+      <c r="I18" t="s">
+        <v>188</v>
+      </c>
+      <c r="J18" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" t="s">
+        <v>188</v>
+      </c>
+      <c r="H19" t="s">
+        <v>188</v>
+      </c>
+      <c r="I19" t="s">
+        <v>188</v>
+      </c>
+      <c r="J19" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" t="s">
+        <v>188</v>
+      </c>
+      <c r="H20" t="s">
+        <v>188</v>
+      </c>
+      <c r="I20" t="s">
+        <v>188</v>
+      </c>
+      <c r="J20" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" t="s">
+        <v>188</v>
+      </c>
+      <c r="I21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" t="s">
+        <v>188</v>
+      </c>
+      <c r="I22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" t="s">
+        <v>188</v>
+      </c>
+      <c r="I23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" t="s">
+        <v>188</v>
+      </c>
+      <c r="I24" t="s">
+        <v>26</v>
+      </c>
+      <c r="J24" t="s">
+        <v>26</v>
+      </c>
+      <c r="K24" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -8953,7 +9287,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -8970,7 +9304,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="2"/>
   </sheetPr>
@@ -9190,7 +9524,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9847,7 +10181,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
A whole bunch of changes. (1) all circuits have been re-reviewed to check their capacitor status; all caps controls have been put back in. (2) new capacitor control model, whereby the capacitors are switched in as if they had the caps at teh linearization point (3) script updated to create all results in one go for the paper/plotting (4) some new plotting functions
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E83D7FF-D8FD-4957-AFBB-2AF382744B9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AE9521-21C4-442D-8D81-6468BE26753E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="195">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -540,9 +540,6 @@
     <t>&lt;-- there are two voltage regulator settings here for some reason?\</t>
   </si>
   <si>
-    <t>Chgd</t>
-  </si>
-  <si>
     <t>&lt;--- for some reason, some are commented out in orgnl script</t>
   </si>
   <si>
@@ -610,6 +607,21 @@
   </si>
   <si>
     <t>linHcCalcs Sns</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>6//4</t>
+  </si>
+  <si>
+    <t>2//0</t>
+  </si>
+  <si>
+    <t>0//0</t>
+  </si>
+  <si>
+    <t>3//2</t>
   </si>
 </sst>
 </file>
@@ -1530,7 +1542,7 @@
   <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B16"/>
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5903,8 +5915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" activeCellId="1" sqref="A11:C16 A8:C8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="V8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8079,8 +8091,8 @@
   </sheetPr>
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8109,9 +8121,6 @@
       <c r="I1" t="s">
         <v>148</v>
       </c>
-      <c r="L1" t="s">
-        <v>167</v>
-      </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -8191,6 +8200,9 @@
         <f>H5/I5</f>
         <v>1.075</v>
       </c>
+      <c r="L5" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -8239,6 +8251,9 @@
       <c r="F8" t="s">
         <v>141</v>
       </c>
+      <c r="L8" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -8263,7 +8278,7 @@
         <v>150</v>
       </c>
       <c r="L9" t="s">
-        <v>30</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -8309,10 +8324,10 @@
         <v>120</v>
       </c>
       <c r="L11" t="s">
-        <v>30</v>
+        <v>194</v>
       </c>
       <c r="M11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -8340,7 +8355,13 @@
         <v>3</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>190</v>
+      </c>
+      <c r="L13" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -8395,7 +8416,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8423,7 +8444,7 @@
         <v>162</v>
       </c>
       <c r="I1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J1">
         <v>1</v>
@@ -8687,7 +8708,7 @@
         <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H10" t="s">
         <v>30</v>
@@ -8848,10 +8869,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8868,135 +8889,135 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" t="s">
         <v>171</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" t="s">
         <v>172</v>
       </c>
-      <c r="C3" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="E3" s="28" t="s">
+      <c r="G3" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="F3" t="s">
-        <v>173</v>
-      </c>
-      <c r="G3" s="28" t="s">
-        <v>182</v>
-      </c>
       <c r="K3" t="s">
+        <v>183</v>
+      </c>
+      <c r="L3" t="s">
         <v>184</v>
-      </c>
-      <c r="L3" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F10" s="28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G10" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="H10" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="H10" s="28" t="s">
-        <v>182</v>
-      </c>
       <c r="I10" s="28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J10" s="28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K10" s="28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -9013,7 +9034,7 @@
         <v>26</v>
       </c>
       <c r="I12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J12" t="s">
         <v>26</v>
@@ -9036,7 +9057,7 @@
         <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J13" t="s">
         <v>26</v>
@@ -9050,22 +9071,22 @@
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -9082,7 +9103,7 @@
         <v>26</v>
       </c>
       <c r="I15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J15" t="s">
         <v>26</v>
@@ -9102,7 +9123,7 @@
         <v>26</v>
       </c>
       <c r="H16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I16" t="s">
         <v>26</v>
@@ -9116,13 +9137,13 @@
         <v>26</v>
       </c>
       <c r="G17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J17" t="s">
         <v>26</v>
@@ -9139,13 +9160,13 @@
         <v>26</v>
       </c>
       <c r="G18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J18" t="s">
         <v>26</v>
@@ -9162,13 +9183,13 @@
         <v>26</v>
       </c>
       <c r="G19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J19" t="s">
         <v>26</v>
@@ -9185,13 +9206,13 @@
         <v>26</v>
       </c>
       <c r="G20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J20" t="s">
         <v>26</v>
@@ -9211,7 +9232,7 @@
         <v>26</v>
       </c>
       <c r="H21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I21" t="s">
         <v>26</v>
@@ -9228,7 +9249,7 @@
         <v>26</v>
       </c>
       <c r="H22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I22" t="s">
         <v>26</v>
@@ -9245,7 +9266,7 @@
         <v>26</v>
       </c>
       <c r="H23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I23" t="s">
         <v>26</v>
@@ -9268,16 +9289,165 @@
         <v>26</v>
       </c>
       <c r="H24" t="s">
+        <v>187</v>
+      </c>
+      <c r="I24" t="s">
+        <v>26</v>
+      </c>
+      <c r="J24" t="s">
+        <v>26</v>
+      </c>
+      <c r="K24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F27" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="J27" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="I24" t="s">
-        <v>26</v>
-      </c>
-      <c r="J24" t="s">
-        <v>26</v>
-      </c>
-      <c r="K24" t="s">
-        <v>26</v>
+      <c r="K27" s="28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" t="s">
+        <v>26</v>
+      </c>
+      <c r="I28" t="s">
+        <v>187</v>
+      </c>
+      <c r="J28" t="s">
+        <v>26</v>
+      </c>
+      <c r="K28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" t="s">
+        <v>187</v>
+      </c>
+      <c r="J29" t="s">
+        <v>26</v>
+      </c>
+      <c r="K29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" t="s">
+        <v>187</v>
+      </c>
+      <c r="H31" t="s">
+        <v>187</v>
+      </c>
+      <c r="I31" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" t="s">
+        <v>187</v>
+      </c>
+      <c r="H32" t="s">
+        <v>187</v>
+      </c>
+      <c r="I32" t="s">
+        <v>187</v>
+      </c>
+      <c r="J32" t="s">
+        <v>26</v>
+      </c>
+      <c r="K32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E34" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G34" t="s">
+        <v>26</v>
+      </c>
+      <c r="H34" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>23</v>
+      </c>
+      <c r="H36" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Main changes: - saving the right stuff and plotting the right stuff, ready for the paper, plus half of the results. Have left the final three cases running.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AE9521-21C4-442D-8D81-6468BE26753E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
     <sheet name="varV2stuff" sheetId="7" r:id="rId12"/>
     <sheet name="quarterGenQuarterMax" sheetId="9" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="196">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -622,12 +621,15 @@
   </si>
   <si>
     <t>3//2</t>
+  </si>
+  <si>
+    <t>BSP:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1535,7 +1537,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -3633,7 +3635,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4882,7 +4884,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5912,7 +5914,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -7180,7 +7182,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7717,7 +7719,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -8078,14 +8080,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -8409,7 +8411,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -8865,14 +8867,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8884,7 +8886,7 @@
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -9129,7 +9131,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>9</v>
       </c>
@@ -9152,7 +9154,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>24</v>
       </c>
@@ -9175,7 +9177,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E19" s="6" t="s">
         <v>14</v>
       </c>
@@ -9198,7 +9200,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>15</v>
       </c>
@@ -9221,7 +9223,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>16</v>
       </c>
@@ -9238,7 +9240,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E22" s="6" t="s">
         <v>21</v>
       </c>
@@ -9255,7 +9257,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>22</v>
       </c>
@@ -9278,7 +9280,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>23</v>
       </c>
@@ -9301,27 +9303,33 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F27" s="28" t="s">
         <v>170</v>
       </c>
       <c r="G27" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="H27" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="H27" s="28" t="s">
+      <c r="I27" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="I27" s="28" t="s">
+      <c r="J27" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="J27" s="28" t="s">
+      <c r="K27" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="K27" s="28" t="s">
+      <c r="L27" s="28" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>195</v>
+      </c>
       <c r="E28" t="s">
         <v>6</v>
       </c>
@@ -9335,16 +9343,13 @@
         <v>26</v>
       </c>
       <c r="I28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J28" t="s">
         <v>187</v>
       </c>
-      <c r="J28" t="s">
-        <v>26</v>
-      </c>
-      <c r="K28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>8</v>
       </c>
@@ -9358,27 +9363,39 @@
         <v>26</v>
       </c>
       <c r="I29" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" t="s">
         <v>187</v>
       </c>
-      <c r="J29" t="s">
-        <v>26</v>
-      </c>
-      <c r="K29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
         <v>17</v>
       </c>
+      <c r="F30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" t="s">
+        <v>26</v>
+      </c>
       <c r="H30" t="s">
+        <v>26</v>
+      </c>
+      <c r="I30" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E31" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="F31" t="s">
+        <v>26</v>
+      </c>
       <c r="G31" t="s">
         <v>187</v>
       </c>
@@ -9388,8 +9405,11 @@
       <c r="I31" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>15</v>
       </c>
@@ -9406,21 +9426,30 @@
         <v>187</v>
       </c>
       <c r="J32" t="s">
-        <v>26</v>
-      </c>
-      <c r="K32" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>16</v>
       </c>
+      <c r="F33" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" t="s">
+        <v>26</v>
+      </c>
       <c r="H33" t="s">
+        <v>26</v>
+      </c>
+      <c r="I33" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E34" s="6" t="s">
         <v>21</v>
       </c>
@@ -9431,23 +9460,53 @@
         <v>26</v>
       </c>
       <c r="H34" t="s">
+        <v>26</v>
+      </c>
+      <c r="I34" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
         <v>22</v>
       </c>
+      <c r="F35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G35" t="s">
+        <v>26</v>
+      </c>
       <c r="H35" t="s">
+        <v>26</v>
+      </c>
+      <c r="I35" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
         <v>23</v>
       </c>
+      <c r="F36" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" t="s">
+        <v>26</v>
+      </c>
       <c r="H36" t="s">
+        <v>26</v>
+      </c>
+      <c r="I36" t="s">
         <v>187</v>
+      </c>
+      <c r="J36" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -9457,7 +9516,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -9474,7 +9533,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="2"/>
   </sheetPr>
@@ -9694,7 +9753,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10351,7 +10410,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
A new set of 'final' results; plus, a whole bunch of plotting functions, including now having a style file to save having to do so much when using matplotlib.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC16FE8F-BEDE-46B7-A64A-D26F8A15C176}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <sheet name="varV2stuff" sheetId="7" r:id="rId12"/>
     <sheet name="quarterGenQuarterMax" sheetId="9" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="196">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -629,7 +630,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1537,7 +1538,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -3635,7 +3636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4884,7 +4885,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5914,7 +5915,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -7182,7 +7183,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="B2:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7719,7 +7720,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -8080,14 +8081,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="D11" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -8411,14 +8412,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8867,14 +8868,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9348,6 +9349,12 @@
       <c r="J28" t="s">
         <v>187</v>
       </c>
+      <c r="K28" t="s">
+        <v>26</v>
+      </c>
+      <c r="L28" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
@@ -9368,6 +9375,12 @@
       <c r="J29" t="s">
         <v>187</v>
       </c>
+      <c r="K29" t="s">
+        <v>26</v>
+      </c>
+      <c r="L29" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
@@ -9388,6 +9401,12 @@
       <c r="J30" t="s">
         <v>26</v>
       </c>
+      <c r="K30" t="s">
+        <v>26</v>
+      </c>
+      <c r="L30" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E31" s="6" t="s">
@@ -9408,6 +9427,12 @@
       <c r="J31" t="s">
         <v>187</v>
       </c>
+      <c r="K31" t="s">
+        <v>26</v>
+      </c>
+      <c r="L31" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
@@ -9428,8 +9453,14 @@
       <c r="J32" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>26</v>
+      </c>
+      <c r="L32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>16</v>
       </c>
@@ -9449,7 +9480,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E34" s="6" t="s">
         <v>21</v>
       </c>
@@ -9468,8 +9499,14 @@
       <c r="J34" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
+        <v>26</v>
+      </c>
+      <c r="L34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
         <v>22</v>
       </c>
@@ -9488,8 +9525,14 @@
       <c r="J35" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>26</v>
+      </c>
+      <c r="L35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
         <v>23</v>
       </c>
@@ -9506,6 +9549,12 @@
         <v>187</v>
       </c>
       <c r="J36" t="s">
+        <v>26</v>
+      </c>
+      <c r="K36" t="s">
+        <v>26</v>
+      </c>
+      <c r="L36" t="s">
         <v>26</v>
       </c>
     </row>
@@ -9516,7 +9565,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -9533,7 +9582,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="2"/>
   </sheetPr>
@@ -9753,7 +9802,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10410,7 +10459,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
More plotting updates and tidying crap up.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5528F5E6-32C7-4AF7-8FD5-FAF4A911834E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <sheet name="varV2stuff" sheetId="7" r:id="rId12"/>
     <sheet name="quarterGenQuarterMax" sheetId="9" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,6 +30,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -644,7 +646,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1552,14 +1554,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="A1:AA36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1787,7 +1789,7 @@
         <v>41</v>
       </c>
       <c r="H4" s="6">
-        <f t="shared" ref="H4:H31" si="0">LOG(D4*G4)</f>
+        <f t="shared" ref="H4:H26" si="0">LOG(D4*G4)</f>
         <v>2.7888751157754168</v>
       </c>
       <c r="I4" t="s">
@@ -2038,7 +2040,7 @@
         <v>4</v>
       </c>
       <c r="L7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M7">
         <v>6</v>
@@ -4221,7 +4223,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5470,7 +5472,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6500,7 +6502,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -7768,7 +7770,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="B2:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8305,7 +8307,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -8666,14 +8668,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="D11" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -8997,7 +8999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -9453,7 +9455,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -10150,7 +10152,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -10167,7 +10169,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="2"/>
   </sheetPr>
@@ -10387,7 +10389,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11044,7 +11046,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Changes mostly to to plotting figures.
IMPORTANTLY though, have also changed the tolerance of OpenDSS and it seems to make quite a difference, so need to rerun some of the error calculations, for example.
</commit_message>
<xml_diff>
--- a/ptech18/ieee_tn/distribution_circuits.xlsx
+++ b/ptech18/ieee_tn/distribution_circuits.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5528F5E6-32C7-4AF7-8FD5-FAF4A911834E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4D8B5E-2F71-4BAE-A889-C8414215CDEB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3105" windowWidth="21600" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="202">
   <si>
     <t>IEEE Circuits</t>
   </si>
@@ -641,6 +641,9 @@
   </si>
   <si>
     <t>Manc Ntwx</t>
+  </si>
+  <si>
+    <t>Regc</t>
   </si>
 </sst>
 </file>
@@ -1558,10 +1561,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:AA36"/>
+  <dimension ref="A1:AB36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1576,22 +1579,22 @@
     <col min="8" max="8" width="9.5703125" customWidth="1"/>
     <col min="9" max="9" width="6" customWidth="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.140625" customWidth="1"/>
-    <col min="18" max="18" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="3.42578125" customWidth="1"/>
-    <col min="24" max="24" width="23" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.140625" customWidth="1"/>
+    <col min="19" max="19" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="3.42578125" customWidth="1"/>
+    <col min="25" max="25" width="23" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1629,28 +1632,31 @@
         <v>3</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="R1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="31"/>
       <c r="S1" s="31"/>
       <c r="T1" s="31"/>
       <c r="U1" s="31"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="27"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="V1" s="31"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="27"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -1666,40 +1672,41 @@
       <c r="M2" s="16"/>
       <c r="N2" s="16"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="4" t="s">
+      <c r="P2" s="16"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1735,20 +1742,20 @@
       <c r="L3" s="6">
         <v>0</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="6">
+        <v>0</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="N3" s="6">
-        <v>5.4</v>
       </c>
       <c r="O3" s="6">
         <v>5.4</v>
       </c>
-      <c r="P3" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>27</v>
+      <c r="P3" s="6">
+        <v>5.4</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>26</v>
       </c>
       <c r="R3" s="8" t="s">
         <v>27</v>
@@ -1768,8 +1775,11 @@
       <c r="W3" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="X3" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -1805,21 +1815,21 @@
         <v>1</v>
       </c>
       <c r="M4">
+        <v>3</v>
+      </c>
+      <c r="N4">
         <v>1.5</v>
-      </c>
-      <c r="N4">
-        <v>3.6</v>
       </c>
       <c r="O4">
         <v>3.6</v>
       </c>
       <c r="P4">
+        <v>3.6</v>
+      </c>
+      <c r="Q4">
         <f>LOG10(703)</f>
         <v>2.8469553250198238</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1838,20 +1848,23 @@
       <c r="W4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Y4">
+      <c r="X4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z4">
         <f>18/60</f>
         <v>0.3</v>
       </c>
-      <c r="Z4">
-        <f>(10^P4)*9000*0.000001/60</f>
+      <c r="AA4">
+        <f>(10^Q4)*9000*0.000001/60</f>
         <v>0.10545000000000002</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <f>18/60</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -1887,21 +1900,21 @@
         <v>2</v>
       </c>
       <c r="M5">
+        <v>6</v>
+      </c>
+      <c r="N5">
         <v>50</v>
-      </c>
-      <c r="N5">
-        <v>2</v>
       </c>
       <c r="O5">
         <v>2</v>
       </c>
       <c r="P5">
+        <v>2</v>
+      </c>
+      <c r="Q5">
         <f>LOG10(4000)</f>
         <v>3.6020599913279625</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1920,20 +1933,23 @@
       <c r="W5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Y5">
+      <c r="X5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z5">
         <f>53.7/60</f>
         <v>0.89500000000000002</v>
       </c>
-      <c r="Z5">
-        <f t="shared" ref="Z5:Z26" si="1">(10^P5)*9000*0.000001/60</f>
+      <c r="AA5">
+        <f t="shared" ref="AA5:AA26" si="1">(10^Q5)*9000*0.000001/60</f>
         <v>0.60000000000000098</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <f>19/60</f>
         <v>0.31666666666666665</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -1969,26 +1985,26 @@
         <v>1</v>
       </c>
       <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
         <v>3</v>
-      </c>
-      <c r="N6">
-        <v>2.6</v>
       </c>
       <c r="O6">
         <v>2.6</v>
       </c>
       <c r="P6">
+        <v>2.6</v>
+      </c>
+      <c r="Q6">
         <f>LOG10(2907)</f>
         <v>3.4634450317704277</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="R6" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="S6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>27</v>
@@ -2002,12 +2018,15 @@
       <c r="W6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Z6">
+      <c r="X6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA6">
         <f t="shared" si="1"/>
         <v>0.43605000000000016</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -2040,27 +2059,27 @@
         <v>4</v>
       </c>
       <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7">
         <v>7</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>6</v>
-      </c>
-      <c r="N7">
-        <v>3.6</v>
       </c>
       <c r="O7">
         <v>3.6</v>
       </c>
       <c r="P7">
+        <v>3.6</v>
+      </c>
+      <c r="Q7">
         <f>LOG10(4965)</f>
         <v>3.6959192528313998</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="R7" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="S7" s="1" t="s">
         <v>26</v>
       </c>
@@ -2076,20 +2095,23 @@
       <c r="W7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Y7">
+      <c r="X7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z7">
         <f>72/60</f>
         <v>1.2</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <f t="shared" si="1"/>
         <v>0.74475000000000013</v>
       </c>
-      <c r="AA7">
+      <c r="AB7">
         <f>33/60</f>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -2125,47 +2147,50 @@
         <v>12</v>
       </c>
       <c r="M8">
+        <v>12</v>
+      </c>
+      <c r="N8">
         <v>17</v>
-      </c>
-      <c r="N8">
-        <v>12.05</v>
       </c>
       <c r="O8">
         <v>12.05</v>
       </c>
       <c r="P8">
+        <v>12.05</v>
+      </c>
+      <c r="Q8">
         <f>LOG10(275763)</f>
         <v>5.4405359950748213</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="R8" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="S8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="T8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U8" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="V8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W8" s="1"/>
-      <c r="Z8">
+      <c r="W8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X8" s="1"/>
+      <c r="AA8">
         <f t="shared" si="1"/>
         <v>41.364450000000069</v>
       </c>
-      <c r="AA8">
+      <c r="AB8">
         <f>958/60</f>
         <v>15.966666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -2201,32 +2226,32 @@
         <v>0</v>
       </c>
       <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
         <v>0.3</v>
-      </c>
-      <c r="N9">
-        <v>5.5E-2</v>
       </c>
       <c r="O9">
         <v>5.5E-2</v>
       </c>
       <c r="P9">
+        <v>5.5E-2</v>
+      </c>
+      <c r="Q9">
         <f>LOG10(5144)</f>
         <v>3.7113009599161657</v>
       </c>
-      <c r="Q9" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="V9" s="1" t="s">
         <v>26</v>
@@ -2234,16 +2259,19 @@
       <c r="W9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z9">
+      <c r="X9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA9">
         <f t="shared" si="1"/>
         <v>0.77160000000000128</v>
       </c>
-      <c r="AA9">
+      <c r="AB9">
         <f>59/60</f>
         <v>0.98333333333333328</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -2278,47 +2306,50 @@
       <c r="L10">
         <v>0</v>
       </c>
-      <c r="N10">
-        <v>42.8</v>
+      <c r="M10">
+        <v>0</v>
       </c>
       <c r="O10">
         <v>42.8</v>
       </c>
-      <c r="P10" s="15">
+      <c r="P10">
+        <v>42.8</v>
+      </c>
+      <c r="Q10" s="15">
         <f>LOG10(12061)</f>
         <v>4.0813833174622856</v>
       </c>
-      <c r="Q10" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="V10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="W10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z10">
+      <c r="X10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA10">
         <f t="shared" si="1"/>
         <v>1.8091500000000034</v>
       </c>
-      <c r="AA10">
+      <c r="AB10">
         <f>145/60</f>
         <v>2.4166666666666665</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -2357,32 +2388,32 @@
         <v>0</v>
       </c>
       <c r="M11" s="6">
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
         <v>5</v>
-      </c>
-      <c r="N11" s="6">
-        <v>16.3</v>
       </c>
       <c r="O11" s="6">
         <v>16.3</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="6">
+        <v>16.3</v>
+      </c>
+      <c r="Q11">
         <f>LOG10(32321)</f>
         <v>4.50948478922394</v>
       </c>
-      <c r="Q11" s="8" t="s">
+      <c r="R11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="R11" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="S11" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T11" s="8" t="s">
         <v>27</v>
       </c>
       <c r="U11" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="V11" s="8" t="s">
         <v>26</v>
@@ -2390,20 +2421,23 @@
       <c r="W11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="Y11">
+      <c r="X11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z11">
         <f>637/60</f>
         <v>10.616666666666667</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <f t="shared" si="1"/>
         <v>4.8481500000000013</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <f>371/60</f>
         <v>6.1833333333333336</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -2439,32 +2473,32 @@
         <v>0</v>
       </c>
       <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
         <v>4</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>78</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>19.3</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <f>LOG10(17450)</f>
         <v>4.2417954312951984</v>
       </c>
-      <c r="Q12" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="V12" s="1" t="s">
         <v>26</v>
@@ -2472,22 +2506,25 @@
       <c r="W12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="X12" t="s">
+      <c r="X12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y12" t="s">
         <v>77</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Z12" t="s">
         <v>89</v>
       </c>
-      <c r="Z12">
+      <c r="AA12">
         <f t="shared" si="1"/>
         <v>2.6175000000000002</v>
       </c>
-      <c r="AA12">
+      <c r="AB12">
         <f>367/60</f>
         <v>6.1166666666666663</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -2523,21 +2560,21 @@
         <v>1</v>
       </c>
       <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
         <v>10</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>52.2</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>69.400000000000006</v>
       </c>
-      <c r="P13" s="15">
+      <c r="Q13" s="15">
         <f>LOG10(87955)</f>
         <v>4.9442605329428515</v>
       </c>
-      <c r="Q13" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R13" s="1" t="s">
         <v>26</v>
       </c>
@@ -2545,28 +2582,31 @@
         <v>26</v>
       </c>
       <c r="T13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U13" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="V13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W13" s="1"/>
-      <c r="Y13" t="s">
+      <c r="W13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X13" s="1"/>
+      <c r="Z13" t="s">
         <v>88</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <f t="shared" si="1"/>
         <v>13.193250000000001</v>
       </c>
-      <c r="AA13">
+      <c r="AB13">
         <f>1996/60</f>
         <v>33.266666666666666</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
@@ -2605,21 +2645,21 @@
         <v>9</v>
       </c>
       <c r="M14" s="6">
+        <v>9</v>
+      </c>
+      <c r="N14" s="6">
         <v>18</v>
-      </c>
-      <c r="N14" s="6">
-        <v>11.6</v>
       </c>
       <c r="O14" s="6">
         <v>11.6</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="6">
+        <v>11.6</v>
+      </c>
+      <c r="Q14">
         <f>LOG10(26279)</f>
         <v>4.4196088349081029</v>
       </c>
-      <c r="Q14" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="R14" s="8" t="s">
         <v>26</v>
       </c>
@@ -2627,28 +2667,31 @@
         <v>26</v>
       </c>
       <c r="T14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="U14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="U14" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="V14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="W14" s="8"/>
-      <c r="X14" t="s">
+      <c r="W14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="X14" s="8"/>
+      <c r="Y14" t="s">
         <v>61</v>
       </c>
-      <c r="Z14">
+      <c r="AA14">
         <f t="shared" si="1"/>
         <v>3.9418500000000019</v>
       </c>
-      <c r="AA14">
+      <c r="AB14">
         <f>551/60</f>
         <v>9.1833333333333336</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -2683,22 +2726,22 @@
       <c r="L15">
         <v>1</v>
       </c>
-      <c r="M15" s="17">
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15" s="17">
         <v>7</v>
-      </c>
-      <c r="N15">
-        <v>12.74</v>
       </c>
       <c r="O15">
         <v>12.74</v>
       </c>
       <c r="P15">
+        <v>12.74</v>
+      </c>
+      <c r="Q15">
         <f>LOG10(20153)</f>
         <v>4.3043397048923389</v>
       </c>
-      <c r="Q15" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R15" s="1" t="s">
         <v>26</v>
       </c>
@@ -2714,17 +2757,20 @@
       <c r="V15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W15" s="1"/>
-      <c r="Z15">
+      <c r="W15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X15" s="1"/>
+      <c r="AA15">
         <f t="shared" si="1"/>
         <v>3.0229500000000038</v>
       </c>
-      <c r="AA15">
+      <c r="AB15">
         <f>107/60</f>
         <v>1.7833333333333334</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>23</v>
       </c>
@@ -2759,22 +2805,22 @@
       <c r="L16">
         <v>1</v>
       </c>
-      <c r="M16" s="17">
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16" s="17">
         <v>3.4</v>
-      </c>
-      <c r="N16">
-        <v>15.67</v>
       </c>
       <c r="O16">
         <v>15.67</v>
       </c>
-      <c r="P16" s="15">
+      <c r="P16">
+        <v>15.67</v>
+      </c>
+      <c r="Q16" s="15">
         <f>LOG10(27688)</f>
         <v>4.4422915862860712</v>
       </c>
-      <c r="Q16" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R16" s="1" t="s">
         <v>26</v>
       </c>
@@ -2782,25 +2828,28 @@
         <v>26</v>
       </c>
       <c r="T16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U16" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="V16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W16" s="1"/>
-      <c r="Z16">
+      <c r="W16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X16" s="1"/>
+      <c r="AA16">
         <f t="shared" si="1"/>
         <v>4.1532000000000036</v>
       </c>
-      <c r="AA16">
+      <c r="AB16">
         <f>445/60</f>
         <v>7.416666666666667</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>92</v>
       </c>
@@ -2839,42 +2888,45 @@
         <v>0</v>
       </c>
       <c r="M17" s="6">
+        <v>0</v>
+      </c>
+      <c r="N17" s="6">
         <v>0.3</v>
       </c>
-      <c r="N17" s="6">
+      <c r="O17" s="6">
         <f>svdStuff!E17*0.001</f>
         <v>5.5E-2</v>
       </c>
-      <c r="O17" s="6">
+      <c r="P17" s="6">
         <v>5.5E-2</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <f>LOG10(10388)</f>
         <v>4.0165319409572655</v>
       </c>
-      <c r="Q17" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="R17" s="8" t="s">
         <v>26</v>
       </c>
       <c r="S17" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T17" s="8" t="s">
         <v>27</v>
       </c>
       <c r="U17" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="V17" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="V17" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="W17" s="8"/>
-      <c r="Z17">
+      <c r="X17" s="8"/>
+      <c r="AA17">
         <f t="shared" si="1"/>
         <v>1.5582000000000018</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>38</v>
       </c>
@@ -2910,42 +2962,45 @@
         <v>0</v>
       </c>
       <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
         <v>0.5</v>
       </c>
-      <c r="N18" s="13">
+      <c r="O18" s="13">
         <f>svdStuff!E18*0.001</f>
         <v>0.17500000000000002</v>
       </c>
-      <c r="O18" s="13">
+      <c r="P18" s="13">
         <v>0.17500000000000002</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <f>LOG10(24732)</f>
         <v>4.3932592378268378</v>
       </c>
-      <c r="Q18" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V18" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="W18" s="1"/>
-      <c r="Z18">
+      <c r="X18" s="1"/>
+      <c r="AA18">
         <f t="shared" si="1"/>
         <v>3.7098000000000053</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>39</v>
       </c>
@@ -2981,42 +3036,45 @@
         <v>0</v>
       </c>
       <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
         <v>0.45</v>
       </c>
-      <c r="N19" s="13">
+      <c r="O19" s="13">
         <f>svdStuff!E19*0.001</f>
         <v>9.4E-2</v>
       </c>
-      <c r="O19" s="13">
+      <c r="P19" s="13">
         <v>9.4E-2</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <f>LOG10(24431)</f>
         <v>4.3879412437066989</v>
       </c>
-      <c r="Q19" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R19" s="1" t="s">
         <v>26</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V19" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="W19" s="1"/>
-      <c r="Z19">
+      <c r="X19" s="1"/>
+      <c r="AA19">
         <f t="shared" si="1"/>
         <v>3.6646500000000035</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>36</v>
       </c>
@@ -3052,42 +3110,45 @@
         <v>0</v>
       </c>
       <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
         <v>0.18</v>
       </c>
-      <c r="N20" s="13">
+      <c r="O20" s="13">
         <f>svdStuff!E20*0.001</f>
         <v>2.4E-2</v>
       </c>
-      <c r="O20" s="13">
+      <c r="P20" s="13">
         <v>2.4E-2</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <f>LOG10(6773)</f>
         <v>3.8307810756063612</v>
       </c>
-      <c r="Q20" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R20" s="1" t="s">
         <v>26</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T20" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V20" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="W20" s="1"/>
-      <c r="Z20">
+      <c r="X20" s="1"/>
+      <c r="AA20">
         <f t="shared" si="1"/>
         <v>1.0159500000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>34</v>
       </c>
@@ -3122,40 +3183,43 @@
       <c r="L21">
         <v>0</v>
       </c>
-      <c r="N21" s="13">
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="O21" s="13">
         <f>svdStuff!E21*0.001</f>
         <v>0.115</v>
       </c>
-      <c r="O21" s="13">
+      <c r="P21" s="13">
         <v>0.115</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <f>LOG10(26276)</f>
         <v>4.4195592531957208</v>
       </c>
-      <c r="Q21" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R21" s="1" t="s">
         <v>26</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T21" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V21" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="W21" s="1"/>
-      <c r="Z21">
+      <c r="X21" s="1"/>
+      <c r="AA21">
         <f t="shared" si="1"/>
         <v>3.9414000000000047</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>35</v>
       </c>
@@ -3190,40 +3254,43 @@
       <c r="L22">
         <v>0</v>
       </c>
-      <c r="N22" s="13">
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="O22" s="13">
         <f>svdStuff!E22*0.001</f>
         <v>0.186</v>
       </c>
-      <c r="O22" s="13">
+      <c r="P22" s="13">
         <v>0.186</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <f>LOG10(20720)</f>
         <v>4.3163897510731957</v>
       </c>
-      <c r="Q22" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V22" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="W22" s="1"/>
-      <c r="Z22">
+      <c r="X22" s="1"/>
+      <c r="AA22">
         <f t="shared" si="1"/>
         <v>3.1080000000000032</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <v>193</v>
       </c>
@@ -3258,40 +3325,43 @@
       <c r="L23">
         <v>0</v>
       </c>
-      <c r="N23" s="13">
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="O23" s="13">
         <f>svdStuff!E23*0.001</f>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="O23" s="13">
+      <c r="P23" s="13">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="P23">
+      <c r="Q23">
         <f>LOG10(16241)</f>
         <v>4.2106127663528978</v>
       </c>
-      <c r="Q23" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V23" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="W23" s="1"/>
-      <c r="Z23">
+      <c r="X23" s="1"/>
+      <c r="AA23">
         <f t="shared" si="1"/>
         <v>2.4361500000000018</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>162</v>
       </c>
@@ -3326,40 +3396,43 @@
       <c r="L24">
         <v>0</v>
       </c>
-      <c r="N24" s="13">
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="O24" s="13">
         <f>svdStuff!E24*0.001</f>
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="O24" s="13">
+      <c r="P24" s="13">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="P24">
+      <c r="Q24">
         <f>LOG10(10072)</f>
         <v>4.0031157170998064</v>
       </c>
-      <c r="Q24" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R24" s="1" t="s">
         <v>26</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V24" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="W24" s="1"/>
-      <c r="Z24">
+      <c r="X24" s="1"/>
+      <c r="AA24">
         <f t="shared" si="1"/>
         <v>1.5108000000000019</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B25" s="12">
         <v>213</v>
       </c>
@@ -3394,40 +3467,43 @@
       <c r="L25">
         <v>0</v>
       </c>
-      <c r="N25" s="13">
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="O25" s="13">
         <f>svdStuff!E25*0.001</f>
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="O25" s="13">
+      <c r="P25" s="13">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <f>LOG10(7623)</f>
         <v>3.882125919770032</v>
       </c>
-      <c r="Q25" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R25" s="1" t="s">
         <v>26</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V25" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="W25" s="1"/>
-      <c r="Z25">
+      <c r="X25" s="1"/>
+      <c r="AA25">
         <f t="shared" si="1"/>
         <v>1.1434500000000012</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>36</v>
       </c>
@@ -3463,40 +3539,43 @@
       <c r="L26">
         <v>0</v>
       </c>
-      <c r="N26" s="13">
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="O26" s="13">
         <f>svdStuff!E26*0.001</f>
         <v>2.4E-2</v>
       </c>
-      <c r="O26" s="13">
+      <c r="P26" s="13">
         <v>2.4E-2</v>
       </c>
-      <c r="P26">
+      <c r="Q26">
         <f>LOG10(5757)</f>
         <v>3.7601962294551341</v>
       </c>
-      <c r="Q26" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="R26" s="1" t="s">
         <v>26</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V26" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="W26" s="1"/>
-      <c r="Z26">
+      <c r="X26" s="1"/>
+      <c r="AA26">
         <f t="shared" si="1"/>
         <v>0.86355000000000015</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
         <v>200</v>
       </c>
@@ -3535,16 +3614,19 @@
         <v>0</v>
       </c>
       <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
         <v>0.7</v>
-      </c>
-      <c r="N27" s="13">
-        <v>0.2</v>
       </c>
       <c r="O27" s="13">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="P27" s="13">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B28" s="12" t="s">
         <v>198</v>
       </c>
@@ -3580,16 +3662,19 @@
         <v>0</v>
       </c>
       <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
         <v>0.45</v>
-      </c>
-      <c r="N28" s="13">
-        <v>0.186</v>
       </c>
       <c r="O28" s="13">
         <v>0.186</v>
       </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="P28" s="13">
+        <v>0.186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B29" s="12" t="s">
         <v>199</v>
       </c>
@@ -3625,72 +3710,75 @@
         <v>0</v>
       </c>
       <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
         <v>0.4</v>
-      </c>
-      <c r="N29" s="13">
-        <v>6.4000000000000001E-2</v>
       </c>
       <c r="O29" s="13">
         <v>6.4000000000000001E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="P29" s="13">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B32" s="12"/>
       <c r="C32" s="20"/>
       <c r="H32" s="13"/>
       <c r="J32" s="2"/>
-      <c r="N32" s="13"/>
       <c r="O32" s="13"/>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P32" s="13"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="12"/>
       <c r="C33" s="20"/>
       <c r="H33" s="13"/>
       <c r="J33" s="2"/>
-      <c r="N33" s="13"/>
       <c r="O33" s="13"/>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P33" s="13"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="12"/>
       <c r="C34" s="20"/>
       <c r="H34" s="13"/>
       <c r="J34" s="2"/>
-      <c r="N34" s="13"/>
       <c r="O34" s="13"/>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P34" s="13"/>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="12"/>
       <c r="C35" s="20"/>
       <c r="H35" s="13"/>
       <c r="J35" s="2"/>
-      <c r="N35" s="13"/>
       <c r="O35" s="13"/>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P35" s="13"/>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="12"/>
       <c r="C36" s="20"/>
       <c r="H36" s="13"/>
       <c r="J36" s="2"/>
-      <c r="N36" s="13"/>
       <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="R1:V1"/>
   </mergeCells>
-  <conditionalFormatting sqref="Q3:Q16 T3:T16">
-    <cfRule type="cellIs" dxfId="39" priority="92" operator="equal">
+  <conditionalFormatting sqref="R3:R16 U3:U16">
+    <cfRule type="cellIs" dxfId="39" priority="99" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="100" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="101" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F16">
-    <cfRule type="colorScale" priority="91">
+    <cfRule type="colorScale" priority="98">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3702,7 +3790,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27:H29 H3:I26">
-    <cfRule type="colorScale" priority="90">
+    <cfRule type="colorScale" priority="97">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3714,7 +3802,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:L16 K18:L26">
-    <cfRule type="colorScale" priority="89">
+    <cfRule type="colorScale" priority="96">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3726,7 +3814,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K16 K18:K26">
-    <cfRule type="colorScale" priority="88">
+    <cfRule type="colorScale" priority="95">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3736,7 +3824,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L16 L18:L26">
-    <cfRule type="colorScale" priority="87">
+    <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3745,8 +3833,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N16 P3:P26">
-    <cfRule type="colorScale" priority="86">
+  <conditionalFormatting sqref="O3:O16 Q3:Q26">
+    <cfRule type="colorScale" priority="93">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3756,34 +3844,34 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32:I36 I3:I29">
-    <cfRule type="cellIs" dxfId="36" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="92" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T17:T26">
-    <cfRule type="cellIs" dxfId="35" priority="82" operator="equal">
+  <conditionalFormatting sqref="U17:U26">
+    <cfRule type="cellIs" dxfId="35" priority="89" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="90" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="91" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q17:Q26">
-    <cfRule type="cellIs" dxfId="32" priority="79" operator="equal">
+  <conditionalFormatting sqref="R17:R26">
+    <cfRule type="cellIs" dxfId="32" priority="86" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="87" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="88" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:L26">
-    <cfRule type="colorScale" priority="78">
+    <cfRule type="colorScale" priority="85">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3793,7 +3881,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F26 H3:H29">
-    <cfRule type="colorScale" priority="77">
+    <cfRule type="colorScale" priority="84">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3804,8 +3892,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N26 P3:P26">
-    <cfRule type="colorScale" priority="76">
+  <conditionalFormatting sqref="O3:O26 Q3:Q26">
+    <cfRule type="colorScale" priority="83">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3815,7 +3903,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H29">
-    <cfRule type="colorScale" priority="75">
+    <cfRule type="colorScale" priority="82">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3826,51 +3914,83 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U3:U16">
-    <cfRule type="cellIs" dxfId="29" priority="72" operator="equal">
+  <conditionalFormatting sqref="V3:V16">
+    <cfRule type="cellIs" dxfId="29" priority="79" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="80" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="81" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U17:U26">
-    <cfRule type="cellIs" dxfId="26" priority="69" operator="equal">
+  <conditionalFormatting sqref="V17:V26">
+    <cfRule type="cellIs" dxfId="26" priority="76" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="77" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="78" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S16">
-    <cfRule type="cellIs" dxfId="23" priority="66" operator="equal">
+  <conditionalFormatting sqref="T3:T16">
+    <cfRule type="cellIs" dxfId="23" priority="73" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="74" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="75" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T17:T26">
+    <cfRule type="cellIs" dxfId="20" priority="70" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="71" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="72" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3:Q26">
+    <cfRule type="colorScale" priority="69">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S16">
+    <cfRule type="cellIs" dxfId="17" priority="66" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="67" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="68" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S17:S26">
-    <cfRule type="cellIs" dxfId="20" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="63" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="64" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="65" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P26">
+  <conditionalFormatting sqref="P3:P16">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
@@ -3880,30 +4000,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3:R16">
-    <cfRule type="cellIs" dxfId="17" priority="59" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="60" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="61" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R17:R26">
-    <cfRule type="cellIs" dxfId="14" priority="56" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="57" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="58" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O16">
-    <cfRule type="colorScale" priority="55">
+  <conditionalFormatting sqref="P3:P26">
+    <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3912,62 +4010,52 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O26">
-    <cfRule type="colorScale" priority="54">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V16">
-    <cfRule type="cellIs" dxfId="11" priority="51" operator="equal">
+  <conditionalFormatting sqref="W3:W16">
+    <cfRule type="cellIs" dxfId="11" priority="58" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="59" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="53" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V17:V26">
-    <cfRule type="cellIs" dxfId="8" priority="48" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="49" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="50" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W3:W16">
-    <cfRule type="cellIs" dxfId="5" priority="45" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="46" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="60" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W17:W26">
-    <cfRule type="cellIs" dxfId="2" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="55" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="56" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="57" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X3:X16">
+    <cfRule type="cellIs" dxfId="5" priority="52" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="53" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="54" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X17:X26">
+    <cfRule type="cellIs" dxfId="2" priority="49" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="50" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="51" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E16">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3979,7 +4067,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E26">
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3991,7 +4079,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G16">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4003,7 +4091,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G26">
-    <cfRule type="colorScale" priority="37">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4015,7 +4103,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27:I29 H32:I36">
-    <cfRule type="colorScale" priority="36">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4026,8 +4114,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N32:N36">
-    <cfRule type="colorScale" priority="22">
+  <conditionalFormatting sqref="O32:O36">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4037,7 +4125,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32:H36">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4048,8 +4136,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N27:N29">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="O27:O29">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4059,7 +4147,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:L36 K27:L29">
-    <cfRule type="colorScale" priority="105">
+    <cfRule type="colorScale" priority="112">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4071,7 +4159,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:K36 K27:K29">
-    <cfRule type="colorScale" priority="108">
+    <cfRule type="colorScale" priority="115">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4081,7 +4169,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L32:L36 L27:L29">
-    <cfRule type="colorScale" priority="111">
+    <cfRule type="colorScale" priority="118">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4091,7 +4179,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:L36 K27:L29">
-    <cfRule type="colorScale" priority="117">
+    <cfRule type="colorScale" priority="124">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4101,7 +4189,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32:F36 F27:F29 H32:H36">
-    <cfRule type="colorScale" priority="120">
+    <cfRule type="colorScale" priority="127">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4112,8 +4200,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O32:O36 O27:O29">
-    <cfRule type="colorScale" priority="126">
+  <conditionalFormatting sqref="P32:P36 P27:P29">
+    <cfRule type="colorScale" priority="133">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4123,7 +4211,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:E36 D27:E29">
-    <cfRule type="colorScale" priority="129">
+    <cfRule type="colorScale" priority="136">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4135,7 +4223,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:G36 G27:G29">
-    <cfRule type="colorScale" priority="132">
+    <cfRule type="colorScale" priority="139">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4147,7 +4235,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:L29">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4157,6 +4245,96 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D29">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G29">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F29">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E29">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:P29">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M16 M18:M26">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M16 M18:M26">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M26">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M32:M36 M27:M29">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -4168,49 +4346,33 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G29">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="M32:M36 M27:M29">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F29">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="M32:M36 M27:M29">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E29">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N3:O29">
+  <conditionalFormatting sqref="M3:M29">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
+        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>